<commit_message>
Start $MDB data entry
</commit_message>
<xml_diff>
--- a/$MDB.xlsx
+++ b/$MDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16C46B3-1226-472A-9563-31D514EAD070}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F969DA5-C97C-46C5-A5CE-4D5871A35C11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27435" windowHeight="11100" xr2:uid="{A0DE9234-8F94-41AD-8663-2284C148F328}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27435" windowHeight="11100" activeTab="1" xr2:uid="{A0DE9234-8F94-41AD-8663-2284C148F328}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="131">
   <si>
     <t>$MDB</t>
   </si>
@@ -134,6 +134,291 @@
   </si>
   <si>
     <t>AWS Collaboration</t>
+  </si>
+  <si>
+    <t>FQ118</t>
+  </si>
+  <si>
+    <t>FQ218</t>
+  </si>
+  <si>
+    <t>FQ318</t>
+  </si>
+  <si>
+    <t>FQ418</t>
+  </si>
+  <si>
+    <t>FQ119</t>
+  </si>
+  <si>
+    <t>FQ219</t>
+  </si>
+  <si>
+    <t>FQ319</t>
+  </si>
+  <si>
+    <t>FQ419</t>
+  </si>
+  <si>
+    <t>FQ120</t>
+  </si>
+  <si>
+    <t>FQ220</t>
+  </si>
+  <si>
+    <t>FQ320</t>
+  </si>
+  <si>
+    <t>FQ420</t>
+  </si>
+  <si>
+    <t>FQ121</t>
+  </si>
+  <si>
+    <t>FQ221</t>
+  </si>
+  <si>
+    <t>FQ321</t>
+  </si>
+  <si>
+    <t>FQ421</t>
+  </si>
+  <si>
+    <t>FQ122</t>
+  </si>
+  <si>
+    <t>FQ222</t>
+  </si>
+  <si>
+    <t>FQ322</t>
+  </si>
+  <si>
+    <t>FQ422</t>
+  </si>
+  <si>
+    <t>FY18</t>
+  </si>
+  <si>
+    <t>FY19</t>
+  </si>
+  <si>
+    <t>FY20</t>
+  </si>
+  <si>
+    <t>FY21</t>
+  </si>
+  <si>
+    <t>FY22</t>
+  </si>
+  <si>
+    <t>FY23</t>
+  </si>
+  <si>
+    <t>FY24</t>
+  </si>
+  <si>
+    <t>FY25</t>
+  </si>
+  <si>
+    <t>FY26</t>
+  </si>
+  <si>
+    <t>FY27</t>
+  </si>
+  <si>
+    <t>FY28</t>
+  </si>
+  <si>
+    <t>FY29</t>
+  </si>
+  <si>
+    <t>FY30</t>
+  </si>
+  <si>
+    <t>FY31</t>
+  </si>
+  <si>
+    <t>FY32</t>
+  </si>
+  <si>
+    <t>FQ323</t>
+  </si>
+  <si>
+    <t>New York City, US</t>
+  </si>
+  <si>
+    <t>IPO</t>
+  </si>
+  <si>
+    <t>In 2013 MongoDB, Inc. was revealed to have received funding through CIA-sponsered In-Q-Tel which has been</t>
+  </si>
+  <si>
+    <t>a concern for foreign nations, such as India</t>
+  </si>
+  <si>
+    <t>FQ123</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>COGS</t>
+  </si>
+  <si>
+    <t>Subscription COGS</t>
+  </si>
+  <si>
+    <t>Services COGS</t>
+  </si>
+  <si>
+    <t>Subscription Revenue</t>
+  </si>
+  <si>
+    <t>Services Revenue</t>
+  </si>
+  <si>
+    <t>Gross Profit</t>
+  </si>
+  <si>
+    <t>Revenue Y/Y</t>
+  </si>
+  <si>
+    <t>Revenue Q/Q</t>
+  </si>
+  <si>
+    <t>Gross Margin</t>
+  </si>
+  <si>
+    <t>Operating Margin</t>
+  </si>
+  <si>
+    <t>Net Margin</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>FQ223</t>
+  </si>
+  <si>
+    <t>FQ423</t>
+  </si>
+  <si>
+    <t>Sales &amp; Marketing</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>G&amp;A</t>
+  </si>
+  <si>
+    <t>Total Operating Expenses</t>
+  </si>
+  <si>
+    <t>Operating Income</t>
+  </si>
+  <si>
+    <t>Interest Income</t>
+  </si>
+  <si>
+    <t>Interest Expense</t>
+  </si>
+  <si>
+    <t>Other Income, Net</t>
+  </si>
+  <si>
+    <t>Pretax Income</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>Net Income</t>
+  </si>
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>Balance Sheet</t>
+  </si>
+  <si>
+    <t>Short-Term Investments</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>Deferred Commission</t>
+  </si>
+  <si>
+    <t>Prepaid Expenses &amp; OCA</t>
+  </si>
+  <si>
+    <t>TCA</t>
+  </si>
+  <si>
+    <t>PP&amp;E</t>
+  </si>
+  <si>
+    <t>Operating Lease ROU</t>
+  </si>
+  <si>
+    <t>Goodwill+Intangibles</t>
+  </si>
+  <si>
+    <t>Deferred Taxes</t>
+  </si>
+  <si>
+    <t>Other Assets</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>Accrued Compensation &amp; Benefits</t>
+  </si>
+  <si>
+    <t>Operating Lease Liabiltiies</t>
+  </si>
+  <si>
+    <t>Other Accrued Liabilities</t>
+  </si>
+  <si>
+    <t>Deferred Revenue</t>
+  </si>
+  <si>
+    <t>TCL</t>
+  </si>
+  <si>
+    <t>Convertible Senior Notes</t>
+  </si>
+  <si>
+    <t>Other Liabilities</t>
+  </si>
+  <si>
+    <t>Liabilities</t>
+  </si>
+  <si>
+    <t>S/E</t>
+  </si>
+  <si>
+    <t>S/E+L</t>
+  </si>
+  <si>
+    <t>Book Value</t>
+  </si>
+  <si>
+    <t>Book Value per Share</t>
+  </si>
+  <si>
+    <t>Share Price</t>
+  </si>
+  <si>
+    <t>ROCE</t>
   </si>
 </sst>
 </file>
@@ -143,7 +428,7 @@
   <numFmts count="1">
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +444,50 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -286,10 +615,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -318,6 +648,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -341,8 +674,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -352,8 +683,41 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -430,6 +794,111 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB38A8F7-E425-4B32-9431-AC4CC1F21B15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16383000" y="0"/>
+          <a:ext cx="0" cy="13916025"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78E59225-2260-40BB-8240-59ADFAA9D236}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21869400" y="0"/>
+          <a:ext cx="0" cy="13916025"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -734,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A27B16A-4CA6-4CC0-B1CB-A0561C46DE09}">
   <dimension ref="A2:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6:W17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -747,12 +1216,12 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -793,18 +1262,18 @@
       <c r="C6" s="8">
         <v>178.79</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="26"/>
+      <c r="D6" s="16"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="25"/>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
@@ -814,21 +1283,21 @@
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="18">
         <v>68.709999999999994</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="26"/>
+      <c r="D7" s="16"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="25"/>
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
@@ -838,23 +1307,23 @@
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="18">
         <f>C6*C7</f>
         <v>12284.660899999999</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="26"/>
-      <c r="T8" s="31" t="s">
+      <c r="D8" s="16"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="25"/>
+      <c r="T8" s="30" t="s">
         <v>35</v>
       </c>
       <c r="U8" s="10"/>
@@ -865,19 +1334,19 @@
       <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="15"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="26"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="16"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="25"/>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
@@ -887,19 +1356,19 @@
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="15"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="26"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="16"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="25"/>
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
@@ -909,22 +1378,22 @@
       <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="18">
         <f>C9-C10</f>
         <v>0</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="26"/>
+      <c r="D11" s="16"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="25"/>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -934,56 +1403,56 @@
       <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="19">
         <f>C8-C11</f>
         <v>12284.660899999999</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="26"/>
+      <c r="D12" s="17"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="25"/>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G13" s="23"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="25"/>
       <c r="T13" s="10"/>
       <c r="U13" s="10"/>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G14" s="23"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="26"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="25"/>
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
@@ -995,24 +1464,24 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="26"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="25"/>
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="30"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="11" t="s">
         <v>10</v>
       </c>
@@ -1020,24 +1489,24 @@
         <v>27</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="26"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="25"/>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="29" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="11" t="s">
@@ -1047,24 +1516,24 @@
         <v>31</v>
       </c>
       <c r="D17" s="13"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="26"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="25"/>
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="11" t="s">
         <v>32</v>
       </c>
@@ -1072,66 +1541,66 @@
         <v>33</v>
       </c>
       <c r="D18" s="13"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="26"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="25"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="25"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="26"/>
+      <c r="D19" s="23"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="25"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G20" s="23"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="26"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="25"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G21" s="23"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="26"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="25"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
@@ -1139,163 +1608,175 @@
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="26"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="25"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="D23" s="13"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="26"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="25"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="12">
+        <v>2007</v>
+      </c>
       <c r="D24" s="13"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="26"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="25"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B25" s="19"/>
-      <c r="C25" s="12"/>
+      <c r="B25" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="12">
+        <v>2017</v>
+      </c>
       <c r="D25" s="13"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="26"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="25"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B26" s="19"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="25"/>
-      <c r="Q26" s="26"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="25"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B27" s="19"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="12"/>
       <c r="D27" s="13"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="26"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="25"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="26"/>
+      <c r="C28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="34">
+        <v>44901</v>
+      </c>
+      <c r="G28" s="20"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="25"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="26"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="23"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="25"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G30" s="23"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="25"/>
-      <c r="Q30" s="26"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="25"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G31" s="23"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25"/>
-      <c r="Q31" s="26"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="25"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
@@ -1303,126 +1784,132 @@
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="25"/>
-      <c r="P32" s="25"/>
-      <c r="Q32" s="26"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="25"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="20" t="s">
         <v>21</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="13"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="25"/>
-      <c r="P33" s="25"/>
-      <c r="Q33" s="26"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="25"/>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="20" t="s">
         <v>22</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="13"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="25"/>
-      <c r="Q34" s="26"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="25"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="13"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="26"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="25"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="13"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="26"/>
+      <c r="G36" s="20">
+        <v>2013</v>
+      </c>
+      <c r="H36" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="25"/>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="13"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="25"/>
-      <c r="P37" s="25"/>
-      <c r="Q37" s="26"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="25"/>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B38" s="19"/>
+      <c r="B38" s="20"/>
       <c r="C38" s="12"/>
       <c r="D38" s="13"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="27"/>
-      <c r="Q38" s="28"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="22">
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
@@ -1430,7 +1917,6 @@
     <mergeCell ref="G5:Q5"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="C33:D33"/>
@@ -1455,17 +1941,776 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509F8013-A317-41E1-99F6-617E09116884}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:AR82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:44" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y1" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z1" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD1" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE1" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG1" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH1" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI1" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL1" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM1" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN1" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO1" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP1" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ1" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR1" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="2:44" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="33"/>
+      <c r="S2" s="36">
+        <v>44316</v>
+      </c>
+      <c r="V2" s="36">
+        <v>44592</v>
+      </c>
+      <c r="W2" s="36">
+        <v>44681</v>
+      </c>
+    </row>
+    <row r="3" spans="2:44" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="33"/>
+    </row>
+    <row r="4" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B4" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="S4" s="38">
+        <v>174.57</v>
+      </c>
+      <c r="W4" s="38">
+        <v>274.58100000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B5" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="S5" s="38">
+        <v>7.0780000000000003</v>
+      </c>
+      <c r="W5" s="38">
+        <v>10.866</v>
+      </c>
+    </row>
+    <row r="6" spans="2:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="S6" s="39">
+        <f>S4+S5</f>
+        <v>181.648</v>
+      </c>
+      <c r="W6" s="39">
+        <f>W4+W5</f>
+        <v>285.447</v>
+      </c>
+    </row>
+    <row r="7" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B7" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="S7" s="1">
+        <v>45.402000000000001</v>
+      </c>
+      <c r="W7" s="1">
+        <v>64.569000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B8" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="S8" s="1">
+        <v>9.1259999999999994</v>
+      </c>
+      <c r="W8" s="1">
+        <v>13.646000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S9" s="1">
+        <f>S7+S8</f>
+        <v>54.527999999999999</v>
+      </c>
+      <c r="W9" s="1">
+        <f>W7+W8</f>
+        <v>78.215000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="2:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S10" s="39">
+        <f>S6-S9</f>
+        <v>127.12</v>
+      </c>
+      <c r="W10" s="39">
+        <f>W6-W9</f>
+        <v>207.232</v>
+      </c>
+    </row>
+    <row r="11" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="S11" s="38">
+        <v>97.89</v>
+      </c>
+      <c r="W11" s="38">
+        <v>150.268</v>
+      </c>
+    </row>
+    <row r="12" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="S12" s="38">
+        <v>64.751000000000005</v>
+      </c>
+      <c r="W12" s="38">
+        <v>96.372</v>
+      </c>
+    </row>
+    <row r="13" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="S13" s="38">
+        <v>25.925000000000001</v>
+      </c>
+      <c r="W13" s="38">
+        <v>36.531999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="S14" s="38">
+        <f>S11+S12+S13</f>
+        <v>188.56600000000003</v>
+      </c>
+      <c r="W14" s="38">
+        <f>W11+W12+W13</f>
+        <v>283.17199999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="2:44" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="S15" s="39">
+        <f>S10-S14</f>
+        <v>-61.446000000000026</v>
+      </c>
+      <c r="W15" s="39">
+        <f>W10-W14</f>
+        <v>-75.939999999999969</v>
+      </c>
+    </row>
+    <row r="16" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="S16" s="38">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="W16" s="38">
+        <v>0.624</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="S17" s="38">
+        <v>3.6579999999999999</v>
+      </c>
+      <c r="W17" s="38">
+        <v>2.4529999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="S18" s="38">
+        <v>-0.437</v>
+      </c>
+      <c r="W18" s="38">
+        <v>1.621</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="S19" s="38">
+        <f>S15+S16-S17+S18</f>
+        <v>-65.368000000000023</v>
+      </c>
+      <c r="W19" s="38">
+        <f>W15+W16-W17+W18</f>
+        <v>-76.147999999999982</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="S20" s="38">
+        <v>-1.3759999999999999</v>
+      </c>
+      <c r="W20" s="38">
+        <v>1.1459999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="S21" s="39">
+        <f>S19-S20</f>
+        <v>-63.992000000000026</v>
+      </c>
+      <c r="W21" s="39">
+        <f>W19-W20</f>
+        <v>-77.293999999999983</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="S22" s="44">
+        <f>S21/S23</f>
+        <v>-1.0428660106545344</v>
+      </c>
+      <c r="W22" s="44">
+        <f>W21/W23</f>
+        <v>-1.1416038004739926</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="S23" s="38">
+        <v>61.361669999999997</v>
+      </c>
+      <c r="W23" s="38">
+        <v>67.706502</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" s="38" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="W26" s="40">
+        <f>W6/S6-1</f>
+        <v>0.57142935787897486</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="S29" s="41">
+        <f>S10/S6</f>
+        <v>0.69981502686514585</v>
+      </c>
+      <c r="W29" s="41">
+        <f>W10/W6</f>
+        <v>0.72599116473460923</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="S30" s="41">
+        <f>S15/S6</f>
+        <v>-0.33826962036466146</v>
+      </c>
+      <c r="W30" s="41">
+        <f>W15/W6</f>
+        <v>-0.26603887937165205</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="S31" s="41">
+        <f>S21/S6</f>
+        <v>-0.35228573945212732</v>
+      </c>
+      <c r="W31" s="41">
+        <f>W21/W6</f>
+        <v>-0.27078231685742005</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="S32" s="41">
+        <f>S20/S19</f>
+        <v>2.1050055072818496E-2</v>
+      </c>
+      <c r="W32" s="41">
+        <f>W20/W19</f>
+        <v>-1.5049640174397229E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B36" s="45" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="V37" s="2">
+        <v>473.904</v>
+      </c>
+      <c r="W37" s="39">
+        <v>456.27499999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W38" s="39">
+        <v>1372.42</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="W39" s="38">
+        <v>164.88499999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="W40" s="38">
+        <v>66.754000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W41" s="38">
+        <v>35.972999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="W42" s="38">
+        <f>SUM(W37:W41)</f>
+        <v>2096.3070000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="W43" s="38">
+        <v>62.761000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="W44" s="38">
+        <v>45.247999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W45" s="38">
+        <f>57.775+18.313</f>
+        <v>76.087999999999994</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="W46" s="38">
+        <v>1.9630000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="W47" s="38">
+        <v>152.17400000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="W48" s="38">
+        <f>W42+SUM(W43:W47)</f>
+        <v>2434.5410000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="W50" s="38">
+        <v>6.2039999999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W51" s="38">
+        <v>87.716999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="W52" s="38">
+        <v>8.6709999999999994</v>
+      </c>
+    </row>
+    <row r="53" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="W53" s="38">
+        <v>49.216000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W54" s="38">
+        <v>351.91399999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="W55" s="38">
+        <f>SUM(W50:W54)</f>
+        <v>503.72199999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="W56" s="38">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="W57" s="38">
+        <v>40.279000000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W58" s="38">
+        <v>23.555</v>
+      </c>
+    </row>
+    <row r="59" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="W59" s="39">
+        <v>1137.3610000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="W60" s="39">
+        <v>56.652000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B61" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="W61" s="38">
+        <f>W55+SUM(W56:W60)</f>
+        <v>1761.662</v>
+      </c>
+    </row>
+    <row r="63" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B63" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="W63" s="38">
+        <v>672.87900000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B64" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W64" s="38">
+        <f>W63+W61</f>
+        <v>2434.5410000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B66" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="W66" s="38">
+        <f>W48-W61</f>
+        <v>672.87900000000013</v>
+      </c>
+    </row>
+    <row r="67" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B67" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="W67" s="1">
+        <f>W66/W23</f>
+        <v>9.9381740323846604</v>
+      </c>
+    </row>
+    <row r="69" spans="2:23" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="W69" s="42">
+        <f>W37+W38</f>
+        <v>1828.6950000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="2:23" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="W70" s="42">
+        <f>W59</f>
+        <v>1137.3610000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W71" s="38">
+        <f>W69-W70</f>
+        <v>691.33400000000006</v>
+      </c>
+    </row>
+    <row r="73" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B73" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B74" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B75" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B77" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B78" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B79" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B80" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="W1" r:id="rId1" location="i38c3139dc7914f5e8533d7dcbc3a2a96_13" xr:uid="{E49C4A64-2AFD-4765-8FED-15375274F6C1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2021 & 2022 Annual reports, first projections
</commit_message>
<xml_diff>
--- a/$MDB.xlsx
+++ b/$MDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EA241D-AAB9-4349-B415-D852E4A18DFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A3FB38-9D4C-4033-AA4D-629AD6D4E025}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27435" windowHeight="11100" xr2:uid="{A0DE9234-8F94-41AD-8663-2284C148F328}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="144">
   <si>
     <t>$MDB</t>
   </si>
@@ -452,18 +452,25 @@
   </si>
   <si>
     <t>New York City, NY</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>(Projected)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0\x"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,8 +535,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,6 +580,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -654,7 +683,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -726,36 +755,6 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -768,6 +767,69 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -857,14 +919,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -881,7 +943,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15782925" y="0"/>
+          <a:off x="16373475" y="0"/>
           <a:ext cx="0" cy="13916025"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1258,7 +1320,7 @@
   <dimension ref="A2:AB38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:D24"/>
+      <selection activeCell="C34" sqref="C34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1284,42 +1346,42 @@
       <c r="G3"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="43"/>
-      <c r="G5" s="41" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="G5" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="43"/>
-      <c r="T5" s="44" t="s">
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
+      <c r="T5" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="44"/>
-      <c r="V5" s="44"/>
-      <c r="W5" s="44"/>
-      <c r="Z5" s="44" t="s">
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="Z5" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="AA5" s="44"/>
-      <c r="AB5" s="44"/>
+      <c r="AA5" s="46"/>
+      <c r="AB5" s="46"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="4">
-        <v>178.79</v>
+        <v>191.75</v>
       </c>
       <c r="D6" s="10"/>
       <c r="G6" s="14"/>
@@ -1348,9 +1410,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="12">
-        <v>68.709999999999994</v>
-      </c>
-      <c r="D7" s="10"/>
+        <f>'Financial Model'!Y23</f>
+        <v>68.916813000000005</v>
+      </c>
+      <c r="D7" s="10" t="str">
+        <f>$C$28</f>
+        <v>FQ323</v>
+      </c>
       <c r="G7" s="14"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
@@ -1366,10 +1432,10 @@
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
-      <c r="Z7" s="53" t="s">
+      <c r="Z7" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="AA7" s="53"/>
+      <c r="AA7" s="43"/>
       <c r="AB7" s="6"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
@@ -1378,7 +1444,7 @@
       </c>
       <c r="C8" s="12">
         <f>C6*C7</f>
-        <v>12284.660899999999</v>
+        <v>13214.798892750001</v>
       </c>
       <c r="D8" s="10"/>
       <c r="G8" s="14"/>
@@ -1398,10 +1464,10 @@
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
-      <c r="Z8" s="53" t="s">
+      <c r="Z8" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="AA8" s="54" t="s">
+      <c r="AA8" s="44" t="s">
         <v>137</v>
       </c>
       <c r="AB8" s="6"/>
@@ -1410,8 +1476,14 @@
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="10"/>
+      <c r="C9" s="12">
+        <f>'Financial Model'!Y69</f>
+        <v>1787.5319999999999</v>
+      </c>
+      <c r="D9" s="10" t="str">
+        <f t="shared" ref="D9:D11" si="0">$C$28</f>
+        <v>FQ323</v>
+      </c>
       <c r="G9" s="14"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
@@ -1427,10 +1499,10 @@
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
-      <c r="Z9" s="54" t="s">
+      <c r="Z9" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="AA9" s="55" t="s">
+      <c r="AA9" s="45" t="s">
         <v>139</v>
       </c>
       <c r="AB9" s="6"/>
@@ -1439,8 +1511,14 @@
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="10"/>
+      <c r="C10" s="12">
+        <f>'Financial Model'!Y70</f>
+        <v>1139.0419999999999</v>
+      </c>
+      <c r="D10" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>FQ323</v>
+      </c>
       <c r="G10" s="14"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
@@ -1456,10 +1534,10 @@
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
-      <c r="Z10" s="53" t="s">
+      <c r="Z10" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="AA10" s="54" t="s">
+      <c r="AA10" s="44" t="s">
         <v>136</v>
       </c>
       <c r="AB10" s="6"/>
@@ -1470,9 +1548,12 @@
       </c>
       <c r="C11" s="12">
         <f>C9-C10</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="10"/>
+        <v>648.49</v>
+      </c>
+      <c r="D11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>FQ323</v>
+      </c>
       <c r="G11" s="14"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
@@ -1488,10 +1569,10 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
-      <c r="Z11" s="53" t="s">
+      <c r="Z11" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="AA11" s="53"/>
+      <c r="AA11" s="43"/>
       <c r="AB11" s="6"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
@@ -1500,7 +1581,7 @@
       </c>
       <c r="C12" s="13">
         <f>C8-C11</f>
-        <v>12284.660899999999</v>
+        <v>12566.308892750001</v>
       </c>
       <c r="D12" s="11"/>
       <c r="G12" s="14"/>
@@ -1563,11 +1644,11 @@
       <c r="AB14" s="6"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="53"/>
       <c r="G15" s="14"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
@@ -1592,10 +1673,10 @@
       <c r="B16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="40"/>
+      <c r="D16" s="48"/>
       <c r="G16" s="14"/>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
@@ -1622,10 +1703,10 @@
       <c r="B17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="40"/>
+      <c r="D17" s="48"/>
       <c r="G17" s="14"/>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
@@ -1650,10 +1731,10 @@
       <c r="B18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="40"/>
+      <c r="D18" s="48"/>
       <c r="G18" s="14"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
@@ -1673,10 +1754,10 @@
       <c r="B19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="46"/>
+      <c r="D19" s="55"/>
       <c r="G19" s="14"/>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
@@ -1716,11 +1797,11 @@
       <c r="Q21" s="17"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="43"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="53"/>
       <c r="G22" s="14"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
@@ -1737,10 +1818,10 @@
       <c r="B23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="D23" s="40"/>
+      <c r="D23" s="48"/>
       <c r="G23" s="14"/>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
@@ -1757,10 +1838,10 @@
       <c r="B24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="39">
+      <c r="C24" s="47">
         <v>2007</v>
       </c>
-      <c r="D24" s="40"/>
+      <c r="D24" s="48"/>
       <c r="G24" s="14"/>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
@@ -1777,10 +1858,10 @@
       <c r="B25" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="39">
+      <c r="C25" s="47">
         <v>2017</v>
       </c>
-      <c r="D25" s="40"/>
+      <c r="D25" s="48"/>
       <c r="G25" s="14"/>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
@@ -1795,8 +1876,8 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B26" s="14"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="40"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="48"/>
       <c r="G26" s="14"/>
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
@@ -1811,8 +1892,8 @@
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B27" s="14"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="40"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48"/>
       <c r="G27" s="14"/>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
@@ -1851,10 +1932,10 @@
       <c r="B29" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="D29" s="48"/>
+      <c r="D29" s="50"/>
       <c r="G29" s="14"/>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
@@ -1894,11 +1975,11 @@
       <c r="Q31" s="17"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="42"/>
-      <c r="D32" s="43"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="53"/>
       <c r="G32" s="14"/>
       <c r="H32" s="16"/>
       <c r="I32" s="16"/>
@@ -1915,8 +1996,11 @@
       <c r="B33" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="40"/>
+      <c r="C33" s="71">
+        <f>C6/'Financial Model'!Y67</f>
+        <v>19.311919490429393</v>
+      </c>
+      <c r="D33" s="72"/>
       <c r="G33" s="14"/>
       <c r="H33" s="16"/>
       <c r="I33" s="16"/>
@@ -1933,8 +2017,11 @@
       <c r="B34" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="40"/>
+      <c r="C34" s="71">
+        <f>C8/SUM('Financial Model'!V6:Y6)</f>
+        <v>11.112137929461445</v>
+      </c>
+      <c r="D34" s="72"/>
       <c r="G34" s="14"/>
       <c r="H34" s="16"/>
       <c r="I34" s="16"/>
@@ -1951,8 +2038,8 @@
       <c r="B35" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="40"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="48"/>
       <c r="G35" s="14"/>
       <c r="H35" s="16"/>
       <c r="I35" s="16"/>
@@ -1969,8 +2056,8 @@
       <c r="B36" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="40"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="48"/>
       <c r="G36" s="14">
         <v>2013</v>
       </c>
@@ -1991,8 +2078,8 @@
       <c r="B37" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="40"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="48"/>
       <c r="G37" s="14"/>
       <c r="H37" s="27" t="s">
         <v>74</v>
@@ -2009,8 +2096,8 @@
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B38" s="14"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="40"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="G38" s="15"/>
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
@@ -2025,29 +2112,29 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="Z5:AB5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="G5:Q5"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
+    <mergeCell ref="Z5:AB5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="G5:Q5"/>
-    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" location="views-exposed-form-widget-sec-filings-table" display="Link" xr:uid="{8C8DCE07-3950-4AA9-A781-B1A96427FDBB}"/>
@@ -2063,17 +2150,21 @@
   <dimension ref="B1:AR82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="K4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AB17" sqref="AB17"/>
+      <selection pane="bottomRight" activeCell="AF30" sqref="AF30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="25" width="9.140625" style="1"/>
+    <col min="26" max="26" width="9.140625" style="59"/>
+    <col min="27" max="34" width="9.140625" style="1"/>
+    <col min="35" max="35" width="9.140625" style="64"/>
+    <col min="36" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:44" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -2143,10 +2234,10 @@
       <c r="X1" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="Y1" s="23" t="s">
+      <c r="Y1" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="Z1" s="23" t="s">
+      <c r="Z1" s="61" t="s">
         <v>90</v>
       </c>
       <c r="AD1" s="23" t="s">
@@ -2161,10 +2252,10 @@
       <c r="AG1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="AH1" s="23" t="s">
+      <c r="AH1" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="AI1" s="23" t="s">
+      <c r="AI1" s="68" t="s">
         <v>61</v>
       </c>
       <c r="AJ1" s="23" t="s">
@@ -2197,12 +2288,18 @@
     </row>
     <row r="2" spans="2:44" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="25"/>
+      <c r="R2" s="28">
+        <v>44227</v>
+      </c>
       <c r="S2" s="28">
         <v>44316</v>
       </c>
       <c r="T2" s="28">
         <v>44408</v>
       </c>
+      <c r="U2" s="28">
+        <v>44500</v>
+      </c>
       <c r="V2" s="28">
         <v>44592</v>
       </c>
@@ -2212,72 +2309,124 @@
       <c r="X2" s="28">
         <v>44773</v>
       </c>
+      <c r="Y2" s="28">
+        <v>44865</v>
+      </c>
+      <c r="Z2" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG2" s="28">
+        <v>44227</v>
+      </c>
+      <c r="AH2" s="28">
+        <v>44592</v>
+      </c>
+      <c r="AI2" s="69" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="3" spans="2:44" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="25"/>
+      <c r="Z3" s="60"/>
+      <c r="AH3" s="56">
+        <v>44638</v>
+      </c>
+      <c r="AI3" s="69"/>
     </row>
     <row r="4" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
         <v>80</v>
       </c>
+      <c r="R4" s="34">
+        <f>AG4-SUM(O4:Q4)</f>
+        <v>565.34900000000005</v>
+      </c>
       <c r="S4" s="34">
         <v>174.57</v>
       </c>
       <c r="T4" s="38">
         <v>191.381</v>
       </c>
+      <c r="U4" s="34">
+        <v>217.87100000000001</v>
+      </c>
+      <c r="V4" s="34">
+        <f>AH4-SUM(S4:U4)</f>
+        <v>258.22500000000002</v>
+      </c>
       <c r="W4" s="34">
         <v>274.58100000000002</v>
       </c>
-      <c r="X4" s="52">
+      <c r="X4" s="42">
         <v>291.60700000000003</v>
       </c>
+      <c r="Y4" s="34">
+        <v>320.75599999999997</v>
+      </c>
+      <c r="Z4" s="59"/>
       <c r="AF4" s="38">
         <f>SUM(K4:N4)</f>
         <v>0</v>
       </c>
       <c r="AG4" s="38">
-        <f>SUM(O4:R4)</f>
-        <v>0</v>
+        <v>565.34900000000005</v>
       </c>
       <c r="AH4" s="34">
-        <f>SUM(S4:V4)</f>
-        <v>365.95100000000002</v>
-      </c>
+        <v>842.04700000000003</v>
+      </c>
+      <c r="AI4" s="64"/>
     </row>
     <row r="5" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="29" t="s">
         <v>81</v>
       </c>
+      <c r="R5" s="34">
+        <f>AG5-SUM(O5:Q5)</f>
+        <v>25.030999999999999</v>
+      </c>
       <c r="S5" s="34">
         <v>7.0780000000000003</v>
       </c>
       <c r="T5" s="38">
         <v>7.3659999999999997</v>
       </c>
+      <c r="U5" s="34">
+        <v>9.0220000000000002</v>
+      </c>
+      <c r="V5" s="34">
+        <f>AH5-SUM(S5:U5)</f>
+        <v>8.2689999999999984</v>
+      </c>
       <c r="W5" s="34">
         <v>10.866</v>
       </c>
-      <c r="X5" s="52">
+      <c r="X5" s="42">
         <v>12.053000000000001</v>
       </c>
+      <c r="Y5" s="34">
+        <v>12.865</v>
+      </c>
+      <c r="Z5" s="59"/>
       <c r="AF5" s="38">
         <f>SUM(K5:N5)</f>
         <v>0</v>
       </c>
       <c r="AG5" s="38">
-        <f>SUM(O5:R5)</f>
-        <v>0</v>
+        <v>25.030999999999999</v>
       </c>
       <c r="AH5" s="34">
-        <f>SUM(S5:V5)</f>
-        <v>14.443999999999999</v>
-      </c>
+        <v>31.734999999999999</v>
+      </c>
+      <c r="AI5" s="64"/>
     </row>
     <row r="6" spans="2:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="R6" s="31">
+        <f>R4+R5</f>
+        <v>590.38</v>
+      </c>
       <c r="S6" s="31">
         <f>S4+S5</f>
         <v>181.648</v>
@@ -2286,166 +2435,437 @@
         <f>T4+T5</f>
         <v>198.74700000000001</v>
       </c>
+      <c r="U6" s="31">
+        <f>U4+U5</f>
+        <v>226.893</v>
+      </c>
+      <c r="V6" s="31">
+        <f>V4+V5</f>
+        <v>266.49400000000003</v>
+      </c>
       <c r="W6" s="31">
         <f>W4+W5</f>
         <v>285.447</v>
       </c>
-      <c r="X6" s="51">
+      <c r="X6" s="41">
         <f>X4+X5</f>
         <v>303.66000000000003</v>
       </c>
-      <c r="AF6" s="51">
+      <c r="Y6" s="31">
+        <f>Y4+Y5</f>
+        <v>333.62099999999998</v>
+      </c>
+      <c r="Z6" s="62">
+        <f>Y6*(1+Z27)</f>
+        <v>373.65552000000002</v>
+      </c>
+      <c r="AF6" s="41">
         <f>AF4+AF5</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="51">
+      <c r="AG6" s="41">
         <f>AG4+AG5</f>
-        <v>0</v>
-      </c>
-      <c r="AH6" s="51">
+        <v>590.38</v>
+      </c>
+      <c r="AH6" s="41">
         <f>AH4+AH5</f>
-        <v>380.39500000000004</v>
+        <v>873.78200000000004</v>
+      </c>
+      <c r="AI6" s="62">
+        <f>SUM(W6:Z6)</f>
+        <v>1296.3835199999999</v>
+      </c>
+      <c r="AJ6" s="31">
+        <f>AI6*(1+AJ26)</f>
+        <v>1970.5029503999999</v>
+      </c>
+      <c r="AK6" s="31">
+        <f t="shared" ref="AK6:AR6" si="0">AJ6*(1+AK26)</f>
+        <v>2916.3443665919999</v>
+      </c>
+      <c r="AL6" s="31">
+        <f t="shared" si="0"/>
+        <v>3937.0648948992002</v>
+      </c>
+      <c r="AM6" s="31">
+        <f t="shared" si="0"/>
+        <v>4921.3311186240007</v>
+      </c>
+      <c r="AN6" s="31">
+        <f t="shared" si="0"/>
+        <v>5905.5973423488003</v>
+      </c>
+      <c r="AO6" s="31">
+        <f t="shared" si="0"/>
+        <v>6791.4369437011201</v>
+      </c>
+      <c r="AP6" s="31">
+        <f t="shared" si="0"/>
+        <v>7810.152485256287</v>
+      </c>
+      <c r="AQ6" s="31">
+        <f t="shared" si="0"/>
+        <v>8981.6753580447294</v>
+      </c>
+      <c r="AR6" s="31">
+        <f t="shared" si="0"/>
+        <v>10328.926661751439</v>
       </c>
     </row>
     <row r="7" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="29" t="s">
         <v>78</v>
       </c>
+      <c r="R7" s="34">
+        <f t="shared" ref="R7:R8" si="1">AG7-SUM(O7:Q7)</f>
+        <v>145.28</v>
+      </c>
       <c r="S7" s="38">
         <v>45.402000000000001</v>
       </c>
       <c r="T7" s="38">
         <v>50.954999999999998</v>
       </c>
+      <c r="U7" s="34">
+        <v>57.378</v>
+      </c>
+      <c r="V7" s="34">
+        <f t="shared" ref="V7:V8" si="2">AH7-SUM(S7:U7)</f>
+        <v>64.165999999999997</v>
+      </c>
       <c r="W7" s="38">
         <v>64.569000000000003</v>
       </c>
-      <c r="X7" s="52">
+      <c r="X7" s="42">
         <v>71.435000000000002</v>
       </c>
-      <c r="Z7" s="2"/>
+      <c r="Y7" s="34">
+        <v>77.150000000000006</v>
+      </c>
+      <c r="Z7" s="63"/>
+      <c r="AG7" s="38">
+        <v>145.28</v>
+      </c>
+      <c r="AH7" s="38">
+        <v>217.90100000000001</v>
+      </c>
+      <c r="AI7" s="64"/>
     </row>
     <row r="8" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="29" t="s">
         <v>79</v>
       </c>
+      <c r="R8" s="34">
+        <f t="shared" si="1"/>
+        <v>31.795999999999999</v>
+      </c>
       <c r="S8" s="38">
         <v>9.1259999999999994</v>
       </c>
       <c r="T8" s="38">
         <v>9.7469999999999999</v>
       </c>
+      <c r="U8" s="34">
+        <v>11.086</v>
+      </c>
+      <c r="V8" s="34">
+        <f t="shared" si="2"/>
+        <v>11.632000000000005</v>
+      </c>
       <c r="W8" s="38">
         <v>13.646000000000001</v>
       </c>
-      <c r="X8" s="52">
+      <c r="X8" s="42">
         <v>16.841999999999999</v>
       </c>
+      <c r="Y8" s="34">
+        <v>16.501999999999999</v>
+      </c>
+      <c r="Z8" s="59"/>
+      <c r="AG8" s="38">
+        <v>31.795999999999999</v>
+      </c>
+      <c r="AH8" s="38">
+        <v>41.591000000000001</v>
+      </c>
+      <c r="AI8" s="64"/>
     </row>
     <row r="9" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="R9" s="30">
+        <f t="shared" ref="R9" si="3">R7+R8</f>
+        <v>177.07599999999999</v>
+      </c>
       <c r="S9" s="1">
         <f>S7+S8</f>
         <v>54.527999999999999</v>
       </c>
       <c r="T9" s="1">
-        <f t="shared" ref="T9" si="0">T7+T8</f>
+        <f t="shared" ref="T9:U9" si="4">T7+T8</f>
         <v>60.701999999999998</v>
+      </c>
+      <c r="U9" s="30">
+        <f t="shared" si="4"/>
+        <v>68.463999999999999</v>
+      </c>
+      <c r="V9" s="1">
+        <f>V7+V8</f>
+        <v>75.798000000000002</v>
       </c>
       <c r="W9" s="1">
         <f>W7+W8</f>
         <v>78.215000000000003</v>
       </c>
-      <c r="X9" s="49">
-        <f t="shared" ref="X9" si="1">X7+X8</f>
+      <c r="X9" s="39">
+        <f t="shared" ref="X9:Y9" si="5">X7+X8</f>
         <v>88.277000000000001</v>
+      </c>
+      <c r="Y9" s="30">
+        <f t="shared" si="5"/>
+        <v>93.652000000000001</v>
+      </c>
+      <c r="Z9" s="67">
+        <f>Z6*(1-Z29)</f>
+        <v>104.62354560000001</v>
+      </c>
+      <c r="AG9" s="30">
+        <f t="shared" ref="AG9:AH9" si="6">AG7+AG8</f>
+        <v>177.07599999999999</v>
+      </c>
+      <c r="AH9" s="30">
+        <f t="shared" si="6"/>
+        <v>259.49200000000002</v>
+      </c>
+      <c r="AI9" s="64">
+        <f>SUM(W9:Z9)</f>
+        <v>364.76754560000001</v>
       </c>
     </row>
     <row r="10" spans="2:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="R10" s="31">
+        <f t="shared" ref="R10" si="7">R6-R9</f>
+        <v>413.30399999999997</v>
+      </c>
       <c r="S10" s="31">
         <f>S6-S9</f>
         <v>127.12</v>
       </c>
       <c r="T10" s="31">
-        <f t="shared" ref="T10" si="2">T6-T9</f>
+        <f t="shared" ref="T10:U10" si="8">T6-T9</f>
         <v>138.04500000000002</v>
+      </c>
+      <c r="U10" s="31">
+        <f t="shared" si="8"/>
+        <v>158.429</v>
+      </c>
+      <c r="V10" s="31">
+        <f>V6-V9</f>
+        <v>190.69600000000003</v>
       </c>
       <c r="W10" s="31">
         <f>W6-W9</f>
         <v>207.232</v>
       </c>
-      <c r="X10" s="51">
-        <f t="shared" ref="X10" si="3">X6-X9</f>
+      <c r="X10" s="41">
+        <f t="shared" ref="X10:Y10" si="9">X6-X9</f>
         <v>215.38300000000004</v>
+      </c>
+      <c r="Y10" s="31">
+        <f t="shared" si="9"/>
+        <v>239.96899999999999</v>
+      </c>
+      <c r="Z10" s="62">
+        <f>Z6-Z9</f>
+        <v>269.03197440000002</v>
+      </c>
+      <c r="AG10" s="31">
+        <f t="shared" ref="AG10:AH10" si="10">AG6-AG9</f>
+        <v>413.30399999999997</v>
+      </c>
+      <c r="AH10" s="31">
+        <f t="shared" si="10"/>
+        <v>614.29</v>
+      </c>
+      <c r="AI10" s="62">
+        <f>AI6-AI9</f>
+        <v>931.61597439999991</v>
       </c>
     </row>
     <row r="11" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="30" t="s">
         <v>91</v>
       </c>
+      <c r="R11" s="30">
+        <f t="shared" ref="R11:R13" si="11">AG11-SUM(O11:Q11)</f>
+        <v>325.10000000000002</v>
+      </c>
       <c r="S11" s="30">
         <v>97.89</v>
       </c>
       <c r="T11" s="30">
         <v>109.377</v>
       </c>
+      <c r="U11" s="30">
+        <v>120.36</v>
+      </c>
+      <c r="V11" s="30">
+        <f>AH11-SUM(S11:U11)</f>
+        <v>144.26299999999998</v>
+      </c>
       <c r="W11" s="30">
         <v>150.268</v>
       </c>
       <c r="X11" s="30">
         <v>181.59800000000001</v>
+      </c>
+      <c r="Y11" s="30">
+        <v>177.41900000000001</v>
+      </c>
+      <c r="Z11" s="64">
+        <f>Z6*0.53</f>
+        <v>198.03742560000003</v>
+      </c>
+      <c r="AB11" s="36"/>
+      <c r="AC11" s="36"/>
+      <c r="AD11" s="36"/>
+      <c r="AE11" s="36"/>
+      <c r="AG11" s="30">
+        <v>325.10000000000002</v>
+      </c>
+      <c r="AH11" s="30">
+        <v>471.89</v>
+      </c>
+      <c r="AI11" s="64">
+        <f t="shared" ref="AI11:AI13" si="12">SUM(W11:Z11)</f>
+        <v>707.32242559999997</v>
       </c>
     </row>
     <row r="12" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="30" t="s">
         <v>92</v>
       </c>
+      <c r="R12" s="30">
+        <f t="shared" si="11"/>
+        <v>205.161</v>
+      </c>
       <c r="S12" s="30">
         <v>64.751000000000005</v>
       </c>
       <c r="T12" s="30">
         <v>72.396000000000001</v>
       </c>
+      <c r="U12" s="30">
+        <v>82.256</v>
+      </c>
+      <c r="V12" s="30">
+        <f t="shared" ref="V12:V13" si="13">AH12-SUM(S12:U12)</f>
+        <v>89.417000000000002</v>
+      </c>
       <c r="W12" s="30">
         <v>96.372</v>
       </c>
       <c r="X12" s="30">
         <v>108.03700000000001</v>
+      </c>
+      <c r="Y12" s="30">
+        <v>106.392</v>
+      </c>
+      <c r="Z12" s="64">
+        <f>Z6*0.31</f>
+        <v>115.83321120000001</v>
+      </c>
+      <c r="AB12" s="36"/>
+      <c r="AC12" s="36"/>
+      <c r="AD12" s="36"/>
+      <c r="AE12" s="36"/>
+      <c r="AG12" s="30">
+        <v>205.161</v>
+      </c>
+      <c r="AH12" s="30">
+        <v>308.82</v>
+      </c>
+      <c r="AI12" s="64">
+        <f t="shared" si="12"/>
+        <v>426.63421119999998</v>
       </c>
     </row>
     <row r="13" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="30" t="s">
         <v>93</v>
       </c>
+      <c r="R13" s="30">
+        <f t="shared" si="11"/>
+        <v>92.346999999999994</v>
+      </c>
       <c r="S13" s="30">
         <v>25.925000000000001</v>
       </c>
       <c r="T13" s="30">
         <v>28.803000000000001</v>
       </c>
+      <c r="U13" s="30">
+        <v>32.581000000000003</v>
+      </c>
+      <c r="V13" s="30">
+        <f t="shared" si="13"/>
+        <v>35.635000000000005</v>
+      </c>
       <c r="W13" s="30">
         <v>36.531999999999996</v>
       </c>
       <c r="X13" s="30">
         <v>40.591000000000001</v>
+      </c>
+      <c r="Y13" s="30">
+        <v>39.081000000000003</v>
+      </c>
+      <c r="Z13" s="64">
+        <f>Z6*0.12</f>
+        <v>44.838662400000004</v>
+      </c>
+      <c r="AB13" s="36"/>
+      <c r="AC13" s="36"/>
+      <c r="AD13" s="36"/>
+      <c r="AE13" s="36"/>
+      <c r="AG13" s="30">
+        <v>92.346999999999994</v>
+      </c>
+      <c r="AH13" s="30">
+        <v>122.944</v>
+      </c>
+      <c r="AI13" s="64">
+        <f t="shared" si="12"/>
+        <v>161.04266239999998</v>
       </c>
     </row>
     <row r="14" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="30" t="s">
         <v>94</v>
       </c>
+      <c r="R14" s="30">
+        <f t="shared" ref="R14" si="14">R11+R12+R13</f>
+        <v>622.60799999999995</v>
+      </c>
       <c r="S14" s="30">
         <f>S11+S12+S13</f>
         <v>188.56600000000003</v>
       </c>
       <c r="T14" s="30">
-        <f t="shared" ref="T14" si="4">T11+T12+T13</f>
+        <f t="shared" ref="T14:U14" si="15">T11+T12+T13</f>
         <v>210.57599999999999</v>
+      </c>
+      <c r="U14" s="30">
+        <f t="shared" si="15"/>
+        <v>235.197</v>
+      </c>
+      <c r="V14" s="30">
+        <f t="shared" ref="V14" si="16">V11+V12+V13</f>
+        <v>269.315</v>
       </c>
       <c r="W14" s="30">
         <f>W11+W12+W13</f>
@@ -2455,18 +2875,50 @@
         <f>X11+X12+X13</f>
         <v>330.226</v>
       </c>
+      <c r="Y14" s="30">
+        <f t="shared" ref="Y14:Z14" si="17">Y11+Y12+Y13</f>
+        <v>322.89200000000005</v>
+      </c>
+      <c r="Z14" s="64">
+        <f t="shared" si="17"/>
+        <v>358.70929920000003</v>
+      </c>
+      <c r="AG14" s="30">
+        <f t="shared" ref="AG14" si="18">AG11+AG12+AG13</f>
+        <v>622.60799999999995</v>
+      </c>
+      <c r="AH14" s="30">
+        <f t="shared" ref="AH14:AI14" si="19">AH11+AH12+AH13</f>
+        <v>903.654</v>
+      </c>
+      <c r="AI14" s="64">
+        <f t="shared" si="19"/>
+        <v>1294.9992992</v>
+      </c>
     </row>
     <row r="15" spans="2:44" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="31" t="s">
         <v>95</v>
       </c>
+      <c r="R15" s="31">
+        <f t="shared" ref="R15" si="20">R10-R14</f>
+        <v>-209.30399999999997</v>
+      </c>
       <c r="S15" s="31">
         <f>S10-S14</f>
         <v>-61.446000000000026</v>
       </c>
       <c r="T15" s="31">
-        <f t="shared" ref="T15" si="5">T10-T14</f>
+        <f t="shared" ref="T15:U15" si="21">T10-T14</f>
         <v>-72.530999999999977</v>
+      </c>
+      <c r="U15" s="31">
+        <f t="shared" si="21"/>
+        <v>-76.768000000000001</v>
+      </c>
+      <c r="V15" s="31">
+        <f t="shared" ref="V15" si="22">V10-V14</f>
+        <v>-78.618999999999971</v>
       </c>
       <c r="W15" s="31">
         <f>W10-W14</f>
@@ -2476,61 +2928,170 @@
         <f>X10-X14</f>
         <v>-114.84299999999996</v>
       </c>
+      <c r="Y15" s="31">
+        <f t="shared" ref="Y15:Z15" si="23">Y10-Y14</f>
+        <v>-82.923000000000059</v>
+      </c>
+      <c r="Z15" s="62">
+        <f t="shared" si="23"/>
+        <v>-89.677324800000008</v>
+      </c>
+      <c r="AG15" s="31">
+        <f t="shared" ref="AG15" si="24">AG10-AG14</f>
+        <v>-209.30399999999997</v>
+      </c>
+      <c r="AH15" s="31">
+        <f t="shared" ref="AH15:AI15" si="25">AH10-AH14</f>
+        <v>-289.36400000000003</v>
+      </c>
+      <c r="AI15" s="62">
+        <f t="shared" si="25"/>
+        <v>-363.38332480000008</v>
+      </c>
     </row>
     <row r="16" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="30" t="s">
         <v>96</v>
       </c>
+      <c r="R16" s="30">
+        <f t="shared" ref="R16:R18" si="26">AG16-SUM(O16:Q16)</f>
+        <v>4.569</v>
+      </c>
       <c r="S16" s="30">
         <v>0.17299999999999999</v>
       </c>
       <c r="T16" s="30">
         <v>0.157</v>
       </c>
+      <c r="U16" s="30">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="V16" s="30">
+        <f t="shared" ref="V16:V20" si="27">AH16-SUM(S16:U16)</f>
+        <v>0.39200000000000013</v>
+      </c>
       <c r="W16" s="30">
         <v>0.624</v>
       </c>
       <c r="X16" s="30">
         <v>1.68</v>
       </c>
-    </row>
-    <row r="17" spans="2:24" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y16" s="30">
+        <v>6.9320000000000004</v>
+      </c>
+      <c r="Z16" s="64">
+        <f>AVERAGE(V16:Y16)</f>
+        <v>2.407</v>
+      </c>
+      <c r="AB16" s="36"/>
+      <c r="AG16" s="30">
+        <v>4.569</v>
+      </c>
+      <c r="AH16" s="30">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="AI16" s="64">
+        <f t="shared" ref="AI16:AI20" si="28">SUM(W16:Z16)</f>
+        <v>11.643000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="30" t="s">
         <v>97</v>
       </c>
+      <c r="R17" s="30">
+        <f t="shared" si="26"/>
+        <v>56.106999999999999</v>
+      </c>
       <c r="S17" s="30">
         <v>3.6579999999999999</v>
       </c>
       <c r="T17" s="30">
         <v>2.556</v>
       </c>
+      <c r="U17" s="30">
+        <v>-2.597</v>
+      </c>
+      <c r="V17" s="30">
+        <f t="shared" si="27"/>
+        <v>7.6989999999999998</v>
+      </c>
       <c r="W17" s="30">
         <v>2.4529999999999998</v>
       </c>
       <c r="X17" s="30">
         <v>2.4289999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="2:24" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y17" s="30">
+        <v>2.4969999999999999</v>
+      </c>
+      <c r="Z17" s="64">
+        <f>AVERAGE(V17:Y17)</f>
+        <v>3.7694999999999999</v>
+      </c>
+      <c r="AG17" s="30">
+        <v>56.106999999999999</v>
+      </c>
+      <c r="AH17" s="30">
+        <v>11.316000000000001</v>
+      </c>
+      <c r="AI17" s="64">
+        <f t="shared" si="28"/>
+        <v>11.148499999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="30" t="s">
         <v>98</v>
       </c>
+      <c r="R18" s="30">
+        <f t="shared" si="26"/>
+        <v>-1.851</v>
+      </c>
       <c r="S18" s="30">
         <v>-0.437</v>
       </c>
       <c r="T18" s="30">
         <v>-0.66500000000000004</v>
       </c>
+      <c r="U18" s="30">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="V18" s="30">
+        <f t="shared" si="27"/>
+        <v>-2.1499999999999995</v>
+      </c>
       <c r="W18" s="30">
         <v>1.621</v>
       </c>
       <c r="X18" s="30">
         <v>-0.224</v>
       </c>
-    </row>
-    <row r="19" spans="2:24" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y18" s="30">
+        <v>-1.3180000000000001</v>
+      </c>
+      <c r="Z18" s="64">
+        <f>AVERAGE(V18:Y18)</f>
+        <v>-0.51774999999999993</v>
+      </c>
+      <c r="AG18" s="30">
+        <v>-1.851</v>
+      </c>
+      <c r="AH18" s="30">
+        <v>-3.1349999999999998</v>
+      </c>
+      <c r="AI18" s="64">
+        <f t="shared" si="28"/>
+        <v>-0.43874999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="30" t="s">
         <v>99</v>
+      </c>
+      <c r="R19" s="30">
+        <f>R15+R16-R17+R18</f>
+        <v>-262.69299999999998</v>
       </c>
       <c r="S19" s="30">
         <f>S15+S16-S17+S18</f>
@@ -2540,6 +3101,14 @@
         <f>T15+T16-T17+T18</f>
         <v>-75.594999999999985</v>
       </c>
+      <c r="U19" s="30">
+        <f>U15+U16-U17+U18</f>
+        <v>-73.850000000000009</v>
+      </c>
+      <c r="V19" s="30">
+        <f>V15+V16-V17+V18</f>
+        <v>-88.075999999999979</v>
+      </c>
       <c r="W19" s="30">
         <f>W15+W16-W17+W18</f>
         <v>-76.147999999999982</v>
@@ -2548,27 +3117,79 @@
         <f>X15+X16-X17+X18</f>
         <v>-115.81599999999996</v>
       </c>
-    </row>
-    <row r="20" spans="2:24" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y19" s="30">
+        <f>Y15+Y16-Y17+Y18</f>
+        <v>-79.806000000000054</v>
+      </c>
+      <c r="Z19" s="64">
+        <f>Z15+Z16-Z17+Z18</f>
+        <v>-91.557574800000012</v>
+      </c>
+      <c r="AG19" s="30">
+        <f>AG15+AG16-AG17+AG18</f>
+        <v>-262.69299999999998</v>
+      </c>
+      <c r="AH19" s="30">
+        <f>AH15+AH16-AH17+AH18</f>
+        <v>-302.88900000000001</v>
+      </c>
+      <c r="AI19" s="64">
+        <f>AI15+AI16-AI17+AI18</f>
+        <v>-363.32757480000009</v>
+      </c>
+    </row>
+    <row r="20" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="30" t="s">
         <v>100</v>
       </c>
+      <c r="R20" s="30">
+        <f>AG20-SUM(O20:Q20)</f>
+        <v>4.2510000000000003</v>
+      </c>
       <c r="S20" s="30">
         <v>-1.3759999999999999</v>
       </c>
       <c r="T20" s="30">
         <v>1.538</v>
       </c>
+      <c r="U20" s="30">
+        <v>2.2490000000000001</v>
+      </c>
+      <c r="V20" s="30">
+        <f t="shared" si="27"/>
+        <v>1.5659999999999994</v>
+      </c>
       <c r="W20" s="30">
         <v>1.1459999999999999</v>
       </c>
       <c r="X20" s="30">
         <v>3.0489999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="2:24" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y20" s="30">
+        <v>5.0350000000000001</v>
+      </c>
+      <c r="Z20" s="64">
+        <f>Z19*(Z32)</f>
+        <v>4.5778787400000009</v>
+      </c>
+      <c r="AG20" s="30">
+        <v>4.2510000000000003</v>
+      </c>
+      <c r="AH20" s="30">
+        <v>3.9769999999999999</v>
+      </c>
+      <c r="AI20" s="64">
+        <f t="shared" si="28"/>
+        <v>13.807878740000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:44" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="31" t="s">
         <v>101</v>
+      </c>
+      <c r="R21" s="31">
+        <f>R19-R20</f>
+        <v>-266.94399999999996</v>
       </c>
       <c r="S21" s="31">
         <f>S19-S20</f>
@@ -2578,6 +3199,14 @@
         <f>T19-T20</f>
         <v>-77.132999999999981</v>
       </c>
+      <c r="U21" s="31">
+        <f>U19-U20</f>
+        <v>-76.099000000000004</v>
+      </c>
+      <c r="V21" s="31">
+        <f>V19-V20</f>
+        <v>-89.641999999999982</v>
+      </c>
       <c r="W21" s="31">
         <f>W19-W20</f>
         <v>-77.293999999999983</v>
@@ -2586,10 +3215,34 @@
         <f>X19-X20</f>
         <v>-118.86499999999997</v>
       </c>
-    </row>
-    <row r="22" spans="2:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y21" s="31">
+        <f>Y19-Y20</f>
+        <v>-84.841000000000051</v>
+      </c>
+      <c r="Z21" s="62">
+        <f>Z19-Z20</f>
+        <v>-96.135453540000015</v>
+      </c>
+      <c r="AG21" s="31">
+        <f>AG19-AG20</f>
+        <v>-266.94399999999996</v>
+      </c>
+      <c r="AH21" s="31">
+        <f>AH19-AH20</f>
+        <v>-306.86599999999999</v>
+      </c>
+      <c r="AI21" s="62">
+        <f>AI19-AI20</f>
+        <v>-377.13545354000007</v>
+      </c>
+    </row>
+    <row r="22" spans="2:44" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="36" t="s">
         <v>102</v>
+      </c>
+      <c r="R22" s="36">
+        <f>R21/R23</f>
+        <v>-4.525655542249635</v>
       </c>
       <c r="S22" s="36">
         <f>S21/S23</f>
@@ -2599,6 +3252,14 @@
         <f>T21/T23</f>
         <v>-1.2160968061806907</v>
       </c>
+      <c r="U22" s="36">
+        <f>U21/U23</f>
+        <v>-1.1463044248881236</v>
+      </c>
+      <c r="V22" s="36">
+        <f>V21/V23</f>
+        <v>-1.3884416085043834</v>
+      </c>
       <c r="W22" s="36">
         <f>W21/W23</f>
         <v>-1.1416038004739926</v>
@@ -2607,26 +3268,77 @@
         <f>X21/X23</f>
         <v>-1.739459023195089</v>
       </c>
-    </row>
-    <row r="23" spans="2:24" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y22" s="36">
+        <f>Y21/Y23</f>
+        <v>-1.2310638914773968</v>
+      </c>
+      <c r="Z22" s="65">
+        <f>Z21/Z23</f>
+        <v>-1.3949492055008406</v>
+      </c>
+      <c r="AG22" s="36">
+        <f>AG21/AG23</f>
+        <v>-4.525655542249635</v>
+      </c>
+      <c r="AH22" s="36">
+        <f>AH21/AH23</f>
+        <v>-4.7529676115582671</v>
+      </c>
+      <c r="AI22" s="65">
+        <f>AI21/AI23</f>
+        <v>-5.4723286977881589</v>
+      </c>
+    </row>
+    <row r="23" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="30" t="s">
         <v>3</v>
       </c>
+      <c r="R23" s="30">
+        <f>AG23</f>
+        <v>58.984603999999997</v>
+      </c>
       <c r="S23" s="30">
         <v>61.361669999999997</v>
       </c>
       <c r="T23" s="30">
         <v>63.426693999999998</v>
       </c>
+      <c r="U23" s="30">
+        <v>66.386379000000005</v>
+      </c>
+      <c r="V23" s="30">
+        <f>AH23</f>
+        <v>64.563032000000007</v>
+      </c>
       <c r="W23" s="30">
         <v>67.706502</v>
       </c>
       <c r="X23" s="30">
         <v>68.334463999999997</v>
       </c>
-    </row>
-    <row r="24" spans="2:24" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y23" s="30">
+        <v>68.916813000000005</v>
+      </c>
+      <c r="Z23" s="64">
+        <f>Y23</f>
+        <v>68.916813000000005</v>
+      </c>
+      <c r="AG23" s="30">
+        <v>58.984603999999997</v>
+      </c>
+      <c r="AH23" s="30">
+        <v>64.563032000000007</v>
+      </c>
+      <c r="AI23" s="64">
+        <f>Z23</f>
+        <v>68.916813000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Z24" s="64"/>
+      <c r="AI24" s="64"/>
+    </row>
+    <row r="26" spans="2:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>83</v>
       </c>
@@ -2638,8 +3350,51 @@
         <f>X6/T6-1</f>
         <v>0.52787211882443508</v>
       </c>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="Y26" s="32">
+        <f t="shared" ref="Y26:Z26" si="29">Y6/U6-1</f>
+        <v>0.47038912615197459</v>
+      </c>
+      <c r="Z26" s="70">
+        <f t="shared" si="29"/>
+        <v>0.40211607015542561</v>
+      </c>
+      <c r="AH26" s="32">
+        <f>AH6/AG6-1</f>
+        <v>0.48003319895660423</v>
+      </c>
+      <c r="AI26" s="70">
+        <f>AI6/AH6-1</f>
+        <v>0.48364640150518068</v>
+      </c>
+      <c r="AJ26" s="32">
+        <v>0.52</v>
+      </c>
+      <c r="AK26" s="32">
+        <v>0.48</v>
+      </c>
+      <c r="AL26" s="32">
+        <v>0.35</v>
+      </c>
+      <c r="AM26" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="AN26" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="AO26" s="32">
+        <v>0.15</v>
+      </c>
+      <c r="AP26" s="32">
+        <v>0.15</v>
+      </c>
+      <c r="AQ26" s="32">
+        <v>0.15</v>
+      </c>
+      <c r="AR26" s="32">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="27" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>84</v>
       </c>
@@ -2647,12 +3402,46 @@
         <f>T6/S6-1</f>
         <v>9.41326081212015E-2</v>
       </c>
+      <c r="U27" s="33">
+        <f>U6/T6-1</f>
+        <v>0.14161723195821807</v>
+      </c>
+      <c r="V27" s="33">
+        <f t="shared" ref="V27:W27" si="30">V6/U6-1</f>
+        <v>0.17453601477348357</v>
+      </c>
+      <c r="W27" s="33">
+        <f t="shared" si="30"/>
+        <v>7.1119800070545525E-2</v>
+      </c>
       <c r="X27" s="33">
         <f>X6/W6-1</f>
         <v>6.3805189755015812E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:24" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y27" s="33">
+        <f t="shared" ref="Y27" si="31">Y6/X6-1</f>
+        <v>9.8666271487848123E-2</v>
+      </c>
+      <c r="Z27" s="66">
+        <v>0.12</v>
+      </c>
+      <c r="AD27" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE27" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF27" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG27" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH27" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="2:44" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="33" t="s">
         <v>85</v>
       </c>
@@ -2661,19 +3450,46 @@
         <v>0.69981502686514585</v>
       </c>
       <c r="T29" s="33">
-        <f t="shared" ref="T29" si="6">T10/T6</f>
+        <f t="shared" ref="T29" si="32">T10/T6</f>
         <v>0.69457652190976471</v>
+      </c>
+      <c r="U29" s="33">
+        <f>U10/U6</f>
+        <v>0.69825424318952101</v>
+      </c>
+      <c r="V29" s="33">
+        <f t="shared" ref="V29" si="33">V10/V6</f>
+        <v>0.71557333373359255</v>
       </c>
       <c r="W29" s="33">
         <f>W10/W6</f>
         <v>0.72599116473460923</v>
       </c>
       <c r="X29" s="33">
-        <f t="shared" ref="X29" si="7">X10/X6</f>
+        <f t="shared" ref="X29:Y29" si="34">X10/X6</f>
         <v>0.70928999538958049</v>
       </c>
-    </row>
-    <row r="30" spans="2:24" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y29" s="33">
+        <f t="shared" si="34"/>
+        <v>0.71928625596110563</v>
+      </c>
+      <c r="Z29" s="66">
+        <v>0.72</v>
+      </c>
+      <c r="AG29" s="33">
+        <f t="shared" ref="AG29:AR29" si="35">AG10/AG6</f>
+        <v>0.7000643653240286</v>
+      </c>
+      <c r="AH29" s="33">
+        <f t="shared" si="35"/>
+        <v>0.703024324144924</v>
+      </c>
+      <c r="AI29" s="66">
+        <f t="shared" ref="AI29" si="36">AI10/AI6</f>
+        <v>0.71862682611084105</v>
+      </c>
+    </row>
+    <row r="30" spans="2:44" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="33" t="s">
         <v>86</v>
       </c>
@@ -2682,19 +3498,47 @@
         <v>-0.33826962036466146</v>
       </c>
       <c r="T30" s="33">
-        <f t="shared" ref="T30" si="8">T15/T6</f>
+        <f t="shared" ref="T30" si="37">T15/T6</f>
         <v>-0.3649413576053977</v>
+      </c>
+      <c r="U30" s="33">
+        <f>U15/U6</f>
+        <v>-0.33834450600062582</v>
+      </c>
+      <c r="V30" s="33">
+        <f t="shared" ref="V30" si="38">V15/V6</f>
+        <v>-0.29501227044511308</v>
       </c>
       <c r="W30" s="33">
         <f>W15/W6</f>
         <v>-0.26603887937165205</v>
       </c>
       <c r="X30" s="33">
-        <f t="shared" ref="X30" si="9">X15/X6</f>
+        <f t="shared" ref="X30:Z31" si="39">X15/X6</f>
         <v>-0.37819600869393383</v>
       </c>
-    </row>
-    <row r="31" spans="2:24" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y30" s="33">
+        <f t="shared" si="39"/>
+        <v>-0.24855449746868472</v>
+      </c>
+      <c r="Z30" s="66">
+        <f t="shared" si="39"/>
+        <v>-0.24000000000000002</v>
+      </c>
+      <c r="AG30" s="33">
+        <f t="shared" ref="AG30:AH30" si="40">AG15/AG6</f>
+        <v>-0.35452420474948332</v>
+      </c>
+      <c r="AH30" s="33">
+        <f t="shared" si="40"/>
+        <v>-0.33116269275402793</v>
+      </c>
+      <c r="AI30" s="66">
+        <f t="shared" ref="AI30" si="41">AI15/AI6</f>
+        <v>-0.2803054182607938</v>
+      </c>
+    </row>
+    <row r="31" spans="2:44" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="33" t="s">
         <v>87</v>
       </c>
@@ -2703,19 +3547,47 @@
         <v>-0.35228573945212732</v>
       </c>
       <c r="T31" s="33">
-        <f t="shared" ref="T31" si="10">T21/T6</f>
+        <f t="shared" ref="T31" si="42">T21/T6</f>
         <v>-0.38809642409696737</v>
+      </c>
+      <c r="U31" s="33">
+        <f>U21/U6</f>
+        <v>-0.33539597960272022</v>
+      </c>
+      <c r="V31" s="33">
+        <f t="shared" ref="V31" si="43">V21/V6</f>
+        <v>-0.336375303008698</v>
       </c>
       <c r="W31" s="33">
         <f>W21/W6</f>
         <v>-0.27078231685742005</v>
       </c>
       <c r="X31" s="33">
-        <f t="shared" ref="X31" si="11">X21/X6</f>
+        <f t="shared" ref="X31:Z31" si="44">X21/X6</f>
         <v>-0.39144108542448774</v>
       </c>
-    </row>
-    <row r="32" spans="2:24" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y31" s="33">
+        <f t="shared" si="44"/>
+        <v>-0.2543035360483904</v>
+      </c>
+      <c r="Z31" s="66">
+        <f t="shared" si="44"/>
+        <v>-0.2572836433407969</v>
+      </c>
+      <c r="AG31" s="33">
+        <f t="shared" ref="AG31:AH31" si="45">AG21/AG6</f>
+        <v>-0.45215623835495777</v>
+      </c>
+      <c r="AH31" s="33">
+        <f t="shared" si="45"/>
+        <v>-0.35119286046176273</v>
+      </c>
+      <c r="AI31" s="66">
+        <f t="shared" ref="AI31" si="46">AI21/AI6</f>
+        <v>-0.29091348950501938</v>
+      </c>
+    </row>
+    <row r="32" spans="2:44" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="33" t="s">
         <v>88</v>
       </c>
@@ -2724,24 +3596,51 @@
         <v>2.1050055072818496E-2</v>
       </c>
       <c r="T32" s="33">
-        <f t="shared" ref="T32" si="12">T20/T19</f>
+        <f t="shared" ref="T32" si="47">T20/T19</f>
         <v>-2.0345260929955689E-2</v>
+      </c>
+      <c r="U32" s="33">
+        <f>U20/U19</f>
+        <v>-3.0453622207176706E-2</v>
+      </c>
+      <c r="V32" s="33">
+        <f t="shared" ref="V32" si="48">V20/V19</f>
+        <v>-1.7780099005404421E-2</v>
       </c>
       <c r="W32" s="33">
         <f>W20/W19</f>
         <v>-1.5049640174397229E-2</v>
       </c>
       <c r="X32" s="33">
-        <f t="shared" ref="X32" si="13">X20/X19</f>
+        <f t="shared" ref="X32:Y32" si="49">X20/X19</f>
         <v>-2.6326241624645998E-2</v>
       </c>
-    </row>
-    <row r="36" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="Y32" s="33">
+        <f t="shared" si="49"/>
+        <v>-6.3090494449038872E-2</v>
+      </c>
+      <c r="Z32" s="66">
+        <v>-0.05</v>
+      </c>
+      <c r="AG32" s="33">
+        <f t="shared" ref="AG32:AH32" si="50">AG20/AG19</f>
+        <v>-1.6182387806298611E-2</v>
+      </c>
+      <c r="AH32" s="33">
+        <f t="shared" si="50"/>
+        <v>-1.3130222622809015E-2</v>
+      </c>
+      <c r="AI32" s="66">
+        <f t="shared" ref="AI32" si="51">AI20/AI19</f>
+        <v>-3.8003938312694226E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B36" s="37" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>5</v>
       </c>
@@ -2753,13 +3652,21 @@
       </c>
       <c r="X37" s="31">
         <v>651.41999999999996</v>
+      </c>
+      <c r="Y37" s="31">
+        <v>999.67399999999998</v>
+      </c>
+      <c r="Z37" s="63"/>
+      <c r="AG37" s="31">
+        <v>429.697</v>
       </c>
       <c r="AH37" s="31">
         <f>V37</f>
         <v>473.904</v>
       </c>
-    </row>
-    <row r="38" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI37" s="62"/>
+    </row>
+    <row r="38" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>104</v>
       </c>
@@ -2771,13 +3678,21 @@
       </c>
       <c r="X38" s="31">
         <v>1144.192</v>
+      </c>
+      <c r="Y38" s="31">
+        <v>787.85799999999995</v>
+      </c>
+      <c r="Z38" s="63"/>
+      <c r="AG38" s="31">
+        <v>528.04499999999996</v>
       </c>
       <c r="AH38" s="31">
         <f>V38</f>
         <v>1352.019</v>
       </c>
-    </row>
-    <row r="39" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AI38" s="62"/>
+    </row>
+    <row r="39" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>105</v>
       </c>
@@ -2789,13 +3704,19 @@
       </c>
       <c r="X39" s="30">
         <v>213.267</v>
+      </c>
+      <c r="Y39" s="30">
+        <v>231.26</v>
+      </c>
+      <c r="AG39" s="30">
+        <v>135.17599999999999</v>
       </c>
       <c r="AH39" s="30">
         <f>V39</f>
         <v>195.38300000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>106</v>
       </c>
@@ -2808,12 +3729,18 @@
       <c r="X40" s="30">
         <v>72.069000000000003</v>
       </c>
+      <c r="Y40" s="30">
+        <v>77.445999999999998</v>
+      </c>
+      <c r="AG40" s="30">
+        <v>36.619</v>
+      </c>
       <c r="AH40" s="30">
-        <f t="shared" ref="AH40:AH47" si="14">V40</f>
+        <f t="shared" ref="AH40:AH47" si="52">V40</f>
         <v>63.523000000000003</v>
       </c>
     </row>
-    <row r="41" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>107</v>
       </c>
@@ -2826,93 +3753,99 @@
       <c r="X41" s="30">
         <v>27.565999999999999</v>
       </c>
+      <c r="Y41" s="30">
+        <v>26.016999999999999</v>
+      </c>
+      <c r="AG41" s="30">
+        <v>12.35</v>
+      </c>
       <c r="AH41" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="52"/>
         <v>32.573</v>
       </c>
     </row>
-    <row r="42" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C42" s="30">
-        <f t="shared" ref="C42:V42" si="15">SUM(C37:C41)</f>
+        <f t="shared" ref="C42:V42" si="53">SUM(C37:C41)</f>
         <v>0</v>
       </c>
       <c r="D42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="E42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="F42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="G42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="H42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="I42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="J42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="K42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="L42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="M42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="O42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="P42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="Q42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="R42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="S42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="T42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="U42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="V42" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="53"/>
         <v>2117.402</v>
       </c>
       <c r="W42" s="30">
@@ -2920,15 +3853,23 @@
         <v>2096.3070000000002</v>
       </c>
       <c r="X42" s="30">
-        <f t="shared" ref="X42" si="16">SUM(X37:X41)</f>
+        <f t="shared" ref="X42:Y42" si="54">SUM(X37:X41)</f>
         <v>2108.5140000000001</v>
       </c>
+      <c r="Y42" s="30">
+        <f t="shared" si="54"/>
+        <v>2122.2549999999997</v>
+      </c>
+      <c r="AG42" s="30">
+        <f t="shared" ref="AG42:AH42" si="55">SUM(AG37:AG41)</f>
+        <v>1141.8869999999997</v>
+      </c>
       <c r="AH42" s="30">
-        <f t="shared" ref="AH42" si="17">SUM(AH37:AH41)</f>
+        <f t="shared" si="55"/>
         <v>2117.402</v>
       </c>
     </row>
-    <row r="43" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>109</v>
       </c>
@@ -2941,12 +3882,18 @@
       <c r="X43" s="30">
         <v>61.603999999999999</v>
       </c>
+      <c r="Y43" s="30">
+        <v>59.488999999999997</v>
+      </c>
+      <c r="AG43" s="30">
+        <v>62.363999999999997</v>
+      </c>
       <c r="AH43" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="52"/>
         <v>62.625</v>
       </c>
     </row>
-    <row r="44" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>110</v>
       </c>
@@ -2959,12 +3906,18 @@
       <c r="X44" s="30">
         <v>46.417999999999999</v>
       </c>
+      <c r="Y44" s="30">
+        <v>43.484999999999999</v>
+      </c>
+      <c r="AG44" s="30">
+        <v>34.587000000000003</v>
+      </c>
       <c r="AH44" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="52"/>
         <v>41.744999999999997</v>
       </c>
     </row>
-    <row r="45" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>111</v>
       </c>
@@ -2980,12 +3933,20 @@
         <f>16.018+57.779</f>
         <v>73.796999999999997</v>
       </c>
+      <c r="Y45" s="30">
+        <f>57.779+13.723</f>
+        <v>71.50200000000001</v>
+      </c>
+      <c r="AG45" s="30">
+        <f>55.83+26.275</f>
+        <v>82.10499999999999</v>
+      </c>
       <c r="AH45" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="52"/>
         <v>78.382999999999996</v>
       </c>
     </row>
-    <row r="46" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>112</v>
       </c>
@@ -2998,12 +3959,18 @@
       <c r="X46" s="30">
         <v>2.1629999999999998</v>
       </c>
+      <c r="Y46" s="30">
+        <v>1.657</v>
+      </c>
+      <c r="AG46" s="30">
+        <v>0.997</v>
+      </c>
       <c r="AH46" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="52"/>
         <v>1.9390000000000001</v>
       </c>
     </row>
-    <row r="47" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>113</v>
       </c>
@@ -3016,93 +3983,99 @@
       <c r="X47" s="30">
         <v>159.102</v>
       </c>
+      <c r="Y47" s="30">
+        <v>168.798</v>
+      </c>
+      <c r="AG47" s="30">
+        <v>85.555000000000007</v>
+      </c>
       <c r="AH47" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="52"/>
         <v>147.494</v>
       </c>
     </row>
-    <row r="48" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C48" s="30">
-        <f t="shared" ref="C48:V48" si="18">C42+SUM(C43:C47)</f>
+        <f t="shared" ref="C48:V48" si="56">C42+SUM(C43:C47)</f>
         <v>0</v>
       </c>
       <c r="D48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="E48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="F48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="G48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="H48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="I48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="J48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="K48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="L48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="M48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="N48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="O48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="P48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="Q48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="R48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="S48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="T48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="U48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="V48" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="56"/>
         <v>2449.5880000000002</v>
       </c>
       <c r="W48" s="30">
@@ -3113,154 +4086,222 @@
         <f>X42+SUM(X43:X47)</f>
         <v>2451.598</v>
       </c>
+      <c r="Y48" s="30">
+        <f>Y42+SUM(Y43:Y47)</f>
+        <v>2467.1859999999997</v>
+      </c>
+      <c r="AG48" s="30">
+        <f>AG42+SUM(AG43:AG47)</f>
+        <v>1407.4949999999997</v>
+      </c>
       <c r="AH48" s="30">
         <f>AH42+SUM(AH43:AH47)</f>
         <v>2449.5880000000002</v>
       </c>
     </row>
-    <row r="50" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="V50" s="30">
+        <v>5.234</v>
+      </c>
       <c r="W50" s="30">
         <v>6.2039999999999997</v>
       </c>
+      <c r="X50" s="30">
+        <v>7.3029999999999999</v>
+      </c>
+      <c r="Y50" s="30">
+        <v>7.734</v>
+      </c>
+      <c r="AG50" s="30">
+        <v>4.1440000000000001</v>
+      </c>
       <c r="AH50" s="30">
         <f>V50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:34" x14ac:dyDescent="0.2">
+        <v>5.234</v>
+      </c>
+    </row>
+    <row r="51" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="V51" s="30">
+        <v>112.568</v>
+      </c>
       <c r="W51" s="30">
         <v>87.716999999999999</v>
       </c>
+      <c r="X51" s="30">
+        <v>83.805999999999997</v>
+      </c>
+      <c r="Y51" s="30">
+        <v>84.442999999999998</v>
+      </c>
+      <c r="AG51" s="30">
+        <v>70.209999999999994</v>
+      </c>
       <c r="AH51" s="30">
-        <f t="shared" ref="AH51:AH54" si="19">V51</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:34" x14ac:dyDescent="0.2">
+        <f t="shared" ref="AH51:AH54" si="57">V51</f>
+        <v>112.568</v>
+      </c>
+    </row>
+    <row r="52" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="V52" s="30">
+        <v>8.0839999999999996</v>
+      </c>
       <c r="W52" s="30">
         <v>8.6709999999999994</v>
       </c>
+      <c r="X52" s="30">
+        <v>9.1630000000000003</v>
+      </c>
+      <c r="Y52" s="30">
+        <v>8.6449999999999996</v>
+      </c>
+      <c r="AG52" s="30">
+        <v>2.343</v>
+      </c>
       <c r="AH52" s="30">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:34" x14ac:dyDescent="0.2">
+        <f t="shared" si="57"/>
+        <v>8.0839999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="V53" s="30">
+        <v>48.847999999999999</v>
+      </c>
       <c r="W53" s="30">
         <v>49.216000000000001</v>
       </c>
+      <c r="X53" s="30">
+        <v>73.915999999999997</v>
+      </c>
+      <c r="Y53" s="30">
+        <v>52.826000000000001</v>
+      </c>
+      <c r="AG53" s="30">
+        <v>56.44</v>
+      </c>
       <c r="AH53" s="30">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:34" x14ac:dyDescent="0.2">
+        <f t="shared" si="57"/>
+        <v>48.847999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="V54" s="30">
+        <v>352.00099999999998</v>
+      </c>
       <c r="W54" s="30">
         <v>351.91399999999999</v>
       </c>
+      <c r="X54" s="30">
+        <v>350.709</v>
+      </c>
+      <c r="Y54" s="30">
+        <v>364.15899999999999</v>
+      </c>
+      <c r="AG54" s="30">
+        <v>221.404</v>
+      </c>
       <c r="AH54" s="30">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="2:34" x14ac:dyDescent="0.2">
+        <f t="shared" si="57"/>
+        <v>352.00099999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C55" s="30">
-        <f t="shared" ref="C55:V55" si="20">SUM(C50:C54)</f>
+        <f t="shared" ref="C55:V55" si="58">SUM(C50:C54)</f>
         <v>0</v>
       </c>
       <c r="D55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="E55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="F55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="G55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="H55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="I55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="J55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="K55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="L55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="M55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="N55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="O55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="P55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="Q55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="R55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="S55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="T55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="U55" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="V55" s="30">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <f t="shared" si="58"/>
+        <v>526.7349999999999</v>
       </c>
       <c r="W55" s="30">
         <f>SUM(W50:W54)</f>
@@ -3268,156 +4309,226 @@
       </c>
       <c r="X55" s="30">
         <f>SUM(X50:X54)</f>
-        <v>0</v>
+        <v>524.89699999999993</v>
+      </c>
+      <c r="Y55" s="30">
+        <f>SUM(Y50:Y54)</f>
+        <v>517.80700000000002</v>
+      </c>
+      <c r="AG55" s="30">
+        <f>SUM(AG50:AG54)</f>
+        <v>354.541</v>
       </c>
       <c r="AH55" s="30">
         <f>SUM(AH50:AH54)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:34" x14ac:dyDescent="0.2">
+        <v>526.7349999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="V56" s="30">
+        <v>8.1000000000000003E-2</v>
+      </c>
       <c r="W56" s="30">
         <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="X56" s="30">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="Y56" s="30">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="AG56" s="30">
+        <v>0.77300000000000002</v>
       </c>
       <c r="AH56" s="30">
         <f>W56</f>
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="V57" s="30">
+        <v>38.707000000000001</v>
+      </c>
       <c r="W57" s="30">
         <v>40.279000000000003</v>
       </c>
+      <c r="X57" s="30">
+        <v>40.436999999999998</v>
+      </c>
+      <c r="Y57" s="30">
+        <v>37.261000000000003</v>
+      </c>
+      <c r="AG57" s="30">
+        <v>39.094999999999999</v>
+      </c>
       <c r="AH57" s="30">
         <f>V57</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:34" x14ac:dyDescent="0.2">
+        <v>38.707000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="V58" s="30">
+        <v>23.178999999999998</v>
+      </c>
       <c r="W58" s="30">
         <v>23.555</v>
       </c>
+      <c r="X58" s="30">
+        <v>24.462</v>
+      </c>
+      <c r="Y58" s="30">
+        <v>34.014000000000003</v>
+      </c>
+      <c r="AG58" s="30">
+        <v>16.547000000000001</v>
+      </c>
       <c r="AH58" s="30">
-        <f t="shared" ref="AH58" si="21">V58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="AH58" si="59">V58</f>
+        <v>23.178999999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
         <v>121</v>
       </c>
+      <c r="V59" s="31">
+        <v>1136.521</v>
+      </c>
       <c r="W59" s="31">
         <v>1137.3610000000001</v>
       </c>
+      <c r="X59" s="31">
+        <v>1138.2</v>
+      </c>
+      <c r="Y59" s="31">
+        <v>1139.0419999999999</v>
+      </c>
+      <c r="Z59" s="63"/>
+      <c r="AG59" s="31">
+        <v>937.72900000000004</v>
+      </c>
       <c r="AH59" s="31">
         <f>V59</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:34" x14ac:dyDescent="0.2">
+        <v>1136.521</v>
+      </c>
+      <c r="AI59" s="62"/>
+    </row>
+    <row r="60" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
         <v>122</v>
       </c>
+      <c r="V60" s="30">
+        <v>57.664999999999999</v>
+      </c>
       <c r="W60" s="31">
         <v>56.652000000000001</v>
       </c>
-      <c r="AH60" s="31">
-        <f t="shared" ref="AH60" si="22">V60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="X60" s="30">
+        <v>55.338999999999999</v>
+      </c>
+      <c r="Y60" s="30">
+        <v>54.374000000000002</v>
+      </c>
+      <c r="AG60" s="30">
+        <v>59.128999999999998</v>
+      </c>
+      <c r="AH60" s="30">
+        <f t="shared" ref="AH60" si="60">V60</f>
+        <v>57.664999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C61" s="30">
-        <f t="shared" ref="C61:V61" si="23">C55+SUM(C56:C60)</f>
+        <f t="shared" ref="C61:V61" si="61">C55+SUM(C56:C60)</f>
         <v>0</v>
       </c>
       <c r="D61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="E61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="F61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="G61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="H61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="I61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="J61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="K61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="L61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="M61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="N61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="O61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="P61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="Q61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="R61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="S61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="T61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="U61" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="V61" s="30">
-        <f t="shared" si="23"/>
-        <v>0</v>
+        <f t="shared" si="61"/>
+        <v>1782.8879999999999</v>
       </c>
       <c r="W61" s="30">
         <f>W55+SUM(W56:W60)</f>
@@ -3425,390 +4536,447 @@
       </c>
       <c r="X61" s="30">
         <f>X55+SUM(X56:X60)</f>
-        <v>0</v>
+        <v>1783.4299999999998</v>
+      </c>
+      <c r="Y61" s="30">
+        <f>Y55+SUM(Y56:Y60)</f>
+        <v>1782.904</v>
+      </c>
+      <c r="AG61" s="30">
+        <f>AG55+SUM(AG56:AG60)</f>
+        <v>1407.8139999999999</v>
       </c>
       <c r="AH61" s="30">
         <f>AH55+SUM(AH56:AH60)</f>
-        <v>9.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="2:34" x14ac:dyDescent="0.2">
+        <v>1782.8999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="V63" s="1">
+        <v>666.7</v>
+      </c>
       <c r="W63" s="30">
         <v>672.87900000000002</v>
       </c>
+      <c r="X63" s="30">
+        <v>668.16800000000001</v>
+      </c>
+      <c r="Y63" s="30">
+        <v>684.28200000000004</v>
+      </c>
+      <c r="AG63" s="1">
+        <v>-5.0330000000000004</v>
+      </c>
       <c r="AH63" s="1">
         <f>V63</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:34" x14ac:dyDescent="0.2">
+        <v>666.7</v>
+      </c>
+    </row>
+    <row r="64" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C64" s="30">
-        <f t="shared" ref="C64" si="24">C63+C61</f>
+        <f t="shared" ref="C64" si="62">C63+C61</f>
         <v>0</v>
       </c>
       <c r="D64" s="30">
-        <f t="shared" ref="D64" si="25">D63+D61</f>
+        <f t="shared" ref="D64" si="63">D63+D61</f>
         <v>0</v>
       </c>
       <c r="E64" s="30">
-        <f t="shared" ref="E64" si="26">E63+E61</f>
+        <f t="shared" ref="E64" si="64">E63+E61</f>
         <v>0</v>
       </c>
       <c r="F64" s="30">
-        <f t="shared" ref="F64" si="27">F63+F61</f>
+        <f t="shared" ref="F64" si="65">F63+F61</f>
         <v>0</v>
       </c>
       <c r="G64" s="30">
-        <f t="shared" ref="G64" si="28">G63+G61</f>
+        <f t="shared" ref="G64" si="66">G63+G61</f>
         <v>0</v>
       </c>
       <c r="H64" s="30">
-        <f t="shared" ref="H64" si="29">H63+H61</f>
+        <f t="shared" ref="H64" si="67">H63+H61</f>
         <v>0</v>
       </c>
       <c r="I64" s="30">
-        <f t="shared" ref="I64" si="30">I63+I61</f>
+        <f t="shared" ref="I64" si="68">I63+I61</f>
         <v>0</v>
       </c>
       <c r="J64" s="30">
-        <f t="shared" ref="J64" si="31">J63+J61</f>
+        <f t="shared" ref="J64" si="69">J63+J61</f>
         <v>0</v>
       </c>
       <c r="K64" s="30">
-        <f t="shared" ref="K64" si="32">K63+K61</f>
+        <f t="shared" ref="K64" si="70">K63+K61</f>
         <v>0</v>
       </c>
       <c r="L64" s="30">
-        <f t="shared" ref="L64" si="33">L63+L61</f>
+        <f t="shared" ref="L64" si="71">L63+L61</f>
         <v>0</v>
       </c>
       <c r="M64" s="30">
-        <f t="shared" ref="M64" si="34">M63+M61</f>
+        <f t="shared" ref="M64" si="72">M63+M61</f>
         <v>0</v>
       </c>
       <c r="N64" s="30">
-        <f t="shared" ref="N64" si="35">N63+N61</f>
+        <f t="shared" ref="N64" si="73">N63+N61</f>
         <v>0</v>
       </c>
       <c r="O64" s="30">
-        <f t="shared" ref="O64" si="36">O63+O61</f>
+        <f t="shared" ref="O64" si="74">O63+O61</f>
         <v>0</v>
       </c>
       <c r="P64" s="30">
-        <f t="shared" ref="P64" si="37">P63+P61</f>
+        <f t="shared" ref="P64" si="75">P63+P61</f>
         <v>0</v>
       </c>
       <c r="Q64" s="30">
-        <f t="shared" ref="Q64" si="38">Q63+Q61</f>
+        <f t="shared" ref="Q64" si="76">Q63+Q61</f>
         <v>0</v>
       </c>
       <c r="R64" s="30">
-        <f t="shared" ref="R64" si="39">R63+R61</f>
+        <f t="shared" ref="R64" si="77">R63+R61</f>
         <v>0</v>
       </c>
       <c r="S64" s="30">
-        <f t="shared" ref="S64" si="40">S63+S61</f>
+        <f t="shared" ref="S64" si="78">S63+S61</f>
         <v>0</v>
       </c>
       <c r="T64" s="30">
-        <f t="shared" ref="T64" si="41">T63+T61</f>
+        <f t="shared" ref="T64" si="79">T63+T61</f>
         <v>0</v>
       </c>
       <c r="U64" s="30">
-        <f t="shared" ref="U64" si="42">U63+U61</f>
+        <f t="shared" ref="U64" si="80">U63+U61</f>
         <v>0</v>
       </c>
       <c r="V64" s="30">
-        <f t="shared" ref="V64" si="43">V63+V61</f>
-        <v>0</v>
+        <f t="shared" ref="V64" si="81">V63+V61</f>
+        <v>2449.5879999999997</v>
       </c>
       <c r="W64" s="30">
-        <f t="shared" ref="W64" si="44">W63+W61</f>
+        <f t="shared" ref="W64:Y64" si="82">W63+W61</f>
         <v>2434.5410000000002</v>
       </c>
       <c r="X64" s="30">
-        <f t="shared" ref="X64" si="45">X63+X61</f>
-        <v>0</v>
+        <f t="shared" ref="X64" si="83">X63+X61</f>
+        <v>2451.598</v>
+      </c>
+      <c r="Y64" s="30">
+        <f t="shared" si="82"/>
+        <v>2467.1860000000001</v>
+      </c>
+      <c r="AF64" s="57"/>
+      <c r="AG64" s="30">
+        <f>AG63+AG61</f>
+        <v>1402.7809999999999</v>
       </c>
       <c r="AH64" s="30">
-        <f t="shared" ref="AH64" si="46">AH63+AH61</f>
-        <v>9.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="2:24" x14ac:dyDescent="0.2">
+        <f t="shared" ref="AG64:AH64" si="84">AH63+AH61</f>
+        <v>2449.6</v>
+      </c>
+    </row>
+    <row r="65" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AF65" s="57"/>
+    </row>
+    <row r="66" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
         <v>126</v>
       </c>
       <c r="C66" s="30">
-        <f t="shared" ref="C66:W66" si="47">C48-C61</f>
+        <f t="shared" ref="C66:V66" si="85">C48-C61</f>
         <v>0</v>
       </c>
       <c r="D66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="E66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="F66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="G66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="H66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="I66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="J66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="K66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="L66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="M66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="N66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="O66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="P66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="Q66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="R66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="S66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="T66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="U66" s="30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="V66" s="30">
-        <f t="shared" si="47"/>
-        <v>2449.5880000000002</v>
+        <f t="shared" si="85"/>
+        <v>666.70000000000027</v>
       </c>
       <c r="W66" s="30">
         <f>W48-W61</f>
         <v>672.87900000000013</v>
       </c>
       <c r="X66" s="30">
-        <f t="shared" ref="X66" si="48">X48-X61</f>
-        <v>2451.598</v>
-      </c>
-    </row>
-    <row r="67" spans="2:24" x14ac:dyDescent="0.2">
+        <f t="shared" ref="X66:Y66" si="86">X48-X61</f>
+        <v>668.16800000000012</v>
+      </c>
+      <c r="Y66" s="30">
+        <f t="shared" si="86"/>
+        <v>684.2819999999997</v>
+      </c>
+      <c r="AF66" s="57"/>
+      <c r="AG66" s="30">
+        <f t="shared" ref="AG66:AH66" si="87">AG48-AG61</f>
+        <v>-0.31900000000018736</v>
+      </c>
+      <c r="AH66" s="30">
+        <f t="shared" si="87"/>
+        <v>666.68800000000033</v>
+      </c>
+    </row>
+    <row r="67" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C67" s="1" t="e">
-        <f t="shared" ref="C67:V67" si="49">C66/C23</f>
+        <f t="shared" ref="C67:V67" si="88">C66/C23</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q67" s="1" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R67" s="1" t="e">
-        <f t="shared" si="49"/>
-        <v>#DIV/0!</v>
+      <c r="R67" s="1">
+        <f t="shared" si="88"/>
+        <v>0</v>
       </c>
       <c r="S67" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="T67" s="1">
-        <f t="shared" si="49"/>
-        <v>0</v>
-      </c>
-      <c r="U67" s="1" t="e">
-        <f t="shared" si="49"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V67" s="1" t="e">
-        <f t="shared" si="49"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+      <c r="U67" s="1">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+      <c r="V67" s="1">
+        <f>V66/V23</f>
+        <v>10.326342790096973</v>
       </c>
       <c r="W67" s="1">
         <f>W66/W23</f>
         <v>9.9381740323846604</v>
       </c>
       <c r="X67" s="1">
-        <f t="shared" ref="X67" si="50">X66/X23</f>
-        <v>35.876450278442221</v>
-      </c>
-    </row>
-    <row r="69" spans="2:24" s="38" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="X67:Y67" si="89">X66/X23</f>
+        <v>9.7779065041031146</v>
+      </c>
+      <c r="Y67" s="1">
+        <f t="shared" si="89"/>
+        <v>9.929101045342879</v>
+      </c>
+      <c r="AG67" s="1">
+        <f t="shared" ref="AG67:AH67" si="90">AG66/AG23</f>
+        <v>-5.4081909238584934E-3</v>
+      </c>
+      <c r="AH67" s="1">
+        <f t="shared" si="90"/>
+        <v>10.326156925219998</v>
+      </c>
+    </row>
+    <row r="69" spans="2:35" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B69" s="38" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="34">
-        <f t="shared" ref="C69:W69" si="51">C37+C38</f>
+        <f t="shared" ref="C69:V69" si="91">C37+C38</f>
         <v>0</v>
       </c>
       <c r="D69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="E69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="F69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="G69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="H69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="I69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="J69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="K69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="L69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="M69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="N69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="O69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="P69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="Q69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="R69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="S69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="T69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="U69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="V69" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="91"/>
         <v>1825.923</v>
       </c>
       <c r="W69" s="34">
@@ -3819,90 +4987,104 @@
         <f>X37+X38</f>
         <v>1795.6120000000001</v>
       </c>
-    </row>
-    <row r="70" spans="2:24" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y69" s="34">
+        <f t="shared" ref="Y69" si="92">Y37+Y38</f>
+        <v>1787.5319999999999</v>
+      </c>
+      <c r="Z69" s="59"/>
+      <c r="AG69" s="34">
+        <f t="shared" ref="AG69:AH69" si="93">AG37+AG38</f>
+        <v>957.74199999999996</v>
+      </c>
+      <c r="AH69" s="34">
+        <f t="shared" si="93"/>
+        <v>1825.923</v>
+      </c>
+      <c r="AI69" s="64"/>
+    </row>
+    <row r="70" spans="2:35" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="38" t="s">
         <v>6</v>
       </c>
       <c r="C70" s="34">
-        <f t="shared" ref="C70:W70" si="52">C59</f>
+        <f t="shared" ref="C70:V70" si="94">C59</f>
         <v>0</v>
       </c>
       <c r="D70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="E70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="F70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="G70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="H70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="I70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="J70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="K70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="L70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="M70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="N70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="O70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="P70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="Q70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="R70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="S70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="T70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="U70" s="34">
-        <f t="shared" si="52"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="V70" s="34">
-        <f t="shared" si="52"/>
-        <v>0</v>
+        <f t="shared" si="94"/>
+        <v>1136.521</v>
       </c>
       <c r="W70" s="34">
         <f>W59</f>
@@ -3910,92 +5092,106 @@
       </c>
       <c r="X70" s="34">
         <f>X59</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="2:24" x14ac:dyDescent="0.2">
+        <v>1138.2</v>
+      </c>
+      <c r="Y70" s="34">
+        <f t="shared" ref="Y70" si="95">Y59</f>
+        <v>1139.0419999999999</v>
+      </c>
+      <c r="Z70" s="59"/>
+      <c r="AG70" s="34">
+        <f t="shared" ref="AG70:AH70" si="96">AG59</f>
+        <v>937.72900000000004</v>
+      </c>
+      <c r="AH70" s="34">
+        <f t="shared" si="96"/>
+        <v>1136.521</v>
+      </c>
+      <c r="AI70" s="64"/>
+    </row>
+    <row r="71" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C71" s="30">
-        <f t="shared" ref="C71:V71" si="53">C69-C70</f>
+        <f t="shared" ref="C71:V71" si="97">C69-C70</f>
         <v>0</v>
       </c>
       <c r="D71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="E71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="F71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="G71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="H71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="I71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="J71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="K71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="L71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="M71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="N71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="O71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="P71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="Q71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="R71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="S71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="T71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="U71" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="V71" s="30">
-        <f t="shared" si="53"/>
-        <v>1825.923</v>
+        <f t="shared" si="97"/>
+        <v>689.40200000000004</v>
       </c>
       <c r="W71" s="30">
         <f>W69-W70</f>
@@ -4003,65 +5199,228 @@
       </c>
       <c r="X71" s="30">
         <f>X69-X70</f>
-        <v>1795.6120000000001</v>
-      </c>
-    </row>
-    <row r="73" spans="2:24" x14ac:dyDescent="0.2">
+        <v>657.41200000000003</v>
+      </c>
+      <c r="Y71" s="30">
+        <f t="shared" ref="Y71" si="98">Y69-Y70</f>
+        <v>648.49</v>
+      </c>
+      <c r="AG71" s="30">
+        <f t="shared" ref="AG71" si="99">AG69-AG70</f>
+        <v>20.01299999999992</v>
+      </c>
+      <c r="AH71" s="30">
+        <f t="shared" ref="AH71" si="100">AH69-AH70</f>
+        <v>689.40200000000004</v>
+      </c>
+    </row>
+    <row r="73" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="V73" s="1">
+        <v>405.11</v>
+      </c>
       <c r="W73" s="30">
         <v>354.93</v>
       </c>
-    </row>
-    <row r="74" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="X73" s="1">
+        <v>312.47000000000003</v>
+      </c>
+      <c r="Y73" s="1">
+        <v>183.03</v>
+      </c>
+      <c r="AG73" s="1">
+        <v>369.61</v>
+      </c>
+      <c r="AH73" s="1">
+        <f>V73</f>
+        <v>405.11</v>
+      </c>
+    </row>
+    <row r="74" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="V74" s="30">
+        <f t="shared" ref="V74" si="101">V73*V23</f>
+        <v>26155.129893520003</v>
       </c>
       <c r="W74" s="30">
         <f>W73*W23</f>
         <v>24031.06875486</v>
       </c>
-    </row>
-    <row r="75" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="X74" s="30">
+        <f t="shared" ref="X74:Y74" si="102">X73*X23</f>
+        <v>21352.46996608</v>
+      </c>
+      <c r="Y74" s="30">
+        <f t="shared" si="102"/>
+        <v>12613.844283390001</v>
+      </c>
+      <c r="AG74" s="30">
+        <f t="shared" ref="AG74" si="103">AG73*AG23</f>
+        <v>21801.299484439998</v>
+      </c>
+      <c r="AH74" s="30">
+        <f>AH73*AH23</f>
+        <v>26155.129893520003</v>
+      </c>
+    </row>
+    <row r="75" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="V75" s="30">
+        <f t="shared" ref="V75" si="104">V74-V71</f>
+        <v>25465.727893520001</v>
       </c>
       <c r="W75" s="30">
         <f>W74-W71</f>
         <v>23339.734754860001</v>
       </c>
-    </row>
-    <row r="77" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="X75" s="30">
+        <f t="shared" ref="X75:Y75" si="105">X74-X71</f>
+        <v>20695.057966079999</v>
+      </c>
+      <c r="Y75" s="30">
+        <f t="shared" si="105"/>
+        <v>11965.354283390001</v>
+      </c>
+      <c r="AG75" s="30">
+        <f t="shared" ref="AG75" si="106">AG74-AG71</f>
+        <v>21781.286484439999</v>
+      </c>
+      <c r="AH75" s="30">
+        <f>AH74-AH71</f>
+        <v>25465.727893520001</v>
+      </c>
+    </row>
+    <row r="77" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W77" s="50">
+      <c r="V77" s="40">
+        <f>V73/V67</f>
+        <v>39.230733303614812</v>
+      </c>
+      <c r="W77" s="40">
         <f>W73/W67</f>
         <v>35.713804049256993</v>
       </c>
-    </row>
-    <row r="78" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="X77" s="40">
+        <f t="shared" ref="X77:Y77" si="107">X73/X67</f>
+        <v>31.956738374301072</v>
+      </c>
+      <c r="Y77" s="40">
+        <f t="shared" si="107"/>
+        <v>18.433692956105823</v>
+      </c>
+      <c r="AG77" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH77" s="40">
+        <f>AH73/AH67</f>
+        <v>39.231439434218089</v>
+      </c>
+    </row>
+    <row r="78" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="79" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="V78" s="40">
+        <f t="shared" ref="V78:X78" si="108">V74/SUM(S6:V6)</f>
+        <v>29.93324409694867</v>
+      </c>
+      <c r="W78" s="40">
+        <f t="shared" si="108"/>
+        <v>24.582176571414543</v>
+      </c>
+      <c r="X78" s="40">
+        <f t="shared" si="108"/>
+        <v>19.725254796867233</v>
+      </c>
+      <c r="Y78" s="40">
+        <f>Y74/SUM(V6:Y6)</f>
+        <v>10.606803677858297</v>
+      </c>
+      <c r="AG78" s="40">
+        <f t="shared" ref="AG78:AH78" si="109">AG74/AG6</f>
+        <v>36.927571198956599</v>
+      </c>
+      <c r="AH78" s="40">
+        <f>AH74/AH6</f>
+        <v>29.93324409694867</v>
+      </c>
+    </row>
+    <row r="79" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="80" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="V79" s="40">
+        <f t="shared" ref="V79:X79" si="110">V75/SUM(S6:V6)</f>
+        <v>29.144257828062376</v>
+      </c>
+      <c r="W79" s="40">
+        <f t="shared" si="110"/>
+        <v>23.874988113373725</v>
+      </c>
+      <c r="X79" s="40">
+        <f t="shared" si="110"/>
+        <v>19.117942423773247</v>
+      </c>
+      <c r="Y79" s="40">
+        <f>Y75/SUM(V6:Y6)</f>
+        <v>10.061497586985441</v>
+      </c>
+      <c r="AG79" s="40">
+        <f t="shared" ref="AG79:AH79" si="111">AG75/AG6</f>
+        <v>36.893672692909654</v>
+      </c>
+      <c r="AH79" s="40">
+        <f>AH75/AH6</f>
+        <v>29.144257828062376</v>
+      </c>
+    </row>
+    <row r="80" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="V80" s="40">
+        <f t="shared" ref="V80" si="112">V73/SUM(S22:V22)</f>
+        <v>-84.508678490299772</v>
+      </c>
+      <c r="W80" s="40">
+        <f t="shared" ref="W80:X80" si="113">W73/SUM(T22:W22)</f>
+        <v>-72.546524492411535</v>
+      </c>
+      <c r="X80" s="40">
+        <f t="shared" si="113"/>
+        <v>-57.695906234315359</v>
+      </c>
+      <c r="Y80" s="40">
+        <f>Y73/SUM(V22:Y22)</f>
+        <v>-33.274743486600045</v>
+      </c>
+      <c r="AG80" s="40">
+        <f t="shared" ref="AG80:AH80" si="114">AG73/AG22</f>
+        <v>-81.669936332863827</v>
+      </c>
+      <c r="AH80" s="40">
+        <f>AH73/AH22</f>
+        <v>-85.233065551478504</v>
+      </c>
+    </row>
+    <row r="81" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B81" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="V81" s="40"/>
+      <c r="W81" s="40"/>
+      <c r="X81" s="40"/>
+      <c r="Y81" s="40"/>
+    </row>
+    <row r="82" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B82" s="1" t="s">
         <v>129</v>
       </c>
@@ -4070,13 +5429,15 @@
   <hyperlinks>
     <hyperlink ref="W1" r:id="rId1" location="i38c3139dc7914f5e8533d7dcbc3a2a96_13" xr:uid="{E49C4A64-2AFD-4765-8FED-15375274F6C1}"/>
     <hyperlink ref="X1" r:id="rId2" xr:uid="{4E7150A9-F871-4F8F-9349-317999221213}"/>
+    <hyperlink ref="Y1" r:id="rId3" xr:uid="{ECCBBB48-7DF4-4D89-B9C2-0F98891117F1}"/>
+    <hyperlink ref="AH1" r:id="rId4" xr:uid="{AD1CDE78-BFA1-4502-94FA-12E996AA6832}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
   <ignoredErrors>
-    <ignoredError sqref="AF4:AH4 AF5:AH5" formulaRange="1"/>
-    <ignoredError sqref="AH42 AH55" formula="1"/>
+    <ignoredError sqref="AF4 AF5" formulaRange="1"/>
+    <ignoredError sqref="AH42 AH55 V6:V23 R6 R19 AI10 AI19:AI21" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
$MDB Rudimentary forecast & NPV share price
</commit_message>
<xml_diff>
--- a/$MDB.xlsx
+++ b/$MDB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881CA092-3D1B-44CC-9F4B-9CA56FC00DDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BA0976-7974-422D-9C8D-4208AACC72E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27435" windowHeight="11100" activeTab="1" xr2:uid="{A0DE9234-8F94-41AD-8663-2284C148F328}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="152">
   <si>
     <t>$MDB</t>
   </si>
@@ -461,6 +461,27 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>Maturity Rate</t>
+  </si>
+  <si>
+    <t>Discount Rate</t>
+  </si>
+  <si>
+    <t>NPV</t>
+  </si>
+  <si>
+    <t>Total Value</t>
+  </si>
+  <si>
+    <t>Per Share</t>
+  </si>
+  <si>
+    <t>Current Share Price</t>
+  </si>
+  <si>
+    <t>Upside</t>
   </si>
 </sst>
 </file>
@@ -686,7 +707,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -771,36 +792,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -828,12 +819,52 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1349,35 +1380,35 @@
       <c r="G3"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
-      <c r="G5" s="51" t="s">
+      <c r="C5" s="64"/>
+      <c r="D5" s="65"/>
+      <c r="G5" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
-      <c r="T5" s="46" t="s">
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="65"/>
+      <c r="T5" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="46"/>
-      <c r="Z5" s="46" t="s">
+      <c r="U5" s="68"/>
+      <c r="V5" s="68"/>
+      <c r="W5" s="68"/>
+      <c r="Z5" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="AA5" s="46"/>
-      <c r="AB5" s="46"/>
+      <c r="AA5" s="68"/>
+      <c r="AB5" s="68"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -1647,11 +1678,11 @@
       <c r="AB14" s="6"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="65"/>
       <c r="G15" s="14"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
@@ -1676,10 +1707,10 @@
       <c r="B16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="48"/>
+      <c r="D16" s="62"/>
       <c r="G16" s="14"/>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
@@ -1706,10 +1737,10 @@
       <c r="B17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="48"/>
+      <c r="D17" s="62"/>
       <c r="G17" s="14"/>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
@@ -1734,10 +1765,10 @@
       <c r="B18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="48"/>
+      <c r="D18" s="62"/>
       <c r="G18" s="14"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
@@ -1757,10 +1788,10 @@
       <c r="B19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="55"/>
+      <c r="D19" s="72"/>
       <c r="G19" s="14"/>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
@@ -1803,11 +1834,11 @@
       <c r="Q21" s="17"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="53"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="65"/>
       <c r="G22" s="14"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
@@ -1824,10 +1855,10 @@
       <c r="B23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="D23" s="48"/>
+      <c r="D23" s="62"/>
       <c r="G23" s="14"/>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
@@ -1844,10 +1875,10 @@
       <c r="B24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="47">
+      <c r="C24" s="61">
         <v>2007</v>
       </c>
-      <c r="D24" s="48"/>
+      <c r="D24" s="62"/>
       <c r="G24" s="14"/>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
@@ -1864,10 +1895,10 @@
       <c r="B25" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="47">
+      <c r="C25" s="61">
         <v>2017</v>
       </c>
-      <c r="D25" s="48"/>
+      <c r="D25" s="62"/>
       <c r="G25" s="14"/>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
@@ -1882,8 +1913,8 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B26" s="14"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="48"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
       <c r="G26" s="14"/>
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
@@ -1898,8 +1929,8 @@
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B27" s="14"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="48"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="62"/>
       <c r="G27" s="14"/>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
@@ -1938,10 +1969,10 @@
       <c r="B29" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="D29" s="50"/>
+      <c r="D29" s="70"/>
       <c r="G29" s="14"/>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
@@ -1981,11 +2012,11 @@
       <c r="Q31" s="17"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="53"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="65"/>
       <c r="G32" s="14"/>
       <c r="H32" s="16"/>
       <c r="I32" s="16"/>
@@ -2002,11 +2033,11 @@
       <c r="B33" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="71">
+      <c r="C33" s="66">
         <f>C6/'Financial Model'!Y67</f>
         <v>19.311919490429393</v>
       </c>
-      <c r="D33" s="72"/>
+      <c r="D33" s="67"/>
       <c r="G33" s="14"/>
       <c r="H33" s="16"/>
       <c r="I33" s="16"/>
@@ -2023,11 +2054,11 @@
       <c r="B34" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="71">
+      <c r="C34" s="66">
         <f>C8/SUM('Financial Model'!V6:Y6)</f>
         <v>11.112137929461445</v>
       </c>
-      <c r="D34" s="72"/>
+      <c r="D34" s="67"/>
       <c r="G34" s="14"/>
       <c r="H34" s="16"/>
       <c r="I34" s="16"/>
@@ -2044,8 +2075,8 @@
       <c r="B35" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="48"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="62"/>
       <c r="G35" s="14"/>
       <c r="H35" s="16"/>
       <c r="I35" s="16"/>
@@ -2062,8 +2093,8 @@
       <c r="B36" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="48"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="62"/>
       <c r="G36" s="14">
         <v>2013</v>
       </c>
@@ -2084,8 +2115,8 @@
       <c r="B37" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="47"/>
-      <c r="D37" s="48"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="62"/>
       <c r="G37" s="14"/>
       <c r="H37" s="27" t="s">
         <v>74</v>
@@ -2102,8 +2133,8 @@
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B38" s="14"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="48"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="62"/>
       <c r="G38" s="15"/>
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
@@ -2118,6 +2149,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="Z5:AB5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
@@ -2130,17 +2172,6 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="Z5:AB5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" location="views-exposed-form-widget-sec-filings-table" display="Link" xr:uid="{8C8DCE07-3950-4AA9-A781-B1A96427FDBB}"/>
@@ -2153,13 +2184,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509F8013-A317-41E1-99F6-617E09116884}">
-  <dimension ref="B1:AR82"/>
+  <dimension ref="B1:CV82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AB4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AJ11" sqref="AJ11:AJ13"/>
+      <selection pane="bottomRight" activeCell="AS26" sqref="AS26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2167,10 +2198,12 @@
     <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="25" width="9.140625" style="1"/>
-    <col min="26" max="26" width="9.140625" style="59"/>
+    <col min="26" max="26" width="9.140625" style="49"/>
     <col min="27" max="34" width="9.140625" style="1"/>
-    <col min="35" max="35" width="9.140625" style="64"/>
-    <col min="36" max="16384" width="9.140625" style="1"/>
+    <col min="35" max="35" width="9.140625" style="54"/>
+    <col min="36" max="45" width="9.140625" style="1"/>
+    <col min="46" max="46" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:44" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -2243,7 +2276,7 @@
       <c r="Y1" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="Z1" s="61" t="s">
+      <c r="Z1" s="51" t="s">
         <v>90</v>
       </c>
       <c r="AD1" s="23" t="s">
@@ -2261,7 +2294,7 @@
       <c r="AH1" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="AI1" s="68" t="s">
+      <c r="AI1" s="58" t="s">
         <v>61</v>
       </c>
       <c r="AJ1" s="23" t="s">
@@ -2318,7 +2351,7 @@
       <c r="Y2" s="28">
         <v>44865</v>
       </c>
-      <c r="Z2" s="60" t="s">
+      <c r="Z2" s="50" t="s">
         <v>143</v>
       </c>
       <c r="AG2" s="28">
@@ -2327,17 +2360,17 @@
       <c r="AH2" s="28">
         <v>44592</v>
       </c>
-      <c r="AI2" s="69" t="s">
+      <c r="AI2" s="59" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="2:44" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="25"/>
-      <c r="Z3" s="60"/>
-      <c r="AH3" s="56">
+      <c r="Z3" s="50"/>
+      <c r="AH3" s="46">
         <v>44638</v>
       </c>
-      <c r="AI3" s="69"/>
+      <c r="AI3" s="59"/>
     </row>
     <row r="4" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
@@ -2369,7 +2402,7 @@
       <c r="Y4" s="34">
         <v>320.75599999999997</v>
       </c>
-      <c r="Z4" s="59"/>
+      <c r="Z4" s="49"/>
       <c r="AF4" s="38">
         <f>SUM(K4:N4)</f>
         <v>0</v>
@@ -2380,7 +2413,7 @@
       <c r="AH4" s="34">
         <v>842.04700000000003</v>
       </c>
-      <c r="AI4" s="64"/>
+      <c r="AI4" s="54"/>
     </row>
     <row r="5" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="29" t="s">
@@ -2412,7 +2445,7 @@
       <c r="Y5" s="34">
         <v>12.865</v>
       </c>
-      <c r="Z5" s="59"/>
+      <c r="Z5" s="49"/>
       <c r="AF5" s="38">
         <f>SUM(K5:N5)</f>
         <v>0</v>
@@ -2423,45 +2456,45 @@
       <c r="AH5" s="34">
         <v>31.734999999999999</v>
       </c>
-      <c r="AI5" s="64"/>
+      <c r="AI5" s="54"/>
     </row>
     <row r="6" spans="2:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>76</v>
       </c>
       <c r="R6" s="31">
-        <f>R4+R5</f>
+        <f t="shared" ref="R6:Y6" si="0">R4+R5</f>
         <v>590.38</v>
       </c>
       <c r="S6" s="31">
-        <f>S4+S5</f>
+        <f t="shared" si="0"/>
         <v>181.648</v>
       </c>
       <c r="T6" s="31">
-        <f>T4+T5</f>
+        <f t="shared" si="0"/>
         <v>198.74700000000001</v>
       </c>
       <c r="U6" s="31">
-        <f>U4+U5</f>
+        <f t="shared" si="0"/>
         <v>226.893</v>
       </c>
       <c r="V6" s="31">
-        <f>V4+V5</f>
+        <f t="shared" si="0"/>
         <v>266.49400000000003</v>
       </c>
       <c r="W6" s="31">
-        <f>W4+W5</f>
+        <f t="shared" si="0"/>
         <v>285.447</v>
       </c>
       <c r="X6" s="41">
-        <f>X4+X5</f>
+        <f t="shared" si="0"/>
         <v>303.66000000000003</v>
       </c>
       <c r="Y6" s="31">
-        <f>Y4+Y5</f>
+        <f t="shared" si="0"/>
         <v>333.62099999999998</v>
       </c>
-      <c r="Z6" s="62">
+      <c r="Z6" s="52">
         <f>Y6*(1+Z27)</f>
         <v>373.65552000000002</v>
       </c>
@@ -2477,45 +2510,45 @@
         <f>AH4+AH5</f>
         <v>873.78200000000004</v>
       </c>
-      <c r="AI6" s="62">
+      <c r="AI6" s="52">
         <f>SUM(W6:Z6)</f>
         <v>1296.3835199999999</v>
       </c>
       <c r="AJ6" s="31">
         <f>AI6*(1+AJ26)</f>
-        <v>1970.5029503999999</v>
+        <v>1944.5752799999998</v>
       </c>
       <c r="AK6" s="31">
-        <f t="shared" ref="AK6:AR6" si="0">AJ6*(1+AK26)</f>
-        <v>2916.3443665919999</v>
+        <f t="shared" ref="AK6:AR6" si="1">AJ6*(1+AK26)</f>
+        <v>2916.8629199999996</v>
       </c>
       <c r="AL6" s="31">
-        <f t="shared" si="0"/>
-        <v>3937.0648948992002</v>
+        <f t="shared" si="1"/>
+        <v>4083.608087999999</v>
       </c>
       <c r="AM6" s="31">
-        <f t="shared" si="0"/>
-        <v>4921.3311186240007</v>
+        <f t="shared" si="1"/>
+        <v>5308.6905143999993</v>
       </c>
       <c r="AN6" s="31">
-        <f t="shared" si="0"/>
-        <v>5905.5973423488003</v>
+        <f t="shared" si="1"/>
+        <v>6635.8631429999987</v>
       </c>
       <c r="AO6" s="31">
-        <f t="shared" si="0"/>
-        <v>6791.4369437011201</v>
+        <f t="shared" si="1"/>
+        <v>7963.035771599998</v>
       </c>
       <c r="AP6" s="31">
-        <f t="shared" si="0"/>
-        <v>7810.152485256287</v>
+        <f t="shared" si="1"/>
+        <v>9157.4911373399973</v>
       </c>
       <c r="AQ6" s="31">
-        <f t="shared" si="0"/>
-        <v>8981.6753580447294</v>
+        <f t="shared" si="1"/>
+        <v>10073.240251073998</v>
       </c>
       <c r="AR6" s="31">
-        <f t="shared" si="0"/>
-        <v>10328.926661751439</v>
+        <f t="shared" si="1"/>
+        <v>10576.902263627699</v>
       </c>
     </row>
     <row r="7" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
@@ -2523,7 +2556,7 @@
         <v>78</v>
       </c>
       <c r="R7" s="34">
-        <f t="shared" ref="R7:R8" si="1">AG7-SUM(O7:Q7)</f>
+        <f t="shared" ref="R7:R8" si="2">AG7-SUM(O7:Q7)</f>
         <v>145.28</v>
       </c>
       <c r="S7" s="38">
@@ -2536,7 +2569,7 @@
         <v>57.378</v>
       </c>
       <c r="V7" s="34">
-        <f t="shared" ref="V7:V8" si="2">AH7-SUM(S7:U7)</f>
+        <f t="shared" ref="V7:V8" si="3">AH7-SUM(S7:U7)</f>
         <v>64.165999999999997</v>
       </c>
       <c r="W7" s="38">
@@ -2548,21 +2581,21 @@
       <c r="Y7" s="34">
         <v>77.150000000000006</v>
       </c>
-      <c r="Z7" s="63"/>
+      <c r="Z7" s="53"/>
       <c r="AG7" s="38">
         <v>145.28</v>
       </c>
       <c r="AH7" s="38">
         <v>217.90100000000001</v>
       </c>
-      <c r="AI7" s="64"/>
+      <c r="AI7" s="54"/>
     </row>
     <row r="8" spans="2:44" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="29" t="s">
         <v>79</v>
       </c>
       <c r="R8" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31.795999999999999</v>
       </c>
       <c r="S8" s="38">
@@ -2575,7 +2608,7 @@
         <v>11.086</v>
       </c>
       <c r="V8" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.632000000000005</v>
       </c>
       <c r="W8" s="38">
@@ -2587,21 +2620,21 @@
       <c r="Y8" s="34">
         <v>16.501999999999999</v>
       </c>
-      <c r="Z8" s="59"/>
+      <c r="Z8" s="49"/>
       <c r="AG8" s="38">
         <v>31.795999999999999</v>
       </c>
       <c r="AH8" s="38">
         <v>41.591000000000001</v>
       </c>
-      <c r="AI8" s="64"/>
+      <c r="AI8" s="54"/>
     </row>
     <row r="9" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>77</v>
       </c>
       <c r="R9" s="30">
-        <f t="shared" ref="R9" si="3">R7+R8</f>
+        <f t="shared" ref="R9" si="4">R7+R8</f>
         <v>177.07599999999999</v>
       </c>
       <c r="S9" s="1">
@@ -2609,11 +2642,11 @@
         <v>54.527999999999999</v>
       </c>
       <c r="T9" s="1">
-        <f t="shared" ref="T9:U9" si="4">T7+T8</f>
+        <f t="shared" ref="T9:U9" si="5">T7+T8</f>
         <v>60.701999999999998</v>
       </c>
       <c r="U9" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>68.463999999999999</v>
       </c>
       <c r="V9" s="1">
@@ -2625,64 +2658,64 @@
         <v>78.215000000000003</v>
       </c>
       <c r="X9" s="39">
-        <f t="shared" ref="X9:Y9" si="5">X7+X8</f>
+        <f t="shared" ref="X9:Y9" si="6">X7+X8</f>
         <v>88.277000000000001</v>
       </c>
       <c r="Y9" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>93.652000000000001</v>
       </c>
-      <c r="Z9" s="67">
+      <c r="Z9" s="57">
         <f>Z6*(1-Z29)</f>
         <v>104.62354560000001</v>
       </c>
       <c r="AG9" s="30">
-        <f t="shared" ref="AG9:AH9" si="6">AG7+AG8</f>
+        <f t="shared" ref="AG9:AH9" si="7">AG7+AG8</f>
         <v>177.07599999999999</v>
       </c>
       <c r="AH9" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>259.49200000000002</v>
       </c>
-      <c r="AI9" s="64">
+      <c r="AI9" s="54">
         <f>SUM(W9:Z9)</f>
         <v>364.76754560000001</v>
       </c>
       <c r="AJ9" s="30">
         <f>AJ6*(1-AJ29)</f>
-        <v>551.74082611200004</v>
+        <v>544.4810784</v>
       </c>
       <c r="AK9" s="30">
-        <f t="shared" ref="AK9:AR9" si="7">AK6*(1-AK29)</f>
-        <v>816.57642264576009</v>
+        <f t="shared" ref="AK9:AR9" si="8">AK6*(1-AK29)</f>
+        <v>816.72161759999995</v>
       </c>
       <c r="AL9" s="30">
-        <f t="shared" si="7"/>
-        <v>1102.3781705717761</v>
+        <f t="shared" si="8"/>
+        <v>1143.4102646399999</v>
       </c>
       <c r="AM9" s="30">
-        <f t="shared" si="7"/>
-        <v>1377.9727132147204</v>
+        <f t="shared" si="8"/>
+        <v>1486.4333440319999</v>
       </c>
       <c r="AN9" s="30">
-        <f t="shared" si="7"/>
-        <v>1653.5672558576643</v>
+        <f t="shared" si="8"/>
+        <v>1858.0416800399998</v>
       </c>
       <c r="AO9" s="30">
-        <f t="shared" si="7"/>
-        <v>1901.6023442363139</v>
+        <f t="shared" si="8"/>
+        <v>2229.6500160479995</v>
       </c>
       <c r="AP9" s="30">
-        <f t="shared" si="7"/>
-        <v>2186.8426958717605</v>
+        <f t="shared" si="8"/>
+        <v>2564.0975184551994</v>
       </c>
       <c r="AQ9" s="30">
-        <f t="shared" si="7"/>
-        <v>2514.8691002525243</v>
+        <f t="shared" si="8"/>
+        <v>2820.5072703007195</v>
       </c>
       <c r="AR9" s="30">
-        <f t="shared" si="7"/>
-        <v>2892.0994652904033</v>
+        <f t="shared" si="8"/>
+        <v>2961.5326338157561</v>
       </c>
     </row>
     <row r="10" spans="2:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2690,7 +2723,7 @@
         <v>82</v>
       </c>
       <c r="R10" s="31">
-        <f t="shared" ref="R10" si="8">R6-R9</f>
+        <f t="shared" ref="R10" si="9">R6-R9</f>
         <v>413.30399999999997</v>
       </c>
       <c r="S10" s="31">
@@ -2698,11 +2731,11 @@
         <v>127.12</v>
       </c>
       <c r="T10" s="31">
-        <f t="shared" ref="T10:U10" si="9">T6-T9</f>
+        <f t="shared" ref="T10:U10" si="10">T6-T9</f>
         <v>138.04500000000002</v>
       </c>
       <c r="U10" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>158.429</v>
       </c>
       <c r="V10" s="31">
@@ -2714,64 +2747,64 @@
         <v>207.232</v>
       </c>
       <c r="X10" s="41">
-        <f t="shared" ref="X10:Y10" si="10">X6-X9</f>
+        <f t="shared" ref="X10:Y10" si="11">X6-X9</f>
         <v>215.38300000000004</v>
       </c>
       <c r="Y10" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>239.96899999999999</v>
       </c>
-      <c r="Z10" s="62">
+      <c r="Z10" s="52">
         <f>Z6-Z9</f>
         <v>269.03197440000002</v>
       </c>
       <c r="AG10" s="31">
-        <f t="shared" ref="AG10:AH10" si="11">AG6-AG9</f>
+        <f t="shared" ref="AG10:AH10" si="12">AG6-AG9</f>
         <v>413.30399999999997</v>
       </c>
       <c r="AH10" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>614.29</v>
       </c>
-      <c r="AI10" s="62">
+      <c r="AI10" s="52">
         <f>AI6-AI9</f>
         <v>931.61597439999991</v>
       </c>
       <c r="AJ10" s="31">
         <f>AJ6-AJ9</f>
-        <v>1418.762124288</v>
+        <v>1400.0942015999999</v>
       </c>
       <c r="AK10" s="31">
-        <f t="shared" ref="AK10:AR10" si="12">AK6-AK9</f>
-        <v>2099.7679439462399</v>
+        <f t="shared" ref="AK10:AR10" si="13">AK6-AK9</f>
+        <v>2100.1413023999994</v>
       </c>
       <c r="AL10" s="31">
-        <f t="shared" si="12"/>
-        <v>2834.6867243274241</v>
+        <f t="shared" si="13"/>
+        <v>2940.1978233599993</v>
       </c>
       <c r="AM10" s="31">
-        <f t="shared" si="12"/>
-        <v>3543.3584054092803</v>
+        <f t="shared" si="13"/>
+        <v>3822.2571703679996</v>
       </c>
       <c r="AN10" s="31">
-        <f t="shared" si="12"/>
-        <v>4252.030086491136</v>
+        <f t="shared" si="13"/>
+        <v>4777.8214629599988</v>
       </c>
       <c r="AO10" s="31">
-        <f t="shared" si="12"/>
-        <v>4889.8345994648062</v>
+        <f t="shared" si="13"/>
+        <v>5733.385755551999</v>
       </c>
       <c r="AP10" s="31">
-        <f t="shared" si="12"/>
-        <v>5623.3097893845261</v>
+        <f t="shared" si="13"/>
+        <v>6593.3936188847983</v>
       </c>
       <c r="AQ10" s="31">
-        <f t="shared" si="12"/>
-        <v>6466.8062577922046</v>
+        <f t="shared" si="13"/>
+        <v>7252.7329807732785</v>
       </c>
       <c r="AR10" s="31">
-        <f t="shared" si="12"/>
-        <v>7436.8271964610358</v>
+        <f t="shared" si="13"/>
+        <v>7615.369629811943</v>
       </c>
     </row>
     <row r="11" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
@@ -2779,7 +2812,7 @@
         <v>91</v>
       </c>
       <c r="R11" s="30">
-        <f t="shared" ref="R11:R13" si="13">AG11-SUM(O11:Q11)</f>
+        <f t="shared" ref="R11:R13" si="14">AG11-SUM(O11:Q11)</f>
         <v>325.10000000000002</v>
       </c>
       <c r="S11" s="30">
@@ -2804,7 +2837,7 @@
       <c r="Y11" s="30">
         <v>177.41900000000001</v>
       </c>
-      <c r="Z11" s="64">
+      <c r="Z11" s="54">
         <f>Z6*0.53</f>
         <v>198.03742560000003</v>
       </c>
@@ -2818,9 +2851,45 @@
       <c r="AH11" s="30">
         <v>471.89</v>
       </c>
-      <c r="AI11" s="64">
-        <f t="shared" ref="AI11:AI13" si="14">SUM(W11:Z11)</f>
+      <c r="AI11" s="54">
+        <f t="shared" ref="AI11:AI13" si="15">SUM(W11:Z11)</f>
         <v>707.32242559999997</v>
+      </c>
+      <c r="AJ11" s="30">
+        <f>AJ6*0.5</f>
+        <v>972.2876399999999</v>
+      </c>
+      <c r="AK11" s="30">
+        <f>AK6*0.45</f>
+        <v>1312.5883139999999</v>
+      </c>
+      <c r="AL11" s="30">
+        <f t="shared" ref="AL11:AR11" si="16">AL6*0.45</f>
+        <v>1837.6236395999997</v>
+      </c>
+      <c r="AM11" s="30">
+        <f t="shared" si="16"/>
+        <v>2388.9107314799999</v>
+      </c>
+      <c r="AN11" s="30">
+        <f>AN6*0.35</f>
+        <v>2322.5521000499994</v>
+      </c>
+      <c r="AO11" s="30">
+        <f t="shared" ref="AO11:AR11" si="17">AO6*0.35</f>
+        <v>2787.0625200599993</v>
+      </c>
+      <c r="AP11" s="30">
+        <f t="shared" si="17"/>
+        <v>3205.1218980689987</v>
+      </c>
+      <c r="AQ11" s="30">
+        <f t="shared" si="17"/>
+        <v>3525.6340878758988</v>
+      </c>
+      <c r="AR11" s="30">
+        <f t="shared" si="17"/>
+        <v>3701.9157922696941</v>
       </c>
     </row>
     <row r="12" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
@@ -2828,7 +2897,7 @@
         <v>92</v>
       </c>
       <c r="R12" s="30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>205.161</v>
       </c>
       <c r="S12" s="30">
@@ -2841,7 +2910,7 @@
         <v>82.256</v>
       </c>
       <c r="V12" s="30">
-        <f t="shared" ref="V12:V13" si="15">AH12-SUM(S12:U12)</f>
+        <f t="shared" ref="V12:V13" si="18">AH12-SUM(S12:U12)</f>
         <v>89.417000000000002</v>
       </c>
       <c r="W12" s="30">
@@ -2853,7 +2922,7 @@
       <c r="Y12" s="30">
         <v>106.392</v>
       </c>
-      <c r="Z12" s="64">
+      <c r="Z12" s="54">
         <f>Z6*0.31</f>
         <v>115.83321120000001</v>
       </c>
@@ -2867,9 +2936,45 @@
       <c r="AH12" s="30">
         <v>308.82</v>
       </c>
-      <c r="AI12" s="64">
-        <f t="shared" si="14"/>
+      <c r="AI12" s="54">
+        <f t="shared" si="15"/>
         <v>426.63421119999998</v>
+      </c>
+      <c r="AJ12" s="30">
+        <f>AJ6*0.28</f>
+        <v>544.4810784</v>
+      </c>
+      <c r="AK12" s="30">
+        <f>AK6*0.26</f>
+        <v>758.38435919999995</v>
+      </c>
+      <c r="AL12" s="30">
+        <f>AL6*0.2</f>
+        <v>816.72161759999983</v>
+      </c>
+      <c r="AM12" s="30">
+        <f>AM6*0.18</f>
+        <v>955.56429259199979</v>
+      </c>
+      <c r="AN12" s="30">
+        <f>AN6*0.15</f>
+        <v>995.37947144999976</v>
+      </c>
+      <c r="AO12" s="30">
+        <f>AO6*0.1</f>
+        <v>796.3035771599998</v>
+      </c>
+      <c r="AP12" s="30">
+        <f>AP6*0.05</f>
+        <v>457.87455686699991</v>
+      </c>
+      <c r="AQ12" s="30">
+        <f t="shared" ref="AQ12:AR12" si="19">AQ6*0.05</f>
+        <v>503.66201255369992</v>
+      </c>
+      <c r="AR12" s="30">
+        <f t="shared" si="19"/>
+        <v>528.84511318138493</v>
       </c>
     </row>
     <row r="13" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
@@ -2877,7 +2982,7 @@
         <v>93</v>
       </c>
       <c r="R13" s="30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>92.346999999999994</v>
       </c>
       <c r="S13" s="30">
@@ -2890,7 +2995,7 @@
         <v>32.581000000000003</v>
       </c>
       <c r="V13" s="30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>35.635000000000005</v>
       </c>
       <c r="W13" s="30">
@@ -2902,7 +3007,7 @@
       <c r="Y13" s="30">
         <v>39.081000000000003</v>
       </c>
-      <c r="Z13" s="64">
+      <c r="Z13" s="54">
         <f>Z6*0.12</f>
         <v>44.838662400000004</v>
       </c>
@@ -2916,9 +3021,45 @@
       <c r="AH13" s="30">
         <v>122.944</v>
       </c>
-      <c r="AI13" s="64">
-        <f t="shared" si="14"/>
+      <c r="AI13" s="54">
+        <f t="shared" si="15"/>
         <v>161.04266239999998</v>
+      </c>
+      <c r="AJ13" s="30">
+        <f>AJ6*0.1</f>
+        <v>194.457528</v>
+      </c>
+      <c r="AK13" s="30">
+        <f t="shared" ref="AK13:AR13" si="20">AK6*0.1</f>
+        <v>291.68629199999998</v>
+      </c>
+      <c r="AL13" s="30">
+        <f t="shared" si="20"/>
+        <v>408.36080879999992</v>
+      </c>
+      <c r="AM13" s="30">
+        <f t="shared" si="20"/>
+        <v>530.86905143999991</v>
+      </c>
+      <c r="AN13" s="30">
+        <f t="shared" si="20"/>
+        <v>663.58631429999991</v>
+      </c>
+      <c r="AO13" s="30">
+        <f t="shared" si="20"/>
+        <v>796.3035771599998</v>
+      </c>
+      <c r="AP13" s="30">
+        <f t="shared" si="20"/>
+        <v>915.74911373399982</v>
+      </c>
+      <c r="AQ13" s="30">
+        <f t="shared" si="20"/>
+        <v>1007.3240251073998</v>
+      </c>
+      <c r="AR13" s="30">
+        <f t="shared" si="20"/>
+        <v>1057.6902263627699</v>
       </c>
     </row>
     <row r="14" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
@@ -2926,7 +3067,7 @@
         <v>94</v>
       </c>
       <c r="R14" s="30">
-        <f t="shared" ref="R14" si="16">R11+R12+R13</f>
+        <f t="shared" ref="R14" si="21">R11+R12+R13</f>
         <v>622.60799999999995</v>
       </c>
       <c r="S14" s="30">
@@ -2934,15 +3075,15 @@
         <v>188.56600000000003</v>
       </c>
       <c r="T14" s="30">
-        <f t="shared" ref="T14:U14" si="17">T11+T12+T13</f>
+        <f t="shared" ref="T14:U14" si="22">T11+T12+T13</f>
         <v>210.57599999999999</v>
       </c>
       <c r="U14" s="30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>235.197</v>
       </c>
       <c r="V14" s="30">
-        <f t="shared" ref="V14" si="18">V11+V12+V13</f>
+        <f t="shared" ref="V14" si="23">V11+V12+V13</f>
         <v>269.315</v>
       </c>
       <c r="W14" s="30">
@@ -2954,24 +3095,60 @@
         <v>330.226</v>
       </c>
       <c r="Y14" s="30">
-        <f t="shared" ref="Y14:Z14" si="19">Y11+Y12+Y13</f>
+        <f t="shared" ref="Y14:Z14" si="24">Y11+Y12+Y13</f>
         <v>322.89200000000005</v>
       </c>
-      <c r="Z14" s="64">
-        <f t="shared" si="19"/>
+      <c r="Z14" s="54">
+        <f t="shared" si="24"/>
         <v>358.70929920000003</v>
       </c>
       <c r="AG14" s="30">
-        <f t="shared" ref="AG14" si="20">AG11+AG12+AG13</f>
+        <f t="shared" ref="AG14" si="25">AG11+AG12+AG13</f>
         <v>622.60799999999995</v>
       </c>
       <c r="AH14" s="30">
-        <f t="shared" ref="AH14:AJ14" si="21">AH11+AH12+AH13</f>
+        <f t="shared" ref="AH14:AR14" si="26">AH11+AH12+AH13</f>
         <v>903.654</v>
       </c>
-      <c r="AI14" s="64">
-        <f t="shared" si="21"/>
+      <c r="AI14" s="54">
+        <f t="shared" si="26"/>
         <v>1294.9992992</v>
+      </c>
+      <c r="AJ14" s="30">
+        <f t="shared" si="26"/>
+        <v>1711.2262463999998</v>
+      </c>
+      <c r="AK14" s="30">
+        <f t="shared" si="26"/>
+        <v>2362.6589651999998</v>
+      </c>
+      <c r="AL14" s="30">
+        <f t="shared" si="26"/>
+        <v>3062.7060659999997</v>
+      </c>
+      <c r="AM14" s="30">
+        <f t="shared" si="26"/>
+        <v>3875.3440755119996</v>
+      </c>
+      <c r="AN14" s="30">
+        <f t="shared" si="26"/>
+        <v>3981.517885799999</v>
+      </c>
+      <c r="AO14" s="30">
+        <f t="shared" si="26"/>
+        <v>4379.6696743799985</v>
+      </c>
+      <c r="AP14" s="30">
+        <f t="shared" si="26"/>
+        <v>4578.7455686699977</v>
+      </c>
+      <c r="AQ14" s="30">
+        <f t="shared" si="26"/>
+        <v>5036.6201255369979</v>
+      </c>
+      <c r="AR14" s="30">
+        <f t="shared" si="26"/>
+        <v>5288.4511318138493</v>
       </c>
     </row>
     <row r="15" spans="2:44" s="31" customFormat="1" x14ac:dyDescent="0.2">
@@ -2979,7 +3156,7 @@
         <v>95</v>
       </c>
       <c r="R15" s="31">
-        <f t="shared" ref="R15" si="22">R10-R14</f>
+        <f t="shared" ref="R15" si="27">R10-R14</f>
         <v>-209.30399999999997</v>
       </c>
       <c r="S15" s="31">
@@ -2987,15 +3164,15 @@
         <v>-61.446000000000026</v>
       </c>
       <c r="T15" s="31">
-        <f t="shared" ref="T15:U15" si="23">T10-T14</f>
+        <f t="shared" ref="T15:U15" si="28">T10-T14</f>
         <v>-72.530999999999977</v>
       </c>
       <c r="U15" s="31">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-76.768000000000001</v>
       </c>
       <c r="V15" s="31">
-        <f t="shared" ref="V15" si="24">V10-V14</f>
+        <f t="shared" ref="V15" si="29">V10-V14</f>
         <v>-78.618999999999971</v>
       </c>
       <c r="W15" s="31">
@@ -3007,24 +3184,60 @@
         <v>-114.84299999999996</v>
       </c>
       <c r="Y15" s="31">
-        <f t="shared" ref="Y15:Z15" si="25">Y10-Y14</f>
+        <f t="shared" ref="Y15:Z15" si="30">Y10-Y14</f>
         <v>-82.923000000000059</v>
       </c>
-      <c r="Z15" s="62">
-        <f t="shared" si="25"/>
+      <c r="Z15" s="52">
+        <f t="shared" si="30"/>
         <v>-89.677324800000008</v>
       </c>
       <c r="AG15" s="31">
-        <f t="shared" ref="AG15" si="26">AG10-AG14</f>
+        <f t="shared" ref="AG15" si="31">AG10-AG14</f>
         <v>-209.30399999999997</v>
       </c>
       <c r="AH15" s="31">
-        <f t="shared" ref="AH15:AJ15" si="27">AH10-AH14</f>
+        <f t="shared" ref="AH15:AR15" si="32">AH10-AH14</f>
         <v>-289.36400000000003</v>
       </c>
-      <c r="AI15" s="62">
-        <f t="shared" si="27"/>
+      <c r="AI15" s="52">
+        <f t="shared" si="32"/>
         <v>-363.38332480000008</v>
+      </c>
+      <c r="AJ15" s="31">
+        <f t="shared" si="32"/>
+        <v>-311.1320447999999</v>
+      </c>
+      <c r="AK15" s="31">
+        <f t="shared" si="32"/>
+        <v>-262.51766280000038</v>
+      </c>
+      <c r="AL15" s="31">
+        <f t="shared" si="32"/>
+        <v>-122.50824264000039</v>
+      </c>
+      <c r="AM15" s="31">
+        <f t="shared" si="32"/>
+        <v>-53.086905143999957</v>
+      </c>
+      <c r="AN15" s="31">
+        <f t="shared" si="32"/>
+        <v>796.3035771599998</v>
+      </c>
+      <c r="AO15" s="31">
+        <f t="shared" si="32"/>
+        <v>1353.7160811720005</v>
+      </c>
+      <c r="AP15" s="31">
+        <f t="shared" si="32"/>
+        <v>2014.6480502148006</v>
+      </c>
+      <c r="AQ15" s="31">
+        <f t="shared" si="32"/>
+        <v>2216.1128552362807</v>
+      </c>
+      <c r="AR15" s="31">
+        <f t="shared" si="32"/>
+        <v>2326.9184979980937</v>
       </c>
     </row>
     <row r="16" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
@@ -3032,7 +3245,7 @@
         <v>96</v>
       </c>
       <c r="R16" s="30">
-        <f t="shared" ref="R16:R18" si="28">AG16-SUM(O16:Q16)</f>
+        <f t="shared" ref="R16:R18" si="33">AG16-SUM(O16:Q16)</f>
         <v>4.569</v>
       </c>
       <c r="S16" s="30">
@@ -3045,7 +3258,7 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="V16" s="30">
-        <f t="shared" ref="V16:V20" si="29">AH16-SUM(S16:U16)</f>
+        <f t="shared" ref="V16:V20" si="34">AH16-SUM(S16:U16)</f>
         <v>0.39200000000000013</v>
       </c>
       <c r="W16" s="30">
@@ -3057,7 +3270,7 @@
       <c r="Y16" s="30">
         <v>6.9320000000000004</v>
       </c>
-      <c r="Z16" s="64">
+      <c r="Z16" s="54">
         <f>AVERAGE(V16:Y16)</f>
         <v>2.407</v>
       </c>
@@ -3068,17 +3281,53 @@
       <c r="AH16" s="30">
         <v>0.92600000000000005</v>
       </c>
-      <c r="AI16" s="64">
-        <f t="shared" ref="AI16:AI20" si="30">SUM(W16:Z16)</f>
+      <c r="AI16" s="54">
+        <f t="shared" ref="AI16:AI20" si="35">SUM(W16:Z16)</f>
         <v>11.643000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ16" s="30">
+        <f>AVERAGE(AG16:AI16)</f>
+        <v>5.7126666666666672</v>
+      </c>
+      <c r="AK16" s="30">
+        <f t="shared" ref="AK16:AR16" si="36">AVERAGE(AH16:AJ16)</f>
+        <v>6.0938888888888885</v>
+      </c>
+      <c r="AL16" s="30">
+        <f t="shared" si="36"/>
+        <v>7.8165185185185182</v>
+      </c>
+      <c r="AM16" s="30">
+        <f t="shared" si="36"/>
+        <v>6.5410246913580243</v>
+      </c>
+      <c r="AN16" s="30">
+        <f t="shared" si="36"/>
+        <v>6.81714403292181</v>
+      </c>
+      <c r="AO16" s="30">
+        <f t="shared" si="36"/>
+        <v>7.0582290809327839</v>
+      </c>
+      <c r="AP16" s="30">
+        <f t="shared" si="36"/>
+        <v>6.8054659350708731</v>
+      </c>
+      <c r="AQ16" s="30">
+        <f t="shared" si="36"/>
+        <v>6.893613016308489</v>
+      </c>
+      <c r="AR16" s="30">
+        <f t="shared" si="36"/>
+        <v>6.9191026774373823</v>
+      </c>
+    </row>
+    <row r="17" spans="2:100" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="30" t="s">
         <v>97</v>
       </c>
       <c r="R17" s="30">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>56.106999999999999</v>
       </c>
       <c r="S17" s="30">
@@ -3091,7 +3340,7 @@
         <v>-2.597</v>
       </c>
       <c r="V17" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>7.6989999999999998</v>
       </c>
       <c r="W17" s="30">
@@ -3103,7 +3352,7 @@
       <c r="Y17" s="30">
         <v>2.4969999999999999</v>
       </c>
-      <c r="Z17" s="64">
+      <c r="Z17" s="54">
         <f>AVERAGE(V17:Y17)</f>
         <v>3.7694999999999999</v>
       </c>
@@ -3113,17 +3362,53 @@
       <c r="AH17" s="30">
         <v>11.316000000000001</v>
       </c>
-      <c r="AI17" s="64">
-        <f t="shared" si="30"/>
+      <c r="AI17" s="54">
+        <f t="shared" si="35"/>
         <v>11.148499999999999</v>
       </c>
-    </row>
-    <row r="18" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ17" s="30">
+        <f t="shared" ref="AJ17:AR17" si="37">AVERAGE(AG17:AI17)</f>
+        <v>26.1905</v>
+      </c>
+      <c r="AK17" s="30">
+        <f t="shared" si="37"/>
+        <v>16.218333333333334</v>
+      </c>
+      <c r="AL17" s="30">
+        <f t="shared" si="37"/>
+        <v>17.852444444444444</v>
+      </c>
+      <c r="AM17" s="30">
+        <f t="shared" si="37"/>
+        <v>20.087092592592594</v>
+      </c>
+      <c r="AN17" s="30">
+        <f t="shared" si="37"/>
+        <v>18.052623456790126</v>
+      </c>
+      <c r="AO17" s="30">
+        <f t="shared" si="37"/>
+        <v>18.66405349794239</v>
+      </c>
+      <c r="AP17" s="30">
+        <f t="shared" si="37"/>
+        <v>18.93458984910837</v>
+      </c>
+      <c r="AQ17" s="30">
+        <f t="shared" si="37"/>
+        <v>18.550422267946963</v>
+      </c>
+      <c r="AR17" s="30">
+        <f t="shared" si="37"/>
+        <v>18.716355204999243</v>
+      </c>
+    </row>
+    <row r="18" spans="2:100" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="30" t="s">
         <v>98</v>
       </c>
       <c r="R18" s="30">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>-1.851</v>
       </c>
       <c r="S18" s="30">
@@ -3136,7 +3421,7 @@
         <v>0.11700000000000001</v>
       </c>
       <c r="V18" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>-2.1499999999999995</v>
       </c>
       <c r="W18" s="30">
@@ -3148,7 +3433,7 @@
       <c r="Y18" s="30">
         <v>-1.3180000000000001</v>
       </c>
-      <c r="Z18" s="64">
+      <c r="Z18" s="54">
         <f>AVERAGE(V18:Y18)</f>
         <v>-0.51774999999999993</v>
       </c>
@@ -3158,49 +3443,85 @@
       <c r="AH18" s="30">
         <v>-3.1349999999999998</v>
       </c>
-      <c r="AI18" s="64">
-        <f t="shared" si="30"/>
+      <c r="AI18" s="54">
+        <f t="shared" si="35"/>
         <v>-0.43874999999999997</v>
       </c>
-    </row>
-    <row r="19" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ18" s="30">
+        <f t="shared" ref="AJ18" si="38">AVERAGE(AG18:AI18)</f>
+        <v>-1.8082499999999999</v>
+      </c>
+      <c r="AK18" s="30">
+        <f t="shared" ref="AK18" si="39">AVERAGE(AH18:AJ18)</f>
+        <v>-1.7939999999999998</v>
+      </c>
+      <c r="AL18" s="30">
+        <f t="shared" ref="AL18" si="40">AVERAGE(AI18:AK18)</f>
+        <v>-1.3469999999999998</v>
+      </c>
+      <c r="AM18" s="30">
+        <f t="shared" ref="AM18" si="41">AVERAGE(AJ18:AL18)</f>
+        <v>-1.6497499999999998</v>
+      </c>
+      <c r="AN18" s="30">
+        <f t="shared" ref="AN18" si="42">AVERAGE(AK18:AM18)</f>
+        <v>-1.5969166666666663</v>
+      </c>
+      <c r="AO18" s="30">
+        <f t="shared" ref="AO18" si="43">AVERAGE(AL18:AN18)</f>
+        <v>-1.5312222222222218</v>
+      </c>
+      <c r="AP18" s="30">
+        <f t="shared" ref="AP18" si="44">AVERAGE(AM18:AO18)</f>
+        <v>-1.5926296296296292</v>
+      </c>
+      <c r="AQ18" s="30">
+        <f t="shared" ref="AQ18" si="45">AVERAGE(AN18:AP18)</f>
+        <v>-1.5735895061728391</v>
+      </c>
+      <c r="AR18" s="30">
+        <f t="shared" ref="AR18" si="46">AVERAGE(AO18:AQ18)</f>
+        <v>-1.5658137860082302</v>
+      </c>
+    </row>
+    <row r="19" spans="2:100" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="30" t="s">
         <v>99</v>
       </c>
       <c r="R19" s="30">
-        <f>R15+R16-R17+R18</f>
+        <f t="shared" ref="R19:Z19" si="47">R15+R16-R17+R18</f>
         <v>-262.69299999999998</v>
       </c>
       <c r="S19" s="30">
-        <f>S15+S16-S17+S18</f>
+        <f t="shared" si="47"/>
         <v>-65.368000000000023</v>
       </c>
       <c r="T19" s="30">
-        <f>T15+T16-T17+T18</f>
+        <f t="shared" si="47"/>
         <v>-75.594999999999985</v>
       </c>
       <c r="U19" s="30">
-        <f>U15+U16-U17+U18</f>
+        <f t="shared" si="47"/>
         <v>-73.850000000000009</v>
       </c>
       <c r="V19" s="30">
-        <f>V15+V16-V17+V18</f>
+        <f t="shared" si="47"/>
         <v>-88.075999999999979</v>
       </c>
       <c r="W19" s="30">
-        <f>W15+W16-W17+W18</f>
+        <f t="shared" si="47"/>
         <v>-76.147999999999982</v>
       </c>
       <c r="X19" s="30">
-        <f>X15+X16-X17+X18</f>
+        <f t="shared" si="47"/>
         <v>-115.81599999999996</v>
       </c>
       <c r="Y19" s="30">
-        <f>Y15+Y16-Y17+Y18</f>
+        <f t="shared" si="47"/>
         <v>-79.806000000000054</v>
       </c>
-      <c r="Z19" s="64">
-        <f>Z15+Z16-Z17+Z18</f>
+      <c r="Z19" s="54">
+        <f t="shared" si="47"/>
         <v>-91.557574800000012</v>
       </c>
       <c r="AG19" s="30">
@@ -3211,12 +3532,48 @@
         <f>AH15+AH16-AH17+AH18</f>
         <v>-302.88900000000001</v>
       </c>
-      <c r="AI19" s="64">
+      <c r="AI19" s="54">
         <f>AI15+AI16-AI17+AI18</f>
         <v>-363.32757480000009</v>
       </c>
-    </row>
-    <row r="20" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ19" s="30">
+        <f t="shared" ref="AJ19:AR19" si="48">AJ15+AJ16-AJ17+AJ18</f>
+        <v>-333.4181281333332</v>
+      </c>
+      <c r="AK19" s="30">
+        <f t="shared" si="48"/>
+        <v>-274.43610724444477</v>
+      </c>
+      <c r="AL19" s="30">
+        <f t="shared" si="48"/>
+        <v>-133.89116856592634</v>
+      </c>
+      <c r="AM19" s="30">
+        <f t="shared" si="48"/>
+        <v>-68.282723045234519</v>
+      </c>
+      <c r="AN19" s="30">
+        <f t="shared" si="48"/>
+        <v>783.47118106946482</v>
+      </c>
+      <c r="AO19" s="30">
+        <f t="shared" si="48"/>
+        <v>1340.5790345327687</v>
+      </c>
+      <c r="AP19" s="30">
+        <f t="shared" si="48"/>
+        <v>2000.9262966711337</v>
+      </c>
+      <c r="AQ19" s="30">
+        <f t="shared" si="48"/>
+        <v>2202.8824564784691</v>
+      </c>
+      <c r="AR19" s="30">
+        <f t="shared" si="48"/>
+        <v>2313.5554316845237</v>
+      </c>
+    </row>
+    <row r="20" spans="2:100" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="30" t="s">
         <v>100</v>
       </c>
@@ -3234,7 +3591,7 @@
         <v>2.2490000000000001</v>
       </c>
       <c r="V20" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>1.5659999999999994</v>
       </c>
       <c r="W20" s="30">
@@ -3246,7 +3603,7 @@
       <c r="Y20" s="30">
         <v>5.0350000000000001</v>
       </c>
-      <c r="Z20" s="64">
+      <c r="Z20" s="54">
         <f>Z19*(Z32)</f>
         <v>4.5778787400000009</v>
       </c>
@@ -3256,49 +3613,85 @@
       <c r="AH20" s="30">
         <v>3.9769999999999999</v>
       </c>
-      <c r="AI20" s="64">
-        <f t="shared" si="30"/>
+      <c r="AI20" s="54">
+        <f t="shared" si="35"/>
         <v>13.807878740000001</v>
       </c>
-    </row>
-    <row r="21" spans="2:44" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ20" s="30">
+        <f>AJ19*AJ32</f>
+        <v>16.67090640666666</v>
+      </c>
+      <c r="AK20" s="30">
+        <f t="shared" ref="AK20:AR20" si="49">AK19*AK32</f>
+        <v>8.233083217333343</v>
+      </c>
+      <c r="AL20" s="30">
+        <f t="shared" si="49"/>
+        <v>2.6778233713185267</v>
+      </c>
+      <c r="AM20" s="30">
+        <f t="shared" si="49"/>
+        <v>-3.414136152261726</v>
+      </c>
+      <c r="AN20" s="30">
+        <f t="shared" si="49"/>
+        <v>39.173559053473241</v>
+      </c>
+      <c r="AO20" s="30">
+        <f t="shared" si="49"/>
+        <v>134.05790345327688</v>
+      </c>
+      <c r="AP20" s="30">
+        <f t="shared" si="49"/>
+        <v>200.09262966711339</v>
+      </c>
+      <c r="AQ20" s="30">
+        <f t="shared" si="49"/>
+        <v>330.43236847177036</v>
+      </c>
+      <c r="AR20" s="30">
+        <f t="shared" si="49"/>
+        <v>347.03331475267856</v>
+      </c>
+    </row>
+    <row r="21" spans="2:100" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="31" t="s">
         <v>101</v>
       </c>
       <c r="R21" s="31">
-        <f>R19-R20</f>
+        <f t="shared" ref="R21:Z21" si="50">R19-R20</f>
         <v>-266.94399999999996</v>
       </c>
       <c r="S21" s="31">
-        <f>S19-S20</f>
+        <f t="shared" si="50"/>
         <v>-63.992000000000026</v>
       </c>
       <c r="T21" s="31">
-        <f>T19-T20</f>
+        <f t="shared" si="50"/>
         <v>-77.132999999999981</v>
       </c>
       <c r="U21" s="31">
-        <f>U19-U20</f>
+        <f t="shared" si="50"/>
         <v>-76.099000000000004</v>
       </c>
       <c r="V21" s="31">
-        <f>V19-V20</f>
+        <f t="shared" si="50"/>
         <v>-89.641999999999982</v>
       </c>
       <c r="W21" s="31">
-        <f>W19-W20</f>
+        <f t="shared" si="50"/>
         <v>-77.293999999999983</v>
       </c>
       <c r="X21" s="31">
-        <f>X19-X20</f>
+        <f t="shared" si="50"/>
         <v>-118.86499999999997</v>
       </c>
       <c r="Y21" s="31">
-        <f>Y19-Y20</f>
+        <f t="shared" si="50"/>
         <v>-84.841000000000051</v>
       </c>
-      <c r="Z21" s="62">
-        <f>Z19-Z20</f>
+      <c r="Z21" s="52">
+        <f t="shared" si="50"/>
         <v>-96.135453540000015</v>
       </c>
       <c r="AG21" s="31">
@@ -3309,49 +3702,309 @@
         <f>AH19-AH20</f>
         <v>-306.86599999999999</v>
       </c>
-      <c r="AI21" s="62">
+      <c r="AI21" s="52">
         <f>AI19-AI20</f>
         <v>-377.13545354000007</v>
       </c>
-    </row>
-    <row r="22" spans="2:44" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ21" s="31">
+        <f t="shared" ref="AJ21:AR21" si="51">AJ19-AJ20</f>
+        <v>-350.08903453999983</v>
+      </c>
+      <c r="AK21" s="31">
+        <f t="shared" si="51"/>
+        <v>-282.6691904617781</v>
+      </c>
+      <c r="AL21" s="31">
+        <f t="shared" si="51"/>
+        <v>-136.56899193724487</v>
+      </c>
+      <c r="AM21" s="31">
+        <f t="shared" si="51"/>
+        <v>-64.868586892972786</v>
+      </c>
+      <c r="AN21" s="31">
+        <f t="shared" si="51"/>
+        <v>744.29762201599158</v>
+      </c>
+      <c r="AO21" s="31">
+        <f t="shared" si="51"/>
+        <v>1206.5211310794919</v>
+      </c>
+      <c r="AP21" s="31">
+        <f t="shared" si="51"/>
+        <v>1800.8336670040203</v>
+      </c>
+      <c r="AQ21" s="31">
+        <f t="shared" si="51"/>
+        <v>1872.4500880066987</v>
+      </c>
+      <c r="AR21" s="31">
+        <f t="shared" si="51"/>
+        <v>1966.5221169318452</v>
+      </c>
+      <c r="AS21" s="31">
+        <f>AR21*(1+$AU$22)</f>
+        <v>1946.8568957625266</v>
+      </c>
+      <c r="AT21" s="31">
+        <f t="shared" ref="AT21:CV21" si="52">AS21*(1+$AU$22)</f>
+        <v>1927.3883268049012</v>
+      </c>
+      <c r="AU21" s="31">
+        <f t="shared" si="52"/>
+        <v>1908.1144435368521</v>
+      </c>
+      <c r="AV21" s="31">
+        <f t="shared" si="52"/>
+        <v>1889.0332991014836</v>
+      </c>
+      <c r="AW21" s="31">
+        <f t="shared" si="52"/>
+        <v>1870.1429661104687</v>
+      </c>
+      <c r="AX21" s="31">
+        <f t="shared" si="52"/>
+        <v>1851.4415364493641</v>
+      </c>
+      <c r="AY21" s="31">
+        <f t="shared" si="52"/>
+        <v>1832.9271210848704</v>
+      </c>
+      <c r="AZ21" s="31">
+        <f t="shared" si="52"/>
+        <v>1814.5978498740217</v>
+      </c>
+      <c r="BA21" s="31">
+        <f t="shared" si="52"/>
+        <v>1796.4518713752814</v>
+      </c>
+      <c r="BB21" s="31">
+        <f t="shared" si="52"/>
+        <v>1778.4873526615286</v>
+      </c>
+      <c r="BC21" s="31">
+        <f t="shared" si="52"/>
+        <v>1760.7024791349133</v>
+      </c>
+      <c r="BD21" s="31">
+        <f t="shared" si="52"/>
+        <v>1743.0954543435641</v>
+      </c>
+      <c r="BE21" s="31">
+        <f t="shared" si="52"/>
+        <v>1725.6644998001284</v>
+      </c>
+      <c r="BF21" s="31">
+        <f t="shared" si="52"/>
+        <v>1708.4078548021271</v>
+      </c>
+      <c r="BG21" s="31">
+        <f t="shared" si="52"/>
+        <v>1691.3237762541057</v>
+      </c>
+      <c r="BH21" s="31">
+        <f t="shared" si="52"/>
+        <v>1674.4105384915647</v>
+      </c>
+      <c r="BI21" s="31">
+        <f t="shared" si="52"/>
+        <v>1657.666433106649</v>
+      </c>
+      <c r="BJ21" s="31">
+        <f t="shared" si="52"/>
+        <v>1641.0897687755826</v>
+      </c>
+      <c r="BK21" s="31">
+        <f t="shared" si="52"/>
+        <v>1624.6788710878268</v>
+      </c>
+      <c r="BL21" s="31">
+        <f t="shared" si="52"/>
+        <v>1608.4320823769485</v>
+      </c>
+      <c r="BM21" s="31">
+        <f t="shared" si="52"/>
+        <v>1592.347761553179</v>
+      </c>
+      <c r="BN21" s="31">
+        <f t="shared" si="52"/>
+        <v>1576.4242839376473</v>
+      </c>
+      <c r="BO21" s="31">
+        <f t="shared" si="52"/>
+        <v>1560.6600410982708</v>
+      </c>
+      <c r="BP21" s="31">
+        <f t="shared" si="52"/>
+        <v>1545.053440687288</v>
+      </c>
+      <c r="BQ21" s="31">
+        <f t="shared" si="52"/>
+        <v>1529.602906280415</v>
+      </c>
+      <c r="BR21" s="31">
+        <f t="shared" si="52"/>
+        <v>1514.3068772176109</v>
+      </c>
+      <c r="BS21" s="31">
+        <f t="shared" si="52"/>
+        <v>1499.1638084454348</v>
+      </c>
+      <c r="BT21" s="31">
+        <f t="shared" si="52"/>
+        <v>1484.1721703609805</v>
+      </c>
+      <c r="BU21" s="31">
+        <f t="shared" si="52"/>
+        <v>1469.3304486573707</v>
+      </c>
+      <c r="BV21" s="31">
+        <f t="shared" si="52"/>
+        <v>1454.637144170797</v>
+      </c>
+      <c r="BW21" s="31">
+        <f t="shared" si="52"/>
+        <v>1440.0907727290889</v>
+      </c>
+      <c r="BX21" s="31">
+        <f t="shared" si="52"/>
+        <v>1425.6898650017981</v>
+      </c>
+      <c r="BY21" s="31">
+        <f t="shared" si="52"/>
+        <v>1411.4329663517801</v>
+      </c>
+      <c r="BZ21" s="31">
+        <f t="shared" si="52"/>
+        <v>1397.3186366882624</v>
+      </c>
+      <c r="CA21" s="31">
+        <f t="shared" si="52"/>
+        <v>1383.3454503213798</v>
+      </c>
+      <c r="CB21" s="31">
+        <f t="shared" si="52"/>
+        <v>1369.511995818166</v>
+      </c>
+      <c r="CC21" s="31">
+        <f t="shared" si="52"/>
+        <v>1355.8168758599843</v>
+      </c>
+      <c r="CD21" s="31">
+        <f t="shared" si="52"/>
+        <v>1342.2587071013845</v>
+      </c>
+      <c r="CE21" s="31">
+        <f t="shared" si="52"/>
+        <v>1328.8361200303707</v>
+      </c>
+      <c r="CF21" s="31">
+        <f t="shared" si="52"/>
+        <v>1315.5477588300669</v>
+      </c>
+      <c r="CG21" s="31">
+        <f t="shared" si="52"/>
+        <v>1302.3922812417661</v>
+      </c>
+      <c r="CH21" s="31">
+        <f t="shared" si="52"/>
+        <v>1289.3683584293485</v>
+      </c>
+      <c r="CI21" s="31">
+        <f t="shared" si="52"/>
+        <v>1276.474674845055</v>
+      </c>
+      <c r="CJ21" s="31">
+        <f t="shared" si="52"/>
+        <v>1263.7099280966045</v>
+      </c>
+      <c r="CK21" s="31">
+        <f t="shared" si="52"/>
+        <v>1251.0728288156383</v>
+      </c>
+      <c r="CL21" s="31">
+        <f t="shared" si="52"/>
+        <v>1238.562100527482</v>
+      </c>
+      <c r="CM21" s="31">
+        <f t="shared" si="52"/>
+        <v>1226.1764795222073</v>
+      </c>
+      <c r="CN21" s="31">
+        <f t="shared" si="52"/>
+        <v>1213.9147147269853</v>
+      </c>
+      <c r="CO21" s="31">
+        <f t="shared" si="52"/>
+        <v>1201.7755675797155</v>
+      </c>
+      <c r="CP21" s="31">
+        <f t="shared" si="52"/>
+        <v>1189.7578119039183</v>
+      </c>
+      <c r="CQ21" s="31">
+        <f t="shared" si="52"/>
+        <v>1177.860233784879</v>
+      </c>
+      <c r="CR21" s="31">
+        <f t="shared" si="52"/>
+        <v>1166.0816314470303</v>
+      </c>
+      <c r="CS21" s="31">
+        <f t="shared" si="52"/>
+        <v>1154.4208151325599</v>
+      </c>
+      <c r="CT21" s="31">
+        <f t="shared" si="52"/>
+        <v>1142.8766069812343</v>
+      </c>
+      <c r="CU21" s="31">
+        <f t="shared" si="52"/>
+        <v>1131.447840911422</v>
+      </c>
+      <c r="CV21" s="31">
+        <f t="shared" si="52"/>
+        <v>1120.1333625023078</v>
+      </c>
+    </row>
+    <row r="22" spans="2:100" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="36" t="s">
         <v>102</v>
       </c>
       <c r="R22" s="36">
-        <f>R21/R23</f>
+        <f t="shared" ref="R22:Z22" si="53">R21/R23</f>
         <v>-4.525655542249635</v>
       </c>
       <c r="S22" s="36">
-        <f>S21/S23</f>
+        <f t="shared" si="53"/>
         <v>-1.0428660106545344</v>
       </c>
       <c r="T22" s="36">
-        <f>T21/T23</f>
+        <f t="shared" si="53"/>
         <v>-1.2160968061806907</v>
       </c>
       <c r="U22" s="36">
-        <f>U21/U23</f>
+        <f t="shared" si="53"/>
         <v>-1.1463044248881236</v>
       </c>
       <c r="V22" s="36">
-        <f>V21/V23</f>
+        <f t="shared" si="53"/>
         <v>-1.3884416085043834</v>
       </c>
       <c r="W22" s="36">
-        <f>W21/W23</f>
+        <f t="shared" si="53"/>
         <v>-1.1416038004739926</v>
       </c>
       <c r="X22" s="36">
-        <f>X21/X23</f>
+        <f t="shared" si="53"/>
         <v>-1.739459023195089</v>
       </c>
       <c r="Y22" s="36">
-        <f>Y21/Y23</f>
+        <f t="shared" si="53"/>
         <v>-1.2310638914773968</v>
       </c>
-      <c r="Z22" s="65">
-        <f>Z21/Z23</f>
+      <c r="Z22" s="55">
+        <f t="shared" si="53"/>
         <v>-1.3949492055008406</v>
       </c>
       <c r="AG22" s="36">
@@ -3362,12 +4015,54 @@
         <f>AH21/AH23</f>
         <v>-4.7529676115582671</v>
       </c>
-      <c r="AI22" s="65">
+      <c r="AI22" s="55">
         <f>AI21/AI23</f>
         <v>-5.4723286977881589</v>
       </c>
-    </row>
-    <row r="23" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ22" s="36">
+        <f t="shared" ref="AJ22:AR22" si="54">AJ21/AJ23</f>
+        <v>-5.0798784694237069</v>
+      </c>
+      <c r="AK22" s="36">
+        <f t="shared" si="54"/>
+        <v>-4.1015998586843834</v>
+      </c>
+      <c r="AL22" s="36">
+        <f t="shared" si="54"/>
+        <v>-1.9816498470009758</v>
+      </c>
+      <c r="AM22" s="36">
+        <f t="shared" si="54"/>
+        <v>-0.94125923804649503</v>
+      </c>
+      <c r="AN22" s="36">
+        <f t="shared" si="54"/>
+        <v>10.799942562869115</v>
+      </c>
+      <c r="AO22" s="36">
+        <f t="shared" si="54"/>
+        <v>17.506919988878355</v>
+      </c>
+      <c r="AP22" s="36">
+        <f t="shared" si="54"/>
+        <v>26.130541860721564</v>
+      </c>
+      <c r="AQ22" s="36">
+        <f t="shared" si="54"/>
+        <v>27.169713840462972</v>
+      </c>
+      <c r="AR22" s="36">
+        <f t="shared" si="54"/>
+        <v>28.534722244510132</v>
+      </c>
+      <c r="AT22" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="AU22" s="80">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="23" spans="2:100" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="30" t="s">
         <v>3</v>
       </c>
@@ -3397,7 +4092,7 @@
       <c r="Y23" s="30">
         <v>68.916813000000005</v>
       </c>
-      <c r="Z23" s="64">
+      <c r="Z23" s="54">
         <f>Y23</f>
         <v>68.916813000000005</v>
       </c>
@@ -3407,16 +4102,74 @@
       <c r="AH23" s="30">
         <v>64.563032000000007</v>
       </c>
-      <c r="AI23" s="64">
+      <c r="AI23" s="54">
         <f>Z23</f>
         <v>68.916813000000005</v>
       </c>
-    </row>
-    <row r="24" spans="2:44" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="Z24" s="64"/>
-      <c r="AI24" s="64"/>
-    </row>
-    <row r="26" spans="2:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ23" s="30">
+        <f>AI23</f>
+        <v>68.916813000000005</v>
+      </c>
+      <c r="AK23" s="30">
+        <f t="shared" ref="AK23:AR23" si="55">AJ23</f>
+        <v>68.916813000000005</v>
+      </c>
+      <c r="AL23" s="30">
+        <f t="shared" si="55"/>
+        <v>68.916813000000005</v>
+      </c>
+      <c r="AM23" s="30">
+        <f t="shared" si="55"/>
+        <v>68.916813000000005</v>
+      </c>
+      <c r="AN23" s="30">
+        <f t="shared" si="55"/>
+        <v>68.916813000000005</v>
+      </c>
+      <c r="AO23" s="30">
+        <f t="shared" si="55"/>
+        <v>68.916813000000005</v>
+      </c>
+      <c r="AP23" s="30">
+        <f t="shared" si="55"/>
+        <v>68.916813000000005</v>
+      </c>
+      <c r="AQ23" s="30">
+        <f t="shared" si="55"/>
+        <v>68.916813000000005</v>
+      </c>
+      <c r="AR23" s="30">
+        <f t="shared" si="55"/>
+        <v>68.916813000000005</v>
+      </c>
+      <c r="AT23" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU23" s="81">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="24" spans="2:100" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Z24" s="54"/>
+      <c r="AI24" s="54"/>
+      <c r="AT24" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="AU24" s="75">
+        <f>NPV(AU23,AI21:CV21)</f>
+        <v>12918.266444642399</v>
+      </c>
+    </row>
+    <row r="25" spans="2:100" x14ac:dyDescent="0.2">
+      <c r="AT25" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="AU25" s="77">
+        <f>Main!C11</f>
+        <v>648.49</v>
+      </c>
+    </row>
+    <row r="26" spans="2:100" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>83</v>
       </c>
@@ -3429,50 +4182,57 @@
         <v>0.52787211882443508</v>
       </c>
       <c r="Y26" s="32">
-        <f t="shared" ref="Y26:Z26" si="31">Y6/U6-1</f>
+        <f t="shared" ref="Y26:Z26" si="56">Y6/U6-1</f>
         <v>0.47038912615197459</v>
       </c>
-      <c r="Z26" s="70">
-        <f t="shared" si="31"/>
+      <c r="Z26" s="60">
+        <f t="shared" si="56"/>
         <v>0.40211607015542561</v>
       </c>
       <c r="AH26" s="32">
         <f>AH6/AG6-1</f>
         <v>0.48003319895660423</v>
       </c>
-      <c r="AI26" s="70">
+      <c r="AI26" s="60">
         <f>AI6/AH6-1</f>
         <v>0.48364640150518068</v>
       </c>
       <c r="AJ26" s="32">
-        <v>0.52</v>
+        <v>0.5</v>
       </c>
       <c r="AK26" s="32">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
       <c r="AL26" s="32">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="AM26" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="AN26" s="32">
         <v>0.25</v>
       </c>
-      <c r="AN26" s="32">
+      <c r="AO26" s="32">
         <v>0.2</v>
-      </c>
-      <c r="AO26" s="32">
-        <v>0.15</v>
       </c>
       <c r="AP26" s="32">
         <v>0.15</v>
       </c>
       <c r="AQ26" s="32">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="AR26" s="32">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="27" spans="2:44" x14ac:dyDescent="0.2">
+        <v>0.05</v>
+      </c>
+      <c r="AT26" s="76" t="s">
+        <v>148</v>
+      </c>
+      <c r="AU26" s="75">
+        <f>AU24-AU25</f>
+        <v>12269.776444642399</v>
+      </c>
+    </row>
+    <row r="27" spans="2:100" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>84</v>
       </c>
@@ -3485,11 +4245,11 @@
         <v>0.14161723195821807</v>
       </c>
       <c r="V27" s="33">
-        <f t="shared" ref="V27:W27" si="32">V6/U6-1</f>
+        <f t="shared" ref="V27:W27" si="57">V6/U6-1</f>
         <v>0.17453601477348357</v>
       </c>
       <c r="W27" s="33">
-        <f t="shared" si="32"/>
+        <f t="shared" si="57"/>
         <v>7.1119800070545525E-2</v>
       </c>
       <c r="X27" s="33">
@@ -3497,10 +4257,10 @@
         <v>6.3805189755015812E-2</v>
       </c>
       <c r="Y27" s="33">
-        <f t="shared" ref="Y27" si="33">Y6/X6-1</f>
+        <f t="shared" ref="Y27" si="58">Y6/X6-1</f>
         <v>9.8666271487848123E-2</v>
       </c>
-      <c r="Z27" s="66">
+      <c r="Z27" s="56">
         <v>0.12</v>
       </c>
       <c r="AD27" s="21" t="s">
@@ -3518,8 +4278,24 @@
       <c r="AH27" s="21" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="29" spans="2:44" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT27" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU27" s="82">
+        <f>AU26/Main!C7</f>
+        <v>178.03749057058687</v>
+      </c>
+    </row>
+    <row r="28" spans="2:100" x14ac:dyDescent="0.2">
+      <c r="AT28" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="AU28" s="77">
+        <f>Main!C6</f>
+        <v>191.75</v>
+      </c>
+    </row>
+    <row r="29" spans="2:100" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="33" t="s">
         <v>85</v>
       </c>
@@ -3528,7 +4304,7 @@
         <v>0.69981502686514585</v>
       </c>
       <c r="T29" s="33">
-        <f t="shared" ref="T29" si="34">T10/T6</f>
+        <f t="shared" ref="T29" si="59">T10/T6</f>
         <v>0.69457652190976471</v>
       </c>
       <c r="U29" s="33">
@@ -3536,7 +4312,7 @@
         <v>0.69825424318952101</v>
       </c>
       <c r="V29" s="33">
-        <f t="shared" ref="V29" si="35">V10/V6</f>
+        <f t="shared" ref="V29" si="60">V10/V6</f>
         <v>0.71557333373359255</v>
       </c>
       <c r="W29" s="33">
@@ -3544,26 +4320,26 @@
         <v>0.72599116473460923</v>
       </c>
       <c r="X29" s="33">
-        <f t="shared" ref="X29:Y29" si="36">X10/X6</f>
+        <f t="shared" ref="X29:Y29" si="61">X10/X6</f>
         <v>0.70928999538958049</v>
       </c>
       <c r="Y29" s="33">
-        <f t="shared" si="36"/>
+        <f t="shared" si="61"/>
         <v>0.71928625596110563</v>
       </c>
-      <c r="Z29" s="66">
+      <c r="Z29" s="56">
         <v>0.72</v>
       </c>
       <c r="AG29" s="33">
-        <f t="shared" ref="AG29:AR29" si="37">AG10/AG6</f>
+        <f t="shared" ref="AG29:AH29" si="62">AG10/AG6</f>
         <v>0.7000643653240286</v>
       </c>
       <c r="AH29" s="33">
-        <f t="shared" si="37"/>
+        <f t="shared" si="62"/>
         <v>0.703024324144924</v>
       </c>
-      <c r="AI29" s="66">
-        <f t="shared" ref="AI29" si="38">AI10/AI6</f>
+      <c r="AI29" s="56">
+        <f t="shared" ref="AI29" si="63">AI10/AI6</f>
         <v>0.71862682611084105</v>
       </c>
       <c r="AJ29" s="33">
@@ -3593,8 +4369,15 @@
       <c r="AR29" s="33">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="30" spans="2:44" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT29" s="78" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU29" s="79">
+        <f>AU27/AU28-1</f>
+        <v>-7.1512435094722937E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:100" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="33" t="s">
         <v>86</v>
       </c>
@@ -3603,7 +4386,7 @@
         <v>-0.33826962036466146</v>
       </c>
       <c r="T30" s="33">
-        <f t="shared" ref="T30" si="39">T15/T6</f>
+        <f t="shared" ref="T30" si="64">T15/T6</f>
         <v>-0.3649413576053977</v>
       </c>
       <c r="U30" s="33">
@@ -3611,7 +4394,7 @@
         <v>-0.33834450600062582</v>
       </c>
       <c r="V30" s="33">
-        <f t="shared" ref="V30" si="40">V15/V6</f>
+        <f t="shared" ref="V30" si="65">V15/V6</f>
         <v>-0.29501227044511308</v>
       </c>
       <c r="W30" s="33">
@@ -3619,31 +4402,31 @@
         <v>-0.26603887937165205</v>
       </c>
       <c r="X30" s="33">
-        <f t="shared" ref="X30:Z31" si="41">X15/X6</f>
+        <f t="shared" ref="X30:Z30" si="66">X15/X6</f>
         <v>-0.37819600869393383</v>
       </c>
       <c r="Y30" s="33">
-        <f t="shared" si="41"/>
+        <f t="shared" si="66"/>
         <v>-0.24855449746868472</v>
       </c>
-      <c r="Z30" s="66">
-        <f t="shared" si="41"/>
+      <c r="Z30" s="56">
+        <f t="shared" si="66"/>
         <v>-0.24000000000000002</v>
       </c>
       <c r="AG30" s="33">
-        <f t="shared" ref="AG30:AR30" si="42">AG15/AG6</f>
+        <f t="shared" ref="AG30:AH30" si="67">AG15/AG6</f>
         <v>-0.35452420474948332</v>
       </c>
       <c r="AH30" s="33">
-        <f t="shared" si="42"/>
+        <f t="shared" si="67"/>
         <v>-0.33116269275402793</v>
       </c>
-      <c r="AI30" s="66">
-        <f t="shared" ref="AI30" si="43">AI15/AI6</f>
+      <c r="AI30" s="56">
+        <f t="shared" ref="AI30" si="68">AI15/AI6</f>
         <v>-0.2803054182607938</v>
       </c>
     </row>
-    <row r="31" spans="2:44" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:100" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="33" t="s">
         <v>87</v>
       </c>
@@ -3652,7 +4435,7 @@
         <v>-0.35228573945212732</v>
       </c>
       <c r="T31" s="33">
-        <f t="shared" ref="T31" si="44">T21/T6</f>
+        <f t="shared" ref="T31" si="69">T21/T6</f>
         <v>-0.38809642409696737</v>
       </c>
       <c r="U31" s="33">
@@ -3660,7 +4443,7 @@
         <v>-0.33539597960272022</v>
       </c>
       <c r="V31" s="33">
-        <f t="shared" ref="V31" si="45">V21/V6</f>
+        <f t="shared" ref="V31" si="70">V21/V6</f>
         <v>-0.336375303008698</v>
       </c>
       <c r="W31" s="33">
@@ -3668,31 +4451,31 @@
         <v>-0.27078231685742005</v>
       </c>
       <c r="X31" s="33">
-        <f t="shared" ref="X31:Z31" si="46">X21/X6</f>
+        <f t="shared" ref="X31:Z31" si="71">X21/X6</f>
         <v>-0.39144108542448774</v>
       </c>
       <c r="Y31" s="33">
-        <f t="shared" si="46"/>
+        <f t="shared" si="71"/>
         <v>-0.2543035360483904</v>
       </c>
-      <c r="Z31" s="66">
-        <f t="shared" si="46"/>
+      <c r="Z31" s="56">
+        <f t="shared" si="71"/>
         <v>-0.2572836433407969</v>
       </c>
       <c r="AG31" s="33">
-        <f t="shared" ref="AG31:AH31" si="47">AG21/AG6</f>
+        <f t="shared" ref="AG31:AH31" si="72">AG21/AG6</f>
         <v>-0.45215623835495777</v>
       </c>
       <c r="AH31" s="33">
-        <f t="shared" si="47"/>
+        <f t="shared" si="72"/>
         <v>-0.35119286046176273</v>
       </c>
-      <c r="AI31" s="66">
-        <f t="shared" ref="AI31" si="48">AI21/AI6</f>
+      <c r="AI31" s="56">
+        <f t="shared" ref="AI31" si="73">AI21/AI6</f>
         <v>-0.29091348950501938</v>
       </c>
     </row>
-    <row r="32" spans="2:44" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:100" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="33" t="s">
         <v>88</v>
       </c>
@@ -3701,7 +4484,7 @@
         <v>2.1050055072818496E-2</v>
       </c>
       <c r="T32" s="33">
-        <f t="shared" ref="T32" si="49">T20/T19</f>
+        <f t="shared" ref="T32" si="74">T20/T19</f>
         <v>-2.0345260929955689E-2</v>
       </c>
       <c r="U32" s="33">
@@ -3709,7 +4492,7 @@
         <v>-3.0453622207176706E-2</v>
       </c>
       <c r="V32" s="33">
-        <f t="shared" ref="V32" si="50">V20/V19</f>
+        <f t="shared" ref="V32" si="75">V20/V19</f>
         <v>-1.7780099005404421E-2</v>
       </c>
       <c r="W32" s="33">
@@ -3717,27 +4500,54 @@
         <v>-1.5049640174397229E-2</v>
       </c>
       <c r="X32" s="33">
-        <f t="shared" ref="X32:Y32" si="51">X20/X19</f>
+        <f t="shared" ref="X32:Y32" si="76">X20/X19</f>
         <v>-2.6326241624645998E-2</v>
       </c>
       <c r="Y32" s="33">
-        <f t="shared" si="51"/>
+        <f t="shared" si="76"/>
         <v>-6.3090494449038872E-2</v>
       </c>
-      <c r="Z32" s="66">
+      <c r="Z32" s="56">
         <v>-0.05</v>
       </c>
       <c r="AG32" s="33">
-        <f t="shared" ref="AG32:AH32" si="52">AG20/AG19</f>
+        <f t="shared" ref="AG32:AH32" si="77">AG20/AG19</f>
         <v>-1.6182387806298611E-2</v>
       </c>
       <c r="AH32" s="33">
-        <f t="shared" si="52"/>
+        <f t="shared" si="77"/>
         <v>-1.3130222622809015E-2</v>
       </c>
-      <c r="AI32" s="66">
-        <f t="shared" ref="AI32" si="53">AI20/AI19</f>
+      <c r="AI32" s="56">
+        <f t="shared" ref="AI32" si="78">AI20/AI19</f>
         <v>-3.8003938312694226E-2</v>
+      </c>
+      <c r="AJ32" s="33">
+        <v>-0.05</v>
+      </c>
+      <c r="AK32" s="33">
+        <v>-0.03</v>
+      </c>
+      <c r="AL32" s="33">
+        <v>-0.02</v>
+      </c>
+      <c r="AM32" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="AN32" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="AO32" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="AP32" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="AQ32" s="33">
+        <v>0.15</v>
+      </c>
+      <c r="AR32" s="33">
+        <v>0.15</v>
       </c>
     </row>
     <row r="36" spans="2:35" x14ac:dyDescent="0.2">
@@ -3761,7 +4571,7 @@
       <c r="Y37" s="31">
         <v>999.67399999999998</v>
       </c>
-      <c r="Z37" s="63"/>
+      <c r="Z37" s="53"/>
       <c r="AG37" s="31">
         <v>429.697</v>
       </c>
@@ -3769,7 +4579,7 @@
         <f>V37</f>
         <v>473.904</v>
       </c>
-      <c r="AI37" s="62"/>
+      <c r="AI37" s="52"/>
     </row>
     <row r="38" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
@@ -3787,7 +4597,7 @@
       <c r="Y38" s="31">
         <v>787.85799999999995</v>
       </c>
-      <c r="Z38" s="63"/>
+      <c r="Z38" s="53"/>
       <c r="AG38" s="31">
         <v>528.04499999999996</v>
       </c>
@@ -3795,7 +4605,7 @@
         <f>V38</f>
         <v>1352.019</v>
       </c>
-      <c r="AI38" s="62"/>
+      <c r="AI38" s="52"/>
     </row>
     <row r="39" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
@@ -3841,7 +4651,7 @@
         <v>36.619</v>
       </c>
       <c r="AH40" s="30">
-        <f t="shared" ref="AH40:AH47" si="54">V40</f>
+        <f t="shared" ref="AH40:AH47" si="79">V40</f>
         <v>63.523000000000003</v>
       </c>
     </row>
@@ -3865,7 +4675,7 @@
         <v>12.35</v>
       </c>
       <c r="AH41" s="30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="79"/>
         <v>32.573</v>
       </c>
     </row>
@@ -3874,83 +4684,83 @@
         <v>108</v>
       </c>
       <c r="C42" s="30">
-        <f t="shared" ref="C42:V42" si="55">SUM(C37:C41)</f>
+        <f t="shared" ref="C42:V42" si="80">SUM(C37:C41)</f>
         <v>0</v>
       </c>
       <c r="D42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="E42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="F42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="G42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="H42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="I42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="J42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="K42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="L42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="M42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="N42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="O42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="P42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="Q42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="R42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="S42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="T42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="U42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="V42" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="80"/>
         <v>2117.402</v>
       </c>
       <c r="W42" s="30">
@@ -3958,19 +4768,19 @@
         <v>2096.3070000000002</v>
       </c>
       <c r="X42" s="30">
-        <f t="shared" ref="X42:Y42" si="56">SUM(X37:X41)</f>
+        <f t="shared" ref="X42:Y42" si="81">SUM(X37:X41)</f>
         <v>2108.5140000000001</v>
       </c>
       <c r="Y42" s="30">
-        <f t="shared" si="56"/>
+        <f t="shared" si="81"/>
         <v>2122.2549999999997</v>
       </c>
       <c r="AG42" s="30">
-        <f t="shared" ref="AG42:AH42" si="57">SUM(AG37:AG41)</f>
+        <f t="shared" ref="AG42:AH42" si="82">SUM(AG37:AG41)</f>
         <v>1141.8869999999997</v>
       </c>
       <c r="AH42" s="30">
-        <f t="shared" si="57"/>
+        <f t="shared" si="82"/>
         <v>2117.402</v>
       </c>
     </row>
@@ -3994,7 +4804,7 @@
         <v>62.363999999999997</v>
       </c>
       <c r="AH43" s="30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="79"/>
         <v>62.625</v>
       </c>
     </row>
@@ -4018,7 +4828,7 @@
         <v>34.587000000000003</v>
       </c>
       <c r="AH44" s="30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="79"/>
         <v>41.744999999999997</v>
       </c>
     </row>
@@ -4047,7 +4857,7 @@
         <v>82.10499999999999</v>
       </c>
       <c r="AH45" s="30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="79"/>
         <v>78.382999999999996</v>
       </c>
     </row>
@@ -4071,7 +4881,7 @@
         <v>0.997</v>
       </c>
       <c r="AH46" s="30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="79"/>
         <v>1.9390000000000001</v>
       </c>
     </row>
@@ -4095,7 +4905,7 @@
         <v>85.555000000000007</v>
       </c>
       <c r="AH47" s="30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="79"/>
         <v>147.494</v>
       </c>
     </row>
@@ -4104,83 +4914,83 @@
         <v>114</v>
       </c>
       <c r="C48" s="30">
-        <f t="shared" ref="C48:V48" si="58">C42+SUM(C43:C47)</f>
+        <f t="shared" ref="C48:V48" si="83">C42+SUM(C43:C47)</f>
         <v>0</v>
       </c>
       <c r="D48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="E48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="F48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="G48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="H48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="I48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="J48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="K48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="L48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="M48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="N48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="O48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="P48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="Q48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="R48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="S48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="T48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="U48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="V48" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="83"/>
         <v>2449.5880000000002</v>
       </c>
       <c r="W48" s="30">
@@ -4248,7 +5058,7 @@
         <v>70.209999999999994</v>
       </c>
       <c r="AH51" s="30">
-        <f t="shared" ref="AH51:AH54" si="59">V51</f>
+        <f t="shared" ref="AH51:AH54" si="84">V51</f>
         <v>112.568</v>
       </c>
     </row>
@@ -4272,7 +5082,7 @@
         <v>2.343</v>
       </c>
       <c r="AH52" s="30">
-        <f t="shared" si="59"/>
+        <f t="shared" si="84"/>
         <v>8.0839999999999996</v>
       </c>
     </row>
@@ -4296,7 +5106,7 @@
         <v>56.44</v>
       </c>
       <c r="AH53" s="30">
-        <f t="shared" si="59"/>
+        <f t="shared" si="84"/>
         <v>48.847999999999999</v>
       </c>
     </row>
@@ -4320,7 +5130,7 @@
         <v>221.404</v>
       </c>
       <c r="AH54" s="30">
-        <f t="shared" si="59"/>
+        <f t="shared" si="84"/>
         <v>352.00099999999998</v>
       </c>
     </row>
@@ -4329,83 +5139,83 @@
         <v>120</v>
       </c>
       <c r="C55" s="30">
-        <f t="shared" ref="C55:V55" si="60">SUM(C50:C54)</f>
+        <f t="shared" ref="C55:V55" si="85">SUM(C50:C54)</f>
         <v>0</v>
       </c>
       <c r="D55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="E55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="F55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="G55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="H55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="I55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="J55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="K55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="L55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="M55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="N55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="O55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="P55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="Q55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="R55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="S55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="T55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="U55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="V55" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="85"/>
         <v>526.7349999999999</v>
       </c>
       <c r="W55" s="30">
@@ -4497,7 +5307,7 @@
         <v>16.547000000000001</v>
       </c>
       <c r="AH58" s="30">
-        <f t="shared" ref="AH58" si="61">V58</f>
+        <f t="shared" ref="AH58" si="86">V58</f>
         <v>23.178999999999998</v>
       </c>
     </row>
@@ -4517,7 +5327,7 @@
       <c r="Y59" s="31">
         <v>1139.0419999999999</v>
       </c>
-      <c r="Z59" s="63"/>
+      <c r="Z59" s="53"/>
       <c r="AG59" s="31">
         <v>937.72900000000004</v>
       </c>
@@ -4525,7 +5335,7 @@
         <f>V59</f>
         <v>1136.521</v>
       </c>
-      <c r="AI59" s="62"/>
+      <c r="AI59" s="52"/>
     </row>
     <row r="60" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
@@ -4547,7 +5357,7 @@
         <v>59.128999999999998</v>
       </c>
       <c r="AH60" s="30">
-        <f t="shared" ref="AH60" si="62">V60</f>
+        <f t="shared" ref="AH60" si="87">V60</f>
         <v>57.664999999999999</v>
       </c>
     </row>
@@ -4556,83 +5366,83 @@
         <v>123</v>
       </c>
       <c r="C61" s="30">
-        <f t="shared" ref="C61:V61" si="63">C55+SUM(C56:C60)</f>
+        <f t="shared" ref="C61:V61" si="88">C55+SUM(C56:C60)</f>
         <v>0</v>
       </c>
       <c r="D61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="E61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="F61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="G61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="H61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="I61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="J61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="K61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="L61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="M61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="N61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="O61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="P61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="Q61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="R61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="S61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="T61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="U61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="V61" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="88"/>
         <v>1782.8879999999999</v>
       </c>
       <c r="W61" s="30">
@@ -4685,192 +5495,192 @@
         <v>125</v>
       </c>
       <c r="C64" s="30">
-        <f t="shared" ref="C64" si="64">C63+C61</f>
+        <f t="shared" ref="C64" si="89">C63+C61</f>
         <v>0</v>
       </c>
       <c r="D64" s="30">
-        <f t="shared" ref="D64" si="65">D63+D61</f>
+        <f t="shared" ref="D64" si="90">D63+D61</f>
         <v>0</v>
       </c>
       <c r="E64" s="30">
-        <f t="shared" ref="E64" si="66">E63+E61</f>
+        <f t="shared" ref="E64" si="91">E63+E61</f>
         <v>0</v>
       </c>
       <c r="F64" s="30">
-        <f t="shared" ref="F64" si="67">F63+F61</f>
+        <f t="shared" ref="F64" si="92">F63+F61</f>
         <v>0</v>
       </c>
       <c r="G64" s="30">
-        <f t="shared" ref="G64" si="68">G63+G61</f>
+        <f t="shared" ref="G64" si="93">G63+G61</f>
         <v>0</v>
       </c>
       <c r="H64" s="30">
-        <f t="shared" ref="H64" si="69">H63+H61</f>
+        <f t="shared" ref="H64" si="94">H63+H61</f>
         <v>0</v>
       </c>
       <c r="I64" s="30">
-        <f t="shared" ref="I64" si="70">I63+I61</f>
+        <f t="shared" ref="I64" si="95">I63+I61</f>
         <v>0</v>
       </c>
       <c r="J64" s="30">
-        <f t="shared" ref="J64" si="71">J63+J61</f>
+        <f t="shared" ref="J64" si="96">J63+J61</f>
         <v>0</v>
       </c>
       <c r="K64" s="30">
-        <f t="shared" ref="K64" si="72">K63+K61</f>
+        <f t="shared" ref="K64" si="97">K63+K61</f>
         <v>0</v>
       </c>
       <c r="L64" s="30">
-        <f t="shared" ref="L64" si="73">L63+L61</f>
+        <f t="shared" ref="L64" si="98">L63+L61</f>
         <v>0</v>
       </c>
       <c r="M64" s="30">
-        <f t="shared" ref="M64" si="74">M63+M61</f>
+        <f t="shared" ref="M64" si="99">M63+M61</f>
         <v>0</v>
       </c>
       <c r="N64" s="30">
-        <f t="shared" ref="N64" si="75">N63+N61</f>
+        <f t="shared" ref="N64" si="100">N63+N61</f>
         <v>0</v>
       </c>
       <c r="O64" s="30">
-        <f t="shared" ref="O64" si="76">O63+O61</f>
+        <f t="shared" ref="O64" si="101">O63+O61</f>
         <v>0</v>
       </c>
       <c r="P64" s="30">
-        <f t="shared" ref="P64" si="77">P63+P61</f>
+        <f t="shared" ref="P64" si="102">P63+P61</f>
         <v>0</v>
       </c>
       <c r="Q64" s="30">
-        <f t="shared" ref="Q64" si="78">Q63+Q61</f>
+        <f t="shared" ref="Q64" si="103">Q63+Q61</f>
         <v>0</v>
       </c>
       <c r="R64" s="30">
-        <f t="shared" ref="R64" si="79">R63+R61</f>
+        <f t="shared" ref="R64" si="104">R63+R61</f>
         <v>0</v>
       </c>
       <c r="S64" s="30">
-        <f t="shared" ref="S64" si="80">S63+S61</f>
+        <f t="shared" ref="S64" si="105">S63+S61</f>
         <v>0</v>
       </c>
       <c r="T64" s="30">
-        <f t="shared" ref="T64" si="81">T63+T61</f>
+        <f t="shared" ref="T64" si="106">T63+T61</f>
         <v>0</v>
       </c>
       <c r="U64" s="30">
-        <f t="shared" ref="U64" si="82">U63+U61</f>
+        <f t="shared" ref="U64" si="107">U63+U61</f>
         <v>0</v>
       </c>
       <c r="V64" s="30">
-        <f t="shared" ref="V64" si="83">V63+V61</f>
+        <f t="shared" ref="V64" si="108">V63+V61</f>
         <v>2449.5879999999997</v>
       </c>
       <c r="W64" s="30">
-        <f t="shared" ref="W64:Y64" si="84">W63+W61</f>
+        <f t="shared" ref="W64:Y64" si="109">W63+W61</f>
         <v>2434.5410000000002</v>
       </c>
       <c r="X64" s="30">
-        <f t="shared" ref="X64" si="85">X63+X61</f>
+        <f t="shared" ref="X64" si="110">X63+X61</f>
         <v>2451.598</v>
       </c>
       <c r="Y64" s="30">
-        <f t="shared" si="84"/>
+        <f t="shared" si="109"/>
         <v>2467.1860000000001</v>
       </c>
-      <c r="AF64" s="57"/>
+      <c r="AF64" s="47"/>
       <c r="AG64" s="30">
         <f>AG63+AG61</f>
         <v>1402.7809999999999</v>
       </c>
       <c r="AH64" s="30">
-        <f t="shared" ref="AG64:AH64" si="86">AH63+AH61</f>
+        <f t="shared" ref="AH64" si="111">AH63+AH61</f>
         <v>2449.6</v>
       </c>
     </row>
     <row r="65" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="AF65" s="57"/>
+      <c r="AF65" s="47"/>
     </row>
     <row r="66" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
         <v>126</v>
       </c>
       <c r="C66" s="30">
-        <f t="shared" ref="C66:V66" si="87">C48-C61</f>
+        <f t="shared" ref="C66:V66" si="112">C48-C61</f>
         <v>0</v>
       </c>
       <c r="D66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="E66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="F66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="G66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="H66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="I66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="J66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="K66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="L66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="M66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="N66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="O66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="P66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="Q66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="R66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="S66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="T66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="U66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="V66" s="30">
-        <f t="shared" si="87"/>
+        <f t="shared" si="112"/>
         <v>666.70000000000027</v>
       </c>
       <c r="W66" s="30">
@@ -4878,20 +5688,20 @@
         <v>672.87900000000013</v>
       </c>
       <c r="X66" s="30">
-        <f t="shared" ref="X66:Y66" si="88">X48-X61</f>
+        <f t="shared" ref="X66:Y66" si="113">X48-X61</f>
         <v>668.16800000000012</v>
       </c>
       <c r="Y66" s="30">
-        <f t="shared" si="88"/>
+        <f t="shared" si="113"/>
         <v>684.2819999999997</v>
       </c>
-      <c r="AF66" s="57"/>
+      <c r="AF66" s="47"/>
       <c r="AG66" s="30">
-        <f t="shared" ref="AG66:AH66" si="89">AG48-AG61</f>
+        <f t="shared" ref="AG66:AH66" si="114">AG48-AG61</f>
         <v>-0.31900000000018736</v>
       </c>
       <c r="AH66" s="30">
-        <f t="shared" si="89"/>
+        <f t="shared" si="114"/>
         <v>666.68800000000033</v>
       </c>
     </row>
@@ -4900,79 +5710,79 @@
         <v>127</v>
       </c>
       <c r="C67" s="1" t="e">
-        <f t="shared" ref="C67:V67" si="90">C66/C23</f>
+        <f t="shared" ref="C67:U67" si="115">C66/C23</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q67" s="1" t="e">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R67" s="1">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>0</v>
       </c>
       <c r="S67" s="1">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>0</v>
       </c>
       <c r="T67" s="1">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>0</v>
       </c>
       <c r="U67" s="1">
-        <f t="shared" si="90"/>
+        <f t="shared" si="115"/>
         <v>0</v>
       </c>
       <c r="V67" s="1">
@@ -4984,19 +5794,19 @@
         <v>9.9381740323846604</v>
       </c>
       <c r="X67" s="1">
-        <f t="shared" ref="X67:Y67" si="91">X66/X23</f>
+        <f t="shared" ref="X67:Y67" si="116">X66/X23</f>
         <v>9.7779065041031146</v>
       </c>
       <c r="Y67" s="1">
-        <f t="shared" si="91"/>
+        <f t="shared" si="116"/>
         <v>9.929101045342879</v>
       </c>
       <c r="AG67" s="1">
-        <f t="shared" ref="AG67:AH67" si="92">AG66/AG23</f>
+        <f t="shared" ref="AG67:AH67" si="117">AG66/AG23</f>
         <v>-5.4081909238584934E-3</v>
       </c>
       <c r="AH67" s="1">
-        <f t="shared" si="92"/>
+        <f t="shared" si="117"/>
         <v>10.326156925219998</v>
       </c>
     </row>
@@ -5005,83 +5815,83 @@
         <v>5</v>
       </c>
       <c r="C69" s="34">
-        <f t="shared" ref="C69:V69" si="93">C37+C38</f>
+        <f t="shared" ref="C69:V69" si="118">C37+C38</f>
         <v>0</v>
       </c>
       <c r="D69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="E69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="F69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="G69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="H69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="I69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="J69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="K69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="L69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="M69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="N69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="O69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="P69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="Q69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="R69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="S69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="T69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="U69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="V69" s="34">
-        <f t="shared" si="93"/>
+        <f t="shared" si="118"/>
         <v>1825.923</v>
       </c>
       <c r="W69" s="34">
@@ -5093,102 +5903,102 @@
         <v>1795.6120000000001</v>
       </c>
       <c r="Y69" s="34">
-        <f t="shared" ref="Y69" si="94">Y37+Y38</f>
+        <f t="shared" ref="Y69" si="119">Y37+Y38</f>
         <v>1787.5319999999999</v>
       </c>
-      <c r="Z69" s="59"/>
+      <c r="Z69" s="49"/>
       <c r="AG69" s="34">
-        <f t="shared" ref="AG69:AH69" si="95">AG37+AG38</f>
+        <f t="shared" ref="AG69:AH69" si="120">AG37+AG38</f>
         <v>957.74199999999996</v>
       </c>
       <c r="AH69" s="34">
-        <f t="shared" si="95"/>
+        <f t="shared" si="120"/>
         <v>1825.923</v>
       </c>
-      <c r="AI69" s="64"/>
+      <c r="AI69" s="54"/>
     </row>
     <row r="70" spans="2:35" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="38" t="s">
         <v>6</v>
       </c>
       <c r="C70" s="34">
-        <f t="shared" ref="C70:V70" si="96">C59</f>
+        <f t="shared" ref="C70:V70" si="121">C59</f>
         <v>0</v>
       </c>
       <c r="D70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="E70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="F70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="G70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="H70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="I70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="J70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="K70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="L70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="M70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="N70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="O70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="P70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="Q70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="R70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="S70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="T70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="U70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>0</v>
       </c>
       <c r="V70" s="34">
-        <f t="shared" si="96"/>
+        <f t="shared" si="121"/>
         <v>1136.521</v>
       </c>
       <c r="W70" s="34">
@@ -5200,102 +6010,102 @@
         <v>1138.2</v>
       </c>
       <c r="Y70" s="34">
-        <f t="shared" ref="Y70" si="97">Y59</f>
+        <f t="shared" ref="Y70" si="122">Y59</f>
         <v>1139.0419999999999</v>
       </c>
-      <c r="Z70" s="59"/>
+      <c r="Z70" s="49"/>
       <c r="AG70" s="34">
-        <f t="shared" ref="AG70:AH70" si="98">AG59</f>
+        <f t="shared" ref="AG70:AH70" si="123">AG59</f>
         <v>937.72900000000004</v>
       </c>
       <c r="AH70" s="34">
-        <f t="shared" si="98"/>
+        <f t="shared" si="123"/>
         <v>1136.521</v>
       </c>
-      <c r="AI70" s="64"/>
+      <c r="AI70" s="54"/>
     </row>
     <row r="71" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C71" s="30">
-        <f t="shared" ref="C71:V71" si="99">C69-C70</f>
+        <f t="shared" ref="C71:V71" si="124">C69-C70</f>
         <v>0</v>
       </c>
       <c r="D71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="E71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="F71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="G71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="H71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="I71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="J71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="K71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="L71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="M71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="N71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="O71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="P71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="Q71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="R71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="S71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="T71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="U71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="V71" s="30">
-        <f t="shared" si="99"/>
+        <f t="shared" si="124"/>
         <v>689.40200000000004</v>
       </c>
       <c r="W71" s="30">
@@ -5307,15 +6117,15 @@
         <v>657.41200000000003</v>
       </c>
       <c r="Y71" s="30">
-        <f t="shared" ref="Y71" si="100">Y69-Y70</f>
+        <f t="shared" ref="Y71" si="125">Y69-Y70</f>
         <v>648.49</v>
       </c>
       <c r="AG71" s="30">
-        <f t="shared" ref="AG71" si="101">AG69-AG70</f>
+        <f t="shared" ref="AG71" si="126">AG69-AG70</f>
         <v>20.01299999999992</v>
       </c>
       <c r="AH71" s="30">
-        <f t="shared" ref="AH71" si="102">AH69-AH70</f>
+        <f t="shared" ref="AH71" si="127">AH69-AH70</f>
         <v>689.40200000000004</v>
       </c>
     </row>
@@ -5348,7 +6158,7 @@
         <v>4</v>
       </c>
       <c r="V74" s="30">
-        <f t="shared" ref="V74" si="103">V73*V23</f>
+        <f t="shared" ref="V74" si="128">V73*V23</f>
         <v>26155.129893520003</v>
       </c>
       <c r="W74" s="30">
@@ -5356,15 +6166,15 @@
         <v>24031.06875486</v>
       </c>
       <c r="X74" s="30">
-        <f t="shared" ref="X74:Y74" si="104">X73*X23</f>
+        <f t="shared" ref="X74:Y74" si="129">X73*X23</f>
         <v>21352.46996608</v>
       </c>
       <c r="Y74" s="30">
-        <f t="shared" si="104"/>
+        <f t="shared" si="129"/>
         <v>12613.844283390001</v>
       </c>
       <c r="AG74" s="30">
-        <f t="shared" ref="AG74" si="105">AG73*AG23</f>
+        <f t="shared" ref="AG74" si="130">AG73*AG23</f>
         <v>21801.299484439998</v>
       </c>
       <c r="AH74" s="30">
@@ -5377,7 +6187,7 @@
         <v>8</v>
       </c>
       <c r="V75" s="30">
-        <f t="shared" ref="V75" si="106">V74-V71</f>
+        <f t="shared" ref="V75" si="131">V74-V71</f>
         <v>25465.727893520001</v>
       </c>
       <c r="W75" s="30">
@@ -5385,15 +6195,15 @@
         <v>23339.734754860001</v>
       </c>
       <c r="X75" s="30">
-        <f t="shared" ref="X75:Y75" si="107">X74-X71</f>
+        <f t="shared" ref="X75:Y75" si="132">X74-X71</f>
         <v>20695.057966079999</v>
       </c>
       <c r="Y75" s="30">
-        <f t="shared" si="107"/>
+        <f t="shared" si="132"/>
         <v>11965.354283390001</v>
       </c>
       <c r="AG75" s="30">
-        <f t="shared" ref="AG75" si="108">AG74-AG71</f>
+        <f t="shared" ref="AG75" si="133">AG74-AG71</f>
         <v>21781.286484439999</v>
       </c>
       <c r="AH75" s="30">
@@ -5414,14 +6224,14 @@
         <v>35.713804049256993</v>
       </c>
       <c r="X77" s="40">
-        <f t="shared" ref="X77:Y77" si="109">X73/X67</f>
+        <f t="shared" ref="X77:Y77" si="134">X73/X67</f>
         <v>31.956738374301072</v>
       </c>
       <c r="Y77" s="40">
-        <f t="shared" si="109"/>
+        <f t="shared" si="134"/>
         <v>18.433692956105823</v>
       </c>
-      <c r="AG77" s="58" t="s">
+      <c r="AG77" s="48" t="s">
         <v>142</v>
       </c>
       <c r="AH77" s="40">
@@ -5434,15 +6244,15 @@
         <v>22</v>
       </c>
       <c r="V78" s="40">
-        <f t="shared" ref="V78:X78" si="110">V74/SUM(S6:V6)</f>
+        <f t="shared" ref="V78:X78" si="135">V74/SUM(S6:V6)</f>
         <v>29.93324409694867</v>
       </c>
       <c r="W78" s="40">
-        <f t="shared" si="110"/>
+        <f t="shared" si="135"/>
         <v>24.582176571414543</v>
       </c>
       <c r="X78" s="40">
-        <f t="shared" si="110"/>
+        <f t="shared" si="135"/>
         <v>19.725254796867233</v>
       </c>
       <c r="Y78" s="40">
@@ -5450,7 +6260,7 @@
         <v>10.606803677858297</v>
       </c>
       <c r="AG78" s="40">
-        <f t="shared" ref="AG78:AH78" si="111">AG74/AG6</f>
+        <f t="shared" ref="AG78" si="136">AG74/AG6</f>
         <v>36.927571198956599</v>
       </c>
       <c r="AH78" s="40">
@@ -5463,15 +6273,15 @@
         <v>23</v>
       </c>
       <c r="V79" s="40">
-        <f t="shared" ref="V79:X79" si="112">V75/SUM(S6:V6)</f>
+        <f t="shared" ref="V79:X79" si="137">V75/SUM(S6:V6)</f>
         <v>29.144257828062376</v>
       </c>
       <c r="W79" s="40">
-        <f t="shared" si="112"/>
+        <f t="shared" si="137"/>
         <v>23.874988113373725</v>
       </c>
       <c r="X79" s="40">
-        <f t="shared" si="112"/>
+        <f t="shared" si="137"/>
         <v>19.117942423773247</v>
       </c>
       <c r="Y79" s="40">
@@ -5479,7 +6289,7 @@
         <v>10.061497586985441</v>
       </c>
       <c r="AG79" s="40">
-        <f t="shared" ref="AG79:AH79" si="113">AG75/AG6</f>
+        <f t="shared" ref="AG79" si="138">AG75/AG6</f>
         <v>36.893672692909654</v>
       </c>
       <c r="AH79" s="40">
@@ -5492,15 +6302,15 @@
         <v>20</v>
       </c>
       <c r="V80" s="40">
-        <f t="shared" ref="V80" si="114">V73/SUM(S22:V22)</f>
+        <f t="shared" ref="V80" si="139">V73/SUM(S22:V22)</f>
         <v>-84.508678490299772</v>
       </c>
       <c r="W80" s="40">
-        <f t="shared" ref="W80:X80" si="115">W73/SUM(T22:W22)</f>
+        <f t="shared" ref="W80:X80" si="140">W73/SUM(T22:W22)</f>
         <v>-72.546524492411535</v>
       </c>
       <c r="X80" s="40">
-        <f t="shared" si="115"/>
+        <f t="shared" si="140"/>
         <v>-57.695906234315359</v>
       </c>
       <c r="Y80" s="40">
@@ -5508,7 +6318,7 @@
         <v>-33.274743486600045</v>
       </c>
       <c r="AG80" s="40">
-        <f t="shared" ref="AG80:AH80" si="116">AG73/AG22</f>
+        <f t="shared" ref="AG80" si="141">AG73/AG22</f>
         <v>-81.669936332863827</v>
       </c>
       <c r="AH80" s="40">

</xml_diff>

<commit_message>
Add headcounts to Software models
</commit_message>
<xml_diff>
--- a/$MDB.xlsx
+++ b/$MDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E500611-7006-4FAD-ACC9-3FCD685CF3C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAA9643-DFD6-4F23-B4BF-F8B471127D59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27435" windowHeight="11100" activeTab="1" xr2:uid="{A0DE9234-8F94-41AD-8663-2284C148F328}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27435" windowHeight="11100" xr2:uid="{A0DE9234-8F94-41AD-8663-2284C148F328}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="159">
   <si>
     <t>$MDB</t>
   </si>
@@ -494,6 +494,15 @@
   </si>
   <si>
     <t>FCF</t>
+  </si>
+  <si>
+    <t>Emply.</t>
+  </si>
+  <si>
+    <t>Non-Finance Metrics</t>
+  </si>
+  <si>
+    <t>Employees</t>
   </si>
 </sst>
 </file>
@@ -719,7 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -877,6 +886,12 @@
     <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -973,7 +988,7 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>108</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1023,7 +1038,7 @@
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1365,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A27B16A-4CA6-4CC0-B1CB-A0561C46DE09}">
   <dimension ref="A2:AB38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1523,7 +1538,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="12">
-        <f>'Financial Model'!Y69</f>
+        <f>'Financial Model'!Y72</f>
         <v>1787.5319999999999</v>
       </c>
       <c r="D9" s="10" t="str">
@@ -1558,7 +1573,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="12">
-        <f>'Financial Model'!Y70</f>
+        <f>'Financial Model'!Y73</f>
         <v>1139.0419999999999</v>
       </c>
       <c r="D10" s="10" t="str">
@@ -1924,8 +1939,13 @@
       <c r="Q25" s="17"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B26" s="14"/>
-      <c r="C26" s="72"/>
+      <c r="B26" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="86">
+        <f>'Financial Model'!AH35</f>
+        <v>3544</v>
+      </c>
       <c r="D26" s="73"/>
       <c r="G26" s="14"/>
       <c r="H26" s="16"/>
@@ -2046,7 +2066,7 @@
         <v>21</v>
       </c>
       <c r="C33" s="81">
-        <f>C6/'Financial Model'!Y67</f>
+        <f>C6/'Financial Model'!Y70</f>
         <v>19.311919490429393</v>
       </c>
       <c r="D33" s="82"/>
@@ -2196,13 +2216,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509F8013-A317-41E1-99F6-617E09116884}">
-  <dimension ref="B1:CV90"/>
+  <dimension ref="B1:CV93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="N64" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AF99" sqref="AF99"/>
+      <selection pane="bottomRight" activeCell="AH35" sqref="AH35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4562,1817 +4582,1838 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="36" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B36" s="37" t="s">
+    <row r="33" spans="2:35" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Z33" s="56"/>
+      <c r="AI33" s="56"/>
+    </row>
+    <row r="34" spans="2:35" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="83" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z34" s="56"/>
+      <c r="AI34" s="56"/>
+    </row>
+    <row r="35" spans="2:35" s="84" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="84" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z35" s="85"/>
+      <c r="AH35" s="84">
+        <v>3544</v>
+      </c>
+      <c r="AI35" s="85"/>
+    </row>
+    <row r="39" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B39" s="37" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="2" t="s">
+    <row r="40" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="V37" s="31">
+      <c r="V40" s="31">
         <v>473.904</v>
       </c>
-      <c r="W37" s="31">
+      <c r="W40" s="31">
         <v>456.27499999999998</v>
       </c>
-      <c r="X37" s="31">
+      <c r="X40" s="31">
         <v>651.41999999999996</v>
       </c>
-      <c r="Y37" s="31">
+      <c r="Y40" s="31">
         <v>999.67399999999998</v>
       </c>
-      <c r="Z37" s="53"/>
-      <c r="AG37" s="31">
+      <c r="Z40" s="53"/>
+      <c r="AG40" s="31">
         <v>429.697</v>
       </c>
-      <c r="AH37" s="31">
-        <f>V37</f>
+      <c r="AH40" s="31">
+        <f>V40</f>
         <v>473.904</v>
       </c>
-      <c r="AI37" s="52"/>
-    </row>
-    <row r="38" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="2" t="s">
+      <c r="AI40" s="52"/>
+    </row>
+    <row r="41" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="V38" s="31">
+      <c r="V41" s="31">
         <v>1352.019</v>
       </c>
-      <c r="W38" s="31">
+      <c r="W41" s="31">
         <v>1372.42</v>
       </c>
-      <c r="X38" s="31">
+      <c r="X41" s="31">
         <v>1144.192</v>
       </c>
-      <c r="Y38" s="31">
+      <c r="Y41" s="31">
         <v>787.85799999999995</v>
       </c>
-      <c r="Z38" s="53"/>
-      <c r="AG38" s="31">
+      <c r="Z41" s="53"/>
+      <c r="AG41" s="31">
         <v>528.04499999999996</v>
       </c>
-      <c r="AH38" s="31">
-        <f>V38</f>
+      <c r="AH41" s="31">
+        <f>V41</f>
         <v>1352.019</v>
       </c>
-      <c r="AI38" s="52"/>
-    </row>
-    <row r="39" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
+      <c r="AI41" s="52"/>
+    </row>
+    <row r="42" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="V39" s="30">
+      <c r="V42" s="30">
         <v>195.38300000000001</v>
       </c>
-      <c r="W39" s="30">
+      <c r="W42" s="30">
         <v>164.88499999999999</v>
       </c>
-      <c r="X39" s="30">
+      <c r="X42" s="30">
         <v>213.267</v>
       </c>
-      <c r="Y39" s="30">
+      <c r="Y42" s="30">
         <v>231.26</v>
       </c>
-      <c r="AG39" s="30">
+      <c r="AG42" s="30">
         <v>135.17599999999999</v>
       </c>
-      <c r="AH39" s="30">
-        <f>V39</f>
+      <c r="AH42" s="30">
+        <f>V42</f>
         <v>195.38300000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
+    <row r="43" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="V40" s="30">
+      <c r="V43" s="30">
         <v>63.523000000000003</v>
       </c>
-      <c r="W40" s="30">
+      <c r="W43" s="30">
         <v>66.754000000000005</v>
       </c>
-      <c r="X40" s="30">
+      <c r="X43" s="30">
         <v>72.069000000000003</v>
       </c>
-      <c r="Y40" s="30">
+      <c r="Y43" s="30">
         <v>77.445999999999998</v>
       </c>
-      <c r="AG40" s="30">
+      <c r="AG43" s="30">
         <v>36.619</v>
       </c>
-      <c r="AH40" s="30">
-        <f t="shared" ref="AH40:AH47" si="79">V40</f>
+      <c r="AH43" s="30">
+        <f t="shared" ref="AH43:AH50" si="79">V43</f>
         <v>63.523000000000003</v>
       </c>
     </row>
-    <row r="41" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
+    <row r="44" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="V41" s="30">
+      <c r="V44" s="30">
         <v>32.573</v>
       </c>
-      <c r="W41" s="30">
+      <c r="W44" s="30">
         <v>35.972999999999999</v>
       </c>
-      <c r="X41" s="30">
+      <c r="X44" s="30">
         <v>27.565999999999999</v>
       </c>
-      <c r="Y41" s="30">
+      <c r="Y44" s="30">
         <v>26.016999999999999</v>
       </c>
-      <c r="AG41" s="30">
+      <c r="AG44" s="30">
         <v>12.35</v>
       </c>
-      <c r="AH41" s="30">
+      <c r="AH44" s="30">
         <f t="shared" si="79"/>
         <v>32.573</v>
       </c>
     </row>
-    <row r="42" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
+    <row r="45" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="30">
-        <f t="shared" ref="C42:V42" si="80">SUM(C37:C41)</f>
-        <v>0</v>
-      </c>
-      <c r="D42" s="30">
+      <c r="C45" s="30">
+        <f t="shared" ref="C45:V45" si="80">SUM(C40:C44)</f>
+        <v>0</v>
+      </c>
+      <c r="D45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="E42" s="30">
+      <c r="E45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="F42" s="30">
+      <c r="F45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="G42" s="30">
+      <c r="G45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="H42" s="30">
+      <c r="H45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="I42" s="30">
+      <c r="I45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="J42" s="30">
+      <c r="J45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="K42" s="30">
+      <c r="K45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="L42" s="30">
+      <c r="L45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="M42" s="30">
+      <c r="M45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="N42" s="30">
+      <c r="N45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="O42" s="30">
+      <c r="O45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="P42" s="30">
+      <c r="P45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="Q42" s="30">
+      <c r="Q45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="R42" s="30">
+      <c r="R45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="S42" s="30">
+      <c r="S45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="T42" s="30">
+      <c r="T45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="U42" s="30">
+      <c r="U45" s="30">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="V42" s="30">
+      <c r="V45" s="30">
         <f t="shared" si="80"/>
         <v>2117.402</v>
       </c>
-      <c r="W42" s="30">
-        <f>SUM(W37:W41)</f>
+      <c r="W45" s="30">
+        <f>SUM(W40:W44)</f>
         <v>2096.3070000000002</v>
       </c>
-      <c r="X42" s="30">
-        <f t="shared" ref="X42:Y42" si="81">SUM(X37:X41)</f>
+      <c r="X45" s="30">
+        <f t="shared" ref="X45:Y45" si="81">SUM(X40:X44)</f>
         <v>2108.5140000000001</v>
       </c>
-      <c r="Y42" s="30">
+      <c r="Y45" s="30">
         <f t="shared" si="81"/>
         <v>2122.2549999999997</v>
       </c>
-      <c r="AG42" s="30">
-        <f t="shared" ref="AG42:AH42" si="82">SUM(AG37:AG41)</f>
+      <c r="AG45" s="30">
+        <f t="shared" ref="AG45:AH45" si="82">SUM(AG40:AG44)</f>
         <v>1141.8869999999997</v>
       </c>
-      <c r="AH42" s="30">
+      <c r="AH45" s="30">
         <f t="shared" si="82"/>
         <v>2117.402</v>
       </c>
     </row>
-    <row r="43" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
+    <row r="46" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="V43" s="30">
+      <c r="V46" s="30">
         <v>62.625</v>
       </c>
-      <c r="W43" s="30">
+      <c r="W46" s="30">
         <v>62.761000000000003</v>
       </c>
-      <c r="X43" s="30">
+      <c r="X46" s="30">
         <v>61.603999999999999</v>
       </c>
-      <c r="Y43" s="30">
+      <c r="Y46" s="30">
         <v>59.488999999999997</v>
       </c>
-      <c r="AG43" s="30">
+      <c r="AG46" s="30">
         <v>62.363999999999997</v>
       </c>
-      <c r="AH43" s="30">
+      <c r="AH46" s="30">
         <f t="shared" si="79"/>
         <v>62.625</v>
       </c>
     </row>
-    <row r="44" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
+    <row r="47" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="V44" s="30">
+      <c r="V47" s="30">
         <v>41.744999999999997</v>
       </c>
-      <c r="W44" s="30">
+      <c r="W47" s="30">
         <v>45.247999999999998</v>
       </c>
-      <c r="X44" s="30">
+      <c r="X47" s="30">
         <v>46.417999999999999</v>
       </c>
-      <c r="Y44" s="30">
+      <c r="Y47" s="30">
         <v>43.484999999999999</v>
       </c>
-      <c r="AG44" s="30">
+      <c r="AG47" s="30">
         <v>34.587000000000003</v>
       </c>
-      <c r="AH44" s="30">
+      <c r="AH47" s="30">
         <f t="shared" si="79"/>
         <v>41.744999999999997</v>
       </c>
     </row>
-    <row r="45" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
+    <row r="48" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="V45" s="30">
+      <c r="V48" s="30">
         <f>57.775+20.608</f>
         <v>78.382999999999996</v>
       </c>
-      <c r="W45" s="30">
+      <c r="W48" s="30">
         <f>57.775+18.313</f>
         <v>76.087999999999994</v>
       </c>
-      <c r="X45" s="30">
+      <c r="X48" s="30">
         <f>16.018+57.779</f>
         <v>73.796999999999997</v>
       </c>
-      <c r="Y45" s="30">
+      <c r="Y48" s="30">
         <f>57.779+13.723</f>
         <v>71.50200000000001</v>
       </c>
-      <c r="AG45" s="30">
+      <c r="AG48" s="30">
         <f>55.83+26.275</f>
         <v>82.10499999999999</v>
       </c>
-      <c r="AH45" s="30">
+      <c r="AH48" s="30">
         <f t="shared" si="79"/>
         <v>78.382999999999996</v>
       </c>
     </row>
-    <row r="46" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
+    <row r="49" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="V46" s="30">
+      <c r="V49" s="30">
         <v>1.9390000000000001</v>
       </c>
-      <c r="W46" s="30">
+      <c r="W49" s="30">
         <v>1.9630000000000001</v>
       </c>
-      <c r="X46" s="30">
+      <c r="X49" s="30">
         <v>2.1629999999999998</v>
       </c>
-      <c r="Y46" s="30">
+      <c r="Y49" s="30">
         <v>1.657</v>
       </c>
-      <c r="AG46" s="30">
+      <c r="AG49" s="30">
         <v>0.997</v>
       </c>
-      <c r="AH46" s="30">
+      <c r="AH49" s="30">
         <f t="shared" si="79"/>
         <v>1.9390000000000001</v>
       </c>
     </row>
-    <row r="47" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
+    <row r="50" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="V47" s="30">
+      <c r="V50" s="30">
         <v>147.494</v>
       </c>
-      <c r="W47" s="30">
+      <c r="W50" s="30">
         <v>152.17400000000001</v>
       </c>
-      <c r="X47" s="30">
+      <c r="X50" s="30">
         <v>159.102</v>
       </c>
-      <c r="Y47" s="30">
+      <c r="Y50" s="30">
         <v>168.798</v>
       </c>
-      <c r="AG47" s="30">
+      <c r="AG50" s="30">
         <v>85.555000000000007</v>
       </c>
-      <c r="AH47" s="30">
+      <c r="AH50" s="30">
         <f t="shared" si="79"/>
         <v>147.494</v>
       </c>
     </row>
-    <row r="48" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
+    <row r="51" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C48" s="30">
-        <f t="shared" ref="C48:V48" si="83">C42+SUM(C43:C47)</f>
-        <v>0</v>
-      </c>
-      <c r="D48" s="30">
+      <c r="C51" s="30">
+        <f t="shared" ref="C51:V51" si="83">C45+SUM(C46:C50)</f>
+        <v>0</v>
+      </c>
+      <c r="D51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="E48" s="30">
+      <c r="E51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="F48" s="30">
+      <c r="F51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="G48" s="30">
+      <c r="G51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="H48" s="30">
+      <c r="H51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="I48" s="30">
+      <c r="I51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="J48" s="30">
+      <c r="J51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="K48" s="30">
+      <c r="K51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="L48" s="30">
+      <c r="L51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="M48" s="30">
+      <c r="M51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="N48" s="30">
+      <c r="N51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="O48" s="30">
+      <c r="O51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="P48" s="30">
+      <c r="P51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="Q48" s="30">
+      <c r="Q51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="R48" s="30">
+      <c r="R51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="S48" s="30">
+      <c r="S51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="T48" s="30">
+      <c r="T51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="U48" s="30">
+      <c r="U51" s="30">
         <f t="shared" si="83"/>
         <v>0</v>
       </c>
-      <c r="V48" s="30">
+      <c r="V51" s="30">
         <f t="shared" si="83"/>
         <v>2449.5880000000002</v>
       </c>
-      <c r="W48" s="30">
-        <f>W42+SUM(W43:W47)</f>
+      <c r="W51" s="30">
+        <f>W45+SUM(W46:W50)</f>
         <v>2434.5410000000002</v>
       </c>
-      <c r="X48" s="30">
-        <f>X42+SUM(X43:X47)</f>
+      <c r="X51" s="30">
+        <f>X45+SUM(X46:X50)</f>
         <v>2451.598</v>
       </c>
-      <c r="Y48" s="30">
-        <f>Y42+SUM(Y43:Y47)</f>
+      <c r="Y51" s="30">
+        <f>Y45+SUM(Y46:Y50)</f>
         <v>2467.1859999999997</v>
       </c>
-      <c r="AG48" s="30">
-        <f>AG42+SUM(AG43:AG47)</f>
+      <c r="AG51" s="30">
+        <f>AG45+SUM(AG46:AG50)</f>
         <v>1407.4949999999997</v>
       </c>
-      <c r="AH48" s="30">
-        <f>AH42+SUM(AH43:AH47)</f>
+      <c r="AH51" s="30">
+        <f>AH45+SUM(AH46:AH50)</f>
         <v>2449.5880000000002</v>
       </c>
     </row>
-    <row r="50" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B50" s="1" t="s">
+    <row r="53" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="V50" s="30">
+      <c r="V53" s="30">
         <v>5.234</v>
       </c>
-      <c r="W50" s="30">
+      <c r="W53" s="30">
         <v>6.2039999999999997</v>
       </c>
-      <c r="X50" s="30">
+      <c r="X53" s="30">
         <v>7.3029999999999999</v>
       </c>
-      <c r="Y50" s="30">
+      <c r="Y53" s="30">
         <v>7.734</v>
       </c>
-      <c r="AG50" s="30">
+      <c r="AG53" s="30">
         <v>4.1440000000000001</v>
       </c>
-      <c r="AH50" s="30">
-        <f>V50</f>
+      <c r="AH53" s="30">
+        <f>V53</f>
         <v>5.234</v>
       </c>
     </row>
-    <row r="51" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B51" s="1" t="s">
+    <row r="54" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="V51" s="30">
+      <c r="V54" s="30">
         <v>112.568</v>
       </c>
-      <c r="W51" s="30">
+      <c r="W54" s="30">
         <v>87.716999999999999</v>
       </c>
-      <c r="X51" s="30">
+      <c r="X54" s="30">
         <v>83.805999999999997</v>
       </c>
-      <c r="Y51" s="30">
+      <c r="Y54" s="30">
         <v>84.442999999999998</v>
       </c>
-      <c r="AG51" s="30">
+      <c r="AG54" s="30">
         <v>70.209999999999994</v>
       </c>
-      <c r="AH51" s="30">
-        <f t="shared" ref="AH51:AH54" si="84">V51</f>
+      <c r="AH54" s="30">
+        <f t="shared" ref="AH54:AH57" si="84">V54</f>
         <v>112.568</v>
       </c>
     </row>
-    <row r="52" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B52" s="1" t="s">
+    <row r="55" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="V52" s="30">
+      <c r="V55" s="30">
         <v>8.0839999999999996</v>
       </c>
-      <c r="W52" s="30">
+      <c r="W55" s="30">
         <v>8.6709999999999994</v>
       </c>
-      <c r="X52" s="30">
+      <c r="X55" s="30">
         <v>9.1630000000000003</v>
       </c>
-      <c r="Y52" s="30">
+      <c r="Y55" s="30">
         <v>8.6449999999999996</v>
       </c>
-      <c r="AG52" s="30">
+      <c r="AG55" s="30">
         <v>2.343</v>
       </c>
-      <c r="AH52" s="30">
+      <c r="AH55" s="30">
         <f t="shared" si="84"/>
         <v>8.0839999999999996</v>
       </c>
     </row>
-    <row r="53" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B53" s="1" t="s">
+    <row r="56" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="V53" s="30">
+      <c r="V56" s="30">
         <v>48.847999999999999</v>
       </c>
-      <c r="W53" s="30">
+      <c r="W56" s="30">
         <v>49.216000000000001</v>
       </c>
-      <c r="X53" s="30">
+      <c r="X56" s="30">
         <v>73.915999999999997</v>
       </c>
-      <c r="Y53" s="30">
+      <c r="Y56" s="30">
         <v>52.826000000000001</v>
       </c>
-      <c r="AG53" s="30">
+      <c r="AG56" s="30">
         <v>56.44</v>
       </c>
-      <c r="AH53" s="30">
+      <c r="AH56" s="30">
         <f t="shared" si="84"/>
         <v>48.847999999999999</v>
       </c>
     </row>
-    <row r="54" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B54" s="1" t="s">
+    <row r="57" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="V54" s="30">
+      <c r="V57" s="30">
         <v>352.00099999999998</v>
       </c>
-      <c r="W54" s="30">
+      <c r="W57" s="30">
         <v>351.91399999999999</v>
       </c>
-      <c r="X54" s="30">
+      <c r="X57" s="30">
         <v>350.709</v>
       </c>
-      <c r="Y54" s="30">
+      <c r="Y57" s="30">
         <v>364.15899999999999</v>
       </c>
-      <c r="AG54" s="30">
+      <c r="AG57" s="30">
         <v>221.404</v>
       </c>
-      <c r="AH54" s="30">
+      <c r="AH57" s="30">
         <f t="shared" si="84"/>
         <v>352.00099999999998</v>
       </c>
     </row>
-    <row r="55" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B55" s="1" t="s">
+    <row r="58" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C55" s="30">
-        <f t="shared" ref="C55:V55" si="85">SUM(C50:C54)</f>
-        <v>0</v>
-      </c>
-      <c r="D55" s="30">
+      <c r="C58" s="30">
+        <f t="shared" ref="C58:V58" si="85">SUM(C53:C57)</f>
+        <v>0</v>
+      </c>
+      <c r="D58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="E55" s="30">
+      <c r="E58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="F55" s="30">
+      <c r="F58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="G55" s="30">
+      <c r="G58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="H55" s="30">
+      <c r="H58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="I55" s="30">
+      <c r="I58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="J55" s="30">
+      <c r="J58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="K55" s="30">
+      <c r="K58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="L55" s="30">
+      <c r="L58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="M55" s="30">
+      <c r="M58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="N55" s="30">
+      <c r="N58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="O55" s="30">
+      <c r="O58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="P55" s="30">
+      <c r="P58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="Q55" s="30">
+      <c r="Q58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="R55" s="30">
+      <c r="R58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="S55" s="30">
+      <c r="S58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="T55" s="30">
+      <c r="T58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="U55" s="30">
+      <c r="U58" s="30">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="V55" s="30">
+      <c r="V58" s="30">
         <f t="shared" si="85"/>
         <v>526.7349999999999</v>
       </c>
-      <c r="W55" s="30">
-        <f>SUM(W50:W54)</f>
+      <c r="W58" s="30">
+        <f>SUM(W53:W57)</f>
         <v>503.72199999999998</v>
       </c>
-      <c r="X55" s="30">
-        <f>SUM(X50:X54)</f>
+      <c r="X58" s="30">
+        <f>SUM(X53:X57)</f>
         <v>524.89699999999993</v>
       </c>
-      <c r="Y55" s="30">
-        <f>SUM(Y50:Y54)</f>
+      <c r="Y58" s="30">
+        <f>SUM(Y53:Y57)</f>
         <v>517.80700000000002</v>
       </c>
-      <c r="AG55" s="30">
-        <f>SUM(AG50:AG54)</f>
+      <c r="AG58" s="30">
+        <f>SUM(AG53:AG57)</f>
         <v>354.541</v>
       </c>
-      <c r="AH55" s="30">
-        <f>SUM(AH50:AH54)</f>
+      <c r="AH58" s="30">
+        <f>SUM(AH53:AH57)</f>
         <v>526.7349999999999</v>
       </c>
     </row>
-    <row r="56" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B56" s="1" t="s">
+    <row r="59" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="V56" s="30">
+      <c r="V59" s="30">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="W56" s="30">
+      <c r="W59" s="30">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="X56" s="30">
+      <c r="X59" s="30">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="Y56" s="30">
+      <c r="Y59" s="30">
         <v>0.40600000000000003</v>
       </c>
-      <c r="AG56" s="30">
+      <c r="AG59" s="30">
         <v>0.77300000000000002</v>
       </c>
-      <c r="AH56" s="30">
-        <f>W56</f>
+      <c r="AH59" s="30">
+        <f>W59</f>
         <v>9.2999999999999999E-2</v>
       </c>
-    </row>
-    <row r="57" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B57" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="V57" s="30">
-        <v>38.707000000000001</v>
-      </c>
-      <c r="W57" s="30">
-        <v>40.279000000000003</v>
-      </c>
-      <c r="X57" s="30">
-        <v>40.436999999999998</v>
-      </c>
-      <c r="Y57" s="30">
-        <v>37.261000000000003</v>
-      </c>
-      <c r="AG57" s="30">
-        <v>39.094999999999999</v>
-      </c>
-      <c r="AH57" s="30">
-        <f>V57</f>
-        <v>38.707000000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B58" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="V58" s="30">
-        <v>23.178999999999998</v>
-      </c>
-      <c r="W58" s="30">
-        <v>23.555</v>
-      </c>
-      <c r="X58" s="30">
-        <v>24.462</v>
-      </c>
-      <c r="Y58" s="30">
-        <v>34.014000000000003</v>
-      </c>
-      <c r="AG58" s="30">
-        <v>16.547000000000001</v>
-      </c>
-      <c r="AH58" s="30">
-        <f t="shared" ref="AH58" si="86">V58</f>
-        <v>23.178999999999998</v>
-      </c>
-    </row>
-    <row r="59" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="V59" s="31">
-        <v>1136.521</v>
-      </c>
-      <c r="W59" s="31">
-        <v>1137.3610000000001</v>
-      </c>
-      <c r="X59" s="31">
-        <v>1138.2</v>
-      </c>
-      <c r="Y59" s="31">
-        <v>1139.0419999999999</v>
-      </c>
-      <c r="Z59" s="53"/>
-      <c r="AG59" s="31">
-        <v>937.72900000000004</v>
-      </c>
-      <c r="AH59" s="31">
-        <f>V59</f>
-        <v>1136.521</v>
-      </c>
-      <c r="AI59" s="52"/>
     </row>
     <row r="60" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V60" s="30">
-        <v>57.664999999999999</v>
-      </c>
-      <c r="W60" s="31">
-        <v>56.652000000000001</v>
+        <v>38.707000000000001</v>
+      </c>
+      <c r="W60" s="30">
+        <v>40.279000000000003</v>
       </c>
       <c r="X60" s="30">
-        <v>55.338999999999999</v>
+        <v>40.436999999999998</v>
       </c>
       <c r="Y60" s="30">
-        <v>54.374000000000002</v>
+        <v>37.261000000000003</v>
       </c>
       <c r="AG60" s="30">
-        <v>59.128999999999998</v>
+        <v>39.094999999999999</v>
       </c>
       <c r="AH60" s="30">
-        <f t="shared" ref="AH60" si="87">V60</f>
-        <v>57.664999999999999</v>
+        <f>V60</f>
+        <v>38.707000000000001</v>
       </c>
     </row>
     <row r="61" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="V61" s="30">
+        <v>23.178999999999998</v>
+      </c>
+      <c r="W61" s="30">
+        <v>23.555</v>
+      </c>
+      <c r="X61" s="30">
+        <v>24.462</v>
+      </c>
+      <c r="Y61" s="30">
+        <v>34.014000000000003</v>
+      </c>
+      <c r="AG61" s="30">
+        <v>16.547000000000001</v>
+      </c>
+      <c r="AH61" s="30">
+        <f t="shared" ref="AH61" si="86">V61</f>
+        <v>23.178999999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="V62" s="31">
+        <v>1136.521</v>
+      </c>
+      <c r="W62" s="31">
+        <v>1137.3610000000001</v>
+      </c>
+      <c r="X62" s="31">
+        <v>1138.2</v>
+      </c>
+      <c r="Y62" s="31">
+        <v>1139.0419999999999</v>
+      </c>
+      <c r="Z62" s="53"/>
+      <c r="AG62" s="31">
+        <v>937.72900000000004</v>
+      </c>
+      <c r="AH62" s="31">
+        <f>V62</f>
+        <v>1136.521</v>
+      </c>
+      <c r="AI62" s="52"/>
+    </row>
+    <row r="63" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B63" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="V63" s="30">
+        <v>57.664999999999999</v>
+      </c>
+      <c r="W63" s="31">
+        <v>56.652000000000001</v>
+      </c>
+      <c r="X63" s="30">
+        <v>55.338999999999999</v>
+      </c>
+      <c r="Y63" s="30">
+        <v>54.374000000000002</v>
+      </c>
+      <c r="AG63" s="30">
+        <v>59.128999999999998</v>
+      </c>
+      <c r="AH63" s="30">
+        <f t="shared" ref="AH63" si="87">V63</f>
+        <v>57.664999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B64" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C61" s="30">
-        <f t="shared" ref="C61:V61" si="88">C55+SUM(C56:C60)</f>
-        <v>0</v>
-      </c>
-      <c r="D61" s="30">
+      <c r="C64" s="30">
+        <f t="shared" ref="C64:V64" si="88">C58+SUM(C59:C63)</f>
+        <v>0</v>
+      </c>
+      <c r="D64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="E61" s="30">
+      <c r="E64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="F61" s="30">
+      <c r="F64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="G61" s="30">
+      <c r="G64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="H61" s="30">
+      <c r="H64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="I61" s="30">
+      <c r="I64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="J61" s="30">
+      <c r="J64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="K61" s="30">
+      <c r="K64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="L61" s="30">
+      <c r="L64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="M61" s="30">
+      <c r="M64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="N61" s="30">
+      <c r="N64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="O61" s="30">
+      <c r="O64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="P61" s="30">
+      <c r="P64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="Q61" s="30">
+      <c r="Q64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="R61" s="30">
+      <c r="R64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="S61" s="30">
+      <c r="S64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="T61" s="30">
+      <c r="T64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="U61" s="30">
+      <c r="U64" s="30">
         <f t="shared" si="88"/>
         <v>0</v>
       </c>
-      <c r="V61" s="30">
+      <c r="V64" s="30">
         <f t="shared" si="88"/>
         <v>1782.8879999999999</v>
       </c>
-      <c r="W61" s="30">
-        <f>W55+SUM(W56:W60)</f>
+      <c r="W64" s="30">
+        <f>W58+SUM(W59:W63)</f>
         <v>1761.662</v>
       </c>
-      <c r="X61" s="30">
-        <f>X55+SUM(X56:X60)</f>
+      <c r="X64" s="30">
+        <f>X58+SUM(X59:X63)</f>
         <v>1783.4299999999998</v>
       </c>
-      <c r="Y61" s="30">
-        <f>Y55+SUM(Y56:Y60)</f>
+      <c r="Y64" s="30">
+        <f>Y58+SUM(Y59:Y63)</f>
         <v>1782.904</v>
       </c>
-      <c r="AG61" s="30">
-        <f>AG55+SUM(AG56:AG60)</f>
+      <c r="AG64" s="30">
+        <f>AG58+SUM(AG59:AG63)</f>
         <v>1407.8139999999999</v>
       </c>
-      <c r="AH61" s="30">
-        <f>AH55+SUM(AH56:AH60)</f>
+      <c r="AH64" s="30">
+        <f>AH58+SUM(AH59:AH63)</f>
         <v>1782.8999999999999</v>
       </c>
     </row>
-    <row r="63" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B63" s="1" t="s">
+    <row r="66" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B66" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="V63" s="1">
+      <c r="V66" s="1">
         <v>666.7</v>
       </c>
-      <c r="W63" s="30">
+      <c r="W66" s="30">
         <v>672.87900000000002</v>
       </c>
-      <c r="X63" s="30">
+      <c r="X66" s="30">
         <v>668.16800000000001</v>
       </c>
-      <c r="Y63" s="30">
+      <c r="Y66" s="30">
         <v>684.28200000000004</v>
       </c>
-      <c r="AG63" s="1">
+      <c r="AG66" s="1">
         <v>-5.0330000000000004</v>
       </c>
-      <c r="AH63" s="1">
-        <f>V63</f>
+      <c r="AH66" s="1">
+        <f>V66</f>
         <v>666.7</v>
       </c>
     </row>
-    <row r="64" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B64" s="1" t="s">
+    <row r="67" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B67" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C64" s="30">
-        <f t="shared" ref="C64" si="89">C63+C61</f>
-        <v>0</v>
-      </c>
-      <c r="D64" s="30">
-        <f t="shared" ref="D64" si="90">D63+D61</f>
-        <v>0</v>
-      </c>
-      <c r="E64" s="30">
-        <f t="shared" ref="E64" si="91">E63+E61</f>
-        <v>0</v>
-      </c>
-      <c r="F64" s="30">
-        <f t="shared" ref="F64" si="92">F63+F61</f>
-        <v>0</v>
-      </c>
-      <c r="G64" s="30">
-        <f t="shared" ref="G64" si="93">G63+G61</f>
-        <v>0</v>
-      </c>
-      <c r="H64" s="30">
-        <f t="shared" ref="H64" si="94">H63+H61</f>
-        <v>0</v>
-      </c>
-      <c r="I64" s="30">
-        <f t="shared" ref="I64" si="95">I63+I61</f>
-        <v>0</v>
-      </c>
-      <c r="J64" s="30">
-        <f t="shared" ref="J64" si="96">J63+J61</f>
-        <v>0</v>
-      </c>
-      <c r="K64" s="30">
-        <f t="shared" ref="K64" si="97">K63+K61</f>
-        <v>0</v>
-      </c>
-      <c r="L64" s="30">
-        <f t="shared" ref="L64" si="98">L63+L61</f>
-        <v>0</v>
-      </c>
-      <c r="M64" s="30">
-        <f t="shared" ref="M64" si="99">M63+M61</f>
-        <v>0</v>
-      </c>
-      <c r="N64" s="30">
-        <f t="shared" ref="N64" si="100">N63+N61</f>
-        <v>0</v>
-      </c>
-      <c r="O64" s="30">
-        <f t="shared" ref="O64" si="101">O63+O61</f>
-        <v>0</v>
-      </c>
-      <c r="P64" s="30">
-        <f t="shared" ref="P64" si="102">P63+P61</f>
-        <v>0</v>
-      </c>
-      <c r="Q64" s="30">
-        <f t="shared" ref="Q64" si="103">Q63+Q61</f>
-        <v>0</v>
-      </c>
-      <c r="R64" s="30">
-        <f t="shared" ref="R64" si="104">R63+R61</f>
-        <v>0</v>
-      </c>
-      <c r="S64" s="30">
-        <f t="shared" ref="S64" si="105">S63+S61</f>
-        <v>0</v>
-      </c>
-      <c r="T64" s="30">
-        <f t="shared" ref="T64" si="106">T63+T61</f>
-        <v>0</v>
-      </c>
-      <c r="U64" s="30">
-        <f t="shared" ref="U64" si="107">U63+U61</f>
-        <v>0</v>
-      </c>
-      <c r="V64" s="30">
-        <f t="shared" ref="V64" si="108">V63+V61</f>
+      <c r="C67" s="30">
+        <f t="shared" ref="C67" si="89">C66+C64</f>
+        <v>0</v>
+      </c>
+      <c r="D67" s="30">
+        <f t="shared" ref="D67" si="90">D66+D64</f>
+        <v>0</v>
+      </c>
+      <c r="E67" s="30">
+        <f t="shared" ref="E67" si="91">E66+E64</f>
+        <v>0</v>
+      </c>
+      <c r="F67" s="30">
+        <f t="shared" ref="F67" si="92">F66+F64</f>
+        <v>0</v>
+      </c>
+      <c r="G67" s="30">
+        <f t="shared" ref="G67" si="93">G66+G64</f>
+        <v>0</v>
+      </c>
+      <c r="H67" s="30">
+        <f t="shared" ref="H67" si="94">H66+H64</f>
+        <v>0</v>
+      </c>
+      <c r="I67" s="30">
+        <f t="shared" ref="I67" si="95">I66+I64</f>
+        <v>0</v>
+      </c>
+      <c r="J67" s="30">
+        <f t="shared" ref="J67" si="96">J66+J64</f>
+        <v>0</v>
+      </c>
+      <c r="K67" s="30">
+        <f t="shared" ref="K67" si="97">K66+K64</f>
+        <v>0</v>
+      </c>
+      <c r="L67" s="30">
+        <f t="shared" ref="L67" si="98">L66+L64</f>
+        <v>0</v>
+      </c>
+      <c r="M67" s="30">
+        <f t="shared" ref="M67" si="99">M66+M64</f>
+        <v>0</v>
+      </c>
+      <c r="N67" s="30">
+        <f t="shared" ref="N67" si="100">N66+N64</f>
+        <v>0</v>
+      </c>
+      <c r="O67" s="30">
+        <f t="shared" ref="O67" si="101">O66+O64</f>
+        <v>0</v>
+      </c>
+      <c r="P67" s="30">
+        <f t="shared" ref="P67" si="102">P66+P64</f>
+        <v>0</v>
+      </c>
+      <c r="Q67" s="30">
+        <f t="shared" ref="Q67" si="103">Q66+Q64</f>
+        <v>0</v>
+      </c>
+      <c r="R67" s="30">
+        <f t="shared" ref="R67" si="104">R66+R64</f>
+        <v>0</v>
+      </c>
+      <c r="S67" s="30">
+        <f t="shared" ref="S67" si="105">S66+S64</f>
+        <v>0</v>
+      </c>
+      <c r="T67" s="30">
+        <f t="shared" ref="T67" si="106">T66+T64</f>
+        <v>0</v>
+      </c>
+      <c r="U67" s="30">
+        <f t="shared" ref="U67" si="107">U66+U64</f>
+        <v>0</v>
+      </c>
+      <c r="V67" s="30">
+        <f t="shared" ref="V67" si="108">V66+V64</f>
         <v>2449.5879999999997</v>
       </c>
-      <c r="W64" s="30">
-        <f t="shared" ref="W64:Y64" si="109">W63+W61</f>
+      <c r="W67" s="30">
+        <f t="shared" ref="W67:Y67" si="109">W66+W64</f>
         <v>2434.5410000000002</v>
       </c>
-      <c r="X64" s="30">
-        <f t="shared" ref="X64" si="110">X63+X61</f>
+      <c r="X67" s="30">
+        <f t="shared" ref="X67" si="110">X66+X64</f>
         <v>2451.598</v>
       </c>
-      <c r="Y64" s="30">
+      <c r="Y67" s="30">
         <f t="shared" si="109"/>
         <v>2467.1860000000001</v>
       </c>
-      <c r="AF64" s="47"/>
-      <c r="AG64" s="30">
-        <f>AG63+AG61</f>
+      <c r="AF67" s="47"/>
+      <c r="AG67" s="30">
+        <f>AG66+AG64</f>
         <v>1402.7809999999999</v>
       </c>
-      <c r="AH64" s="30">
-        <f t="shared" ref="AH64" si="111">AH63+AH61</f>
+      <c r="AH67" s="30">
+        <f t="shared" ref="AH67" si="111">AH66+AH64</f>
         <v>2449.6</v>
       </c>
     </row>
-    <row r="65" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="AF65" s="47"/>
-    </row>
-    <row r="66" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B66" s="1" t="s">
+    <row r="68" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AF68" s="47"/>
+    </row>
+    <row r="69" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B69" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C66" s="30">
-        <f t="shared" ref="C66:V66" si="112">C48-C61</f>
-        <v>0</v>
-      </c>
-      <c r="D66" s="30">
+      <c r="C69" s="30">
+        <f t="shared" ref="C69:V69" si="112">C51-C64</f>
+        <v>0</v>
+      </c>
+      <c r="D69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="E66" s="30">
+      <c r="E69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="F66" s="30">
+      <c r="F69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="G66" s="30">
+      <c r="G69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="H66" s="30">
+      <c r="H69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="I66" s="30">
+      <c r="I69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="J66" s="30">
+      <c r="J69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="K66" s="30">
+      <c r="K69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="L66" s="30">
+      <c r="L69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="M66" s="30">
+      <c r="M69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="N66" s="30">
+      <c r="N69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="O66" s="30">
+      <c r="O69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="P66" s="30">
+      <c r="P69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="Q66" s="30">
+      <c r="Q69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="R66" s="30">
+      <c r="R69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="S66" s="30">
+      <c r="S69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="T66" s="30">
+      <c r="T69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="U66" s="30">
+      <c r="U69" s="30">
         <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="V66" s="30">
+      <c r="V69" s="30">
         <f t="shared" si="112"/>
         <v>666.70000000000027</v>
       </c>
-      <c r="W66" s="30">
-        <f>W48-W61</f>
+      <c r="W69" s="30">
+        <f>W51-W64</f>
         <v>672.87900000000013</v>
       </c>
-      <c r="X66" s="30">
-        <f t="shared" ref="X66:Y66" si="113">X48-X61</f>
+      <c r="X69" s="30">
+        <f t="shared" ref="X69:Y69" si="113">X51-X64</f>
         <v>668.16800000000012</v>
       </c>
-      <c r="Y66" s="30">
+      <c r="Y69" s="30">
         <f t="shared" si="113"/>
         <v>684.2819999999997</v>
       </c>
-      <c r="AF66" s="47"/>
-      <c r="AG66" s="30">
-        <f t="shared" ref="AG66:AH66" si="114">AG48-AG61</f>
+      <c r="AF69" s="47"/>
+      <c r="AG69" s="30">
+        <f t="shared" ref="AG69:AH69" si="114">AG51-AG64</f>
         <v>-0.31900000000018736</v>
       </c>
-      <c r="AH66" s="30">
+      <c r="AH69" s="30">
         <f t="shared" si="114"/>
         <v>666.68800000000033</v>
       </c>
     </row>
-    <row r="67" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B67" s="1" t="s">
+    <row r="70" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B70" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C67" s="1" t="e">
-        <f t="shared" ref="C67:U67" si="115">C66/C23</f>
+      <c r="C70" s="1" t="e">
+        <f t="shared" ref="C70:U70" si="115">C69/C23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D67" s="1" t="e">
+      <c r="D70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E67" s="1" t="e">
+      <c r="E70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F67" s="1" t="e">
+      <c r="F70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G67" s="1" t="e">
+      <c r="G70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H67" s="1" t="e">
+      <c r="H70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I67" s="1" t="e">
+      <c r="I70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J67" s="1" t="e">
+      <c r="J70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K67" s="1" t="e">
+      <c r="K70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L67" s="1" t="e">
+      <c r="L70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M67" s="1" t="e">
+      <c r="M70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N67" s="1" t="e">
+      <c r="N70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O67" s="1" t="e">
+      <c r="O70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P67" s="1" t="e">
+      <c r="P70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q67" s="1" t="e">
+      <c r="Q70" s="1" t="e">
         <f t="shared" si="115"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R67" s="1">
+      <c r="R70" s="1">
         <f t="shared" si="115"/>
         <v>0</v>
       </c>
-      <c r="S67" s="1">
+      <c r="S70" s="1">
         <f t="shared" si="115"/>
         <v>0</v>
       </c>
-      <c r="T67" s="1">
+      <c r="T70" s="1">
         <f t="shared" si="115"/>
         <v>0</v>
       </c>
-      <c r="U67" s="1">
+      <c r="U70" s="1">
         <f t="shared" si="115"/>
         <v>0</v>
       </c>
-      <c r="V67" s="1">
-        <f>V66/V23</f>
+      <c r="V70" s="1">
+        <f>V69/V23</f>
         <v>10.326342790096973</v>
       </c>
-      <c r="W67" s="1">
-        <f>W66/W23</f>
+      <c r="W70" s="1">
+        <f>W69/W23</f>
         <v>9.9381740323846604</v>
       </c>
-      <c r="X67" s="1">
-        <f t="shared" ref="X67:Y67" si="116">X66/X23</f>
+      <c r="X70" s="1">
+        <f t="shared" ref="X70:Y70" si="116">X69/X23</f>
         <v>9.7779065041031146</v>
       </c>
-      <c r="Y67" s="1">
+      <c r="Y70" s="1">
         <f t="shared" si="116"/>
         <v>9.929101045342879</v>
       </c>
-      <c r="AG67" s="1">
-        <f t="shared" ref="AG67:AH67" si="117">AG66/AG23</f>
+      <c r="AG70" s="1">
+        <f t="shared" ref="AG70:AH70" si="117">AG69/AG23</f>
         <v>-5.4081909238584934E-3</v>
       </c>
-      <c r="AH67" s="1">
+      <c r="AH70" s="1">
         <f t="shared" si="117"/>
         <v>10.326156925219998</v>
       </c>
     </row>
-    <row r="69" spans="2:35" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="38" t="s">
+    <row r="72" spans="2:35" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="34">
-        <f t="shared" ref="C69:V69" si="118">C37+C38</f>
-        <v>0</v>
-      </c>
-      <c r="D69" s="34">
+      <c r="C72" s="34">
+        <f t="shared" ref="C72:V72" si="118">C40+C41</f>
+        <v>0</v>
+      </c>
+      <c r="D72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="E69" s="34">
+      <c r="E72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="F69" s="34">
+      <c r="F72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="G69" s="34">
+      <c r="G72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="H69" s="34">
+      <c r="H72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="I69" s="34">
+      <c r="I72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="J69" s="34">
+      <c r="J72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="K69" s="34">
+      <c r="K72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="L69" s="34">
+      <c r="L72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="M69" s="34">
+      <c r="M72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="N69" s="34">
+      <c r="N72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="O69" s="34">
+      <c r="O72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="P69" s="34">
+      <c r="P72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="Q69" s="34">
+      <c r="Q72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="R69" s="34">
+      <c r="R72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="S69" s="34">
+      <c r="S72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="T69" s="34">
+      <c r="T72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="U69" s="34">
+      <c r="U72" s="34">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="V69" s="34">
+      <c r="V72" s="34">
         <f t="shared" si="118"/>
         <v>1825.923</v>
       </c>
-      <c r="W69" s="34">
-        <f>W37+W38</f>
+      <c r="W72" s="34">
+        <f>W40+W41</f>
         <v>1828.6950000000002</v>
       </c>
-      <c r="X69" s="34">
-        <f>X37+X38</f>
+      <c r="X72" s="34">
+        <f>X40+X41</f>
         <v>1795.6120000000001</v>
       </c>
-      <c r="Y69" s="34">
-        <f t="shared" ref="Y69" si="119">Y37+Y38</f>
+      <c r="Y72" s="34">
+        <f t="shared" ref="Y72" si="119">Y40+Y41</f>
         <v>1787.5319999999999</v>
       </c>
-      <c r="Z69" s="49"/>
-      <c r="AG69" s="34">
-        <f t="shared" ref="AG69:AH69" si="120">AG37+AG38</f>
+      <c r="Z72" s="49"/>
+      <c r="AG72" s="34">
+        <f t="shared" ref="AG72:AH72" si="120">AG40+AG41</f>
         <v>957.74199999999996</v>
       </c>
-      <c r="AH69" s="34">
+      <c r="AH72" s="34">
         <f t="shared" si="120"/>
         <v>1825.923</v>
       </c>
-      <c r="AI69" s="54"/>
-    </row>
-    <row r="70" spans="2:35" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="38" t="s">
+      <c r="AI72" s="54"/>
+    </row>
+    <row r="73" spans="2:35" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C70" s="34">
-        <f t="shared" ref="C70:V70" si="121">C59</f>
-        <v>0</v>
-      </c>
-      <c r="D70" s="34">
+      <c r="C73" s="34">
+        <f t="shared" ref="C73:V73" si="121">C62</f>
+        <v>0</v>
+      </c>
+      <c r="D73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="E70" s="34">
+      <c r="E73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="F70" s="34">
+      <c r="F73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="G70" s="34">
+      <c r="G73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="H70" s="34">
+      <c r="H73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="I70" s="34">
+      <c r="I73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="J70" s="34">
+      <c r="J73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="K70" s="34">
+      <c r="K73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="L70" s="34">
+      <c r="L73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="M70" s="34">
+      <c r="M73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="N70" s="34">
+      <c r="N73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="O70" s="34">
+      <c r="O73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="P70" s="34">
+      <c r="P73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="Q70" s="34">
+      <c r="Q73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="R70" s="34">
+      <c r="R73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="S70" s="34">
+      <c r="S73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="T70" s="34">
+      <c r="T73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="U70" s="34">
+      <c r="U73" s="34">
         <f t="shared" si="121"/>
         <v>0</v>
       </c>
-      <c r="V70" s="34">
+      <c r="V73" s="34">
         <f t="shared" si="121"/>
         <v>1136.521</v>
       </c>
-      <c r="W70" s="34">
-        <f>W59</f>
+      <c r="W73" s="34">
+        <f>W62</f>
         <v>1137.3610000000001</v>
       </c>
-      <c r="X70" s="34">
-        <f>X59</f>
+      <c r="X73" s="34">
+        <f>X62</f>
         <v>1138.2</v>
       </c>
-      <c r="Y70" s="34">
-        <f t="shared" ref="Y70" si="122">Y59</f>
+      <c r="Y73" s="34">
+        <f t="shared" ref="Y73" si="122">Y62</f>
         <v>1139.0419999999999</v>
       </c>
-      <c r="Z70" s="49"/>
-      <c r="AG70" s="34">
-        <f t="shared" ref="AG70:AH70" si="123">AG59</f>
+      <c r="Z73" s="49"/>
+      <c r="AG73" s="34">
+        <f t="shared" ref="AG73:AH73" si="123">AG62</f>
         <v>937.72900000000004</v>
       </c>
-      <c r="AH70" s="34">
+      <c r="AH73" s="34">
         <f t="shared" si="123"/>
         <v>1136.521</v>
       </c>
-      <c r="AI70" s="54"/>
-    </row>
-    <row r="71" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B71" s="1" t="s">
+      <c r="AI73" s="54"/>
+    </row>
+    <row r="74" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B74" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C71" s="30">
-        <f t="shared" ref="C71:V71" si="124">C69-C70</f>
-        <v>0</v>
-      </c>
-      <c r="D71" s="30">
+      <c r="C74" s="30">
+        <f t="shared" ref="C74:V74" si="124">C72-C73</f>
+        <v>0</v>
+      </c>
+      <c r="D74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="E71" s="30">
+      <c r="E74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="F71" s="30">
+      <c r="F74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="G71" s="30">
+      <c r="G74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="H71" s="30">
+      <c r="H74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="I71" s="30">
+      <c r="I74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="J71" s="30">
+      <c r="J74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="K71" s="30">
+      <c r="K74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="L71" s="30">
+      <c r="L74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="M71" s="30">
+      <c r="M74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="N71" s="30">
+      <c r="N74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="O71" s="30">
+      <c r="O74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="P71" s="30">
+      <c r="P74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="Q71" s="30">
+      <c r="Q74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="R71" s="30">
+      <c r="R74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="S71" s="30">
+      <c r="S74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="T71" s="30">
+      <c r="T74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="U71" s="30">
+      <c r="U74" s="30">
         <f t="shared" si="124"/>
         <v>0</v>
       </c>
-      <c r="V71" s="30">
+      <c r="V74" s="30">
         <f t="shared" si="124"/>
         <v>689.40200000000004</v>
       </c>
-      <c r="W71" s="30">
-        <f>W69-W70</f>
+      <c r="W74" s="30">
+        <f>W72-W73</f>
         <v>691.33400000000006</v>
       </c>
-      <c r="X71" s="30">
-        <f>X69-X70</f>
+      <c r="X74" s="30">
+        <f>X72-X73</f>
         <v>657.41200000000003</v>
       </c>
-      <c r="Y71" s="30">
-        <f t="shared" ref="Y71" si="125">Y69-Y70</f>
+      <c r="Y74" s="30">
+        <f t="shared" ref="Y74" si="125">Y72-Y73</f>
         <v>648.49</v>
       </c>
-      <c r="AG71" s="30">
-        <f t="shared" ref="AG71" si="126">AG69-AG70</f>
+      <c r="AG74" s="30">
+        <f t="shared" ref="AG74" si="126">AG72-AG73</f>
         <v>20.01299999999992</v>
       </c>
-      <c r="AH71" s="30">
-        <f t="shared" ref="AH71" si="127">AH69-AH70</f>
+      <c r="AH74" s="30">
+        <f t="shared" ref="AH74" si="127">AH72-AH73</f>
         <v>689.40200000000004</v>
       </c>
     </row>
-    <row r="73" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B73" s="1" t="s">
+    <row r="76" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B76" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="V73" s="1">
+      <c r="V76" s="1">
         <v>405.11</v>
       </c>
-      <c r="W73" s="30">
+      <c r="W76" s="30">
         <v>354.93</v>
       </c>
-      <c r="X73" s="1">
+      <c r="X76" s="1">
         <v>312.47000000000003</v>
       </c>
-      <c r="Y73" s="1">
+      <c r="Y76" s="1">
         <v>183.03</v>
       </c>
-      <c r="AG73" s="1">
+      <c r="AG76" s="1">
         <v>369.61</v>
       </c>
-      <c r="AH73" s="1">
-        <f>V73</f>
+      <c r="AH76" s="1">
+        <f>V76</f>
         <v>405.11</v>
       </c>
     </row>
-    <row r="74" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B74" s="1" t="s">
+    <row r="77" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B77" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V74" s="30">
-        <f t="shared" ref="V74" si="128">V73*V23</f>
+      <c r="V77" s="30">
+        <f t="shared" ref="V77" si="128">V76*V23</f>
         <v>26155.129893520003</v>
       </c>
-      <c r="W74" s="30">
-        <f>W73*W23</f>
+      <c r="W77" s="30">
+        <f>W76*W23</f>
         <v>24031.06875486</v>
       </c>
-      <c r="X74" s="30">
-        <f t="shared" ref="X74:Y74" si="129">X73*X23</f>
+      <c r="X77" s="30">
+        <f t="shared" ref="X77:Y77" si="129">X76*X23</f>
         <v>21352.46996608</v>
       </c>
-      <c r="Y74" s="30">
+      <c r="Y77" s="30">
         <f t="shared" si="129"/>
         <v>12613.844283390001</v>
       </c>
-      <c r="AG74" s="30">
-        <f t="shared" ref="AG74" si="130">AG73*AG23</f>
+      <c r="AG77" s="30">
+        <f t="shared" ref="AG77" si="130">AG76*AG23</f>
         <v>21801.299484439998</v>
       </c>
-      <c r="AH74" s="30">
-        <f>AH73*AH23</f>
+      <c r="AH77" s="30">
+        <f>AH76*AH23</f>
         <v>26155.129893520003</v>
       </c>
     </row>
-    <row r="75" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B75" s="1" t="s">
+    <row r="78" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B78" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V75" s="30">
-        <f t="shared" ref="V75" si="131">V74-V71</f>
+      <c r="V78" s="30">
+        <f t="shared" ref="V78" si="131">V77-V74</f>
         <v>25465.727893520001</v>
       </c>
-      <c r="W75" s="30">
-        <f>W74-W71</f>
+      <c r="W78" s="30">
+        <f>W77-W74</f>
         <v>23339.734754860001</v>
       </c>
-      <c r="X75" s="30">
-        <f t="shared" ref="X75:Y75" si="132">X74-X71</f>
+      <c r="X78" s="30">
+        <f t="shared" ref="X78:Y78" si="132">X77-X74</f>
         <v>20695.057966079999</v>
       </c>
-      <c r="Y75" s="30">
+      <c r="Y78" s="30">
         <f t="shared" si="132"/>
         <v>11965.354283390001</v>
       </c>
-      <c r="AG75" s="30">
-        <f t="shared" ref="AG75" si="133">AG74-AG71</f>
+      <c r="AG78" s="30">
+        <f t="shared" ref="AG78" si="133">AG77-AG74</f>
         <v>21781.286484439999</v>
       </c>
-      <c r="AH75" s="30">
-        <f>AH74-AH71</f>
+      <c r="AH78" s="30">
+        <f>AH77-AH74</f>
         <v>25465.727893520001</v>
       </c>
     </row>
-    <row r="77" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B77" s="1" t="s">
+    <row r="80" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B80" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="V77" s="40">
-        <f>V73/V67</f>
+      <c r="V80" s="40">
+        <f>V76/V70</f>
         <v>39.230733303614812</v>
       </c>
-      <c r="W77" s="40">
-        <f>W73/W67</f>
+      <c r="W80" s="40">
+        <f>W76/W70</f>
         <v>35.713804049256993</v>
       </c>
-      <c r="X77" s="40">
-        <f t="shared" ref="X77:Y77" si="134">X73/X67</f>
+      <c r="X80" s="40">
+        <f t="shared" ref="X80:Y80" si="134">X76/X70</f>
         <v>31.956738374301072</v>
       </c>
-      <c r="Y77" s="40">
+      <c r="Y80" s="40">
         <f t="shared" si="134"/>
         <v>18.433692956105823</v>
       </c>
-      <c r="AG77" s="48" t="s">
+      <c r="AG80" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="AH77" s="40">
-        <f>AH73/AH67</f>
+      <c r="AH80" s="40">
+        <f>AH76/AH70</f>
         <v>39.231439434218089</v>
       </c>
     </row>
-    <row r="78" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B78" s="1" t="s">
+    <row r="81" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B81" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V78" s="40">
-        <f t="shared" ref="V78:X78" si="135">V74/SUM(S6:V6)</f>
+      <c r="V81" s="40">
+        <f t="shared" ref="V81:X81" si="135">V77/SUM(S6:V6)</f>
         <v>29.93324409694867</v>
       </c>
-      <c r="W78" s="40">
+      <c r="W81" s="40">
         <f t="shared" si="135"/>
         <v>24.582176571414543</v>
       </c>
-      <c r="X78" s="40">
+      <c r="X81" s="40">
         <f t="shared" si="135"/>
         <v>19.725254796867233</v>
       </c>
-      <c r="Y78" s="40">
-        <f>Y74/SUM(V6:Y6)</f>
+      <c r="Y81" s="40">
+        <f>Y77/SUM(V6:Y6)</f>
         <v>10.606803677858297</v>
       </c>
-      <c r="AG78" s="40">
-        <f t="shared" ref="AG78" si="136">AG74/AG6</f>
+      <c r="AG81" s="40">
+        <f t="shared" ref="AG81" si="136">AG77/AG6</f>
         <v>36.927571198956599</v>
       </c>
-      <c r="AH78" s="40">
-        <f>AH74/AH6</f>
+      <c r="AH81" s="40">
+        <f>AH77/AH6</f>
         <v>29.93324409694867</v>
       </c>
     </row>
-    <row r="79" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B79" s="1" t="s">
+    <row r="82" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B82" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="V79" s="40">
-        <f t="shared" ref="V79:X79" si="137">V75/SUM(S6:V6)</f>
+      <c r="V82" s="40">
+        <f t="shared" ref="V82:X82" si="137">V78/SUM(S6:V6)</f>
         <v>29.144257828062376</v>
       </c>
-      <c r="W79" s="40">
+      <c r="W82" s="40">
         <f t="shared" si="137"/>
         <v>23.874988113373725</v>
       </c>
-      <c r="X79" s="40">
+      <c r="X82" s="40">
         <f t="shared" si="137"/>
         <v>19.117942423773247</v>
       </c>
-      <c r="Y79" s="40">
-        <f>Y75/SUM(V6:Y6)</f>
+      <c r="Y82" s="40">
+        <f>Y78/SUM(V6:Y6)</f>
         <v>10.061497586985441</v>
       </c>
-      <c r="AG79" s="40">
-        <f t="shared" ref="AG79" si="138">AG75/AG6</f>
+      <c r="AG82" s="40">
+        <f t="shared" ref="AG82" si="138">AG78/AG6</f>
         <v>36.893672692909654</v>
       </c>
-      <c r="AH79" s="40">
-        <f>AH75/AH6</f>
+      <c r="AH82" s="40">
+        <f>AH78/AH6</f>
         <v>29.144257828062376</v>
       </c>
     </row>
-    <row r="80" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B80" s="1" t="s">
+    <row r="83" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B83" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V80" s="40">
-        <f t="shared" ref="V80" si="139">V73/SUM(S22:V22)</f>
+      <c r="V83" s="40">
+        <f t="shared" ref="V83" si="139">V76/SUM(S22:V22)</f>
         <v>-84.508678490299772</v>
       </c>
-      <c r="W80" s="40">
-        <f t="shared" ref="W80:X80" si="140">W73/SUM(T22:W22)</f>
+      <c r="W83" s="40">
+        <f t="shared" ref="W83:X83" si="140">W76/SUM(T22:W22)</f>
         <v>-72.546524492411535</v>
       </c>
-      <c r="X80" s="40">
+      <c r="X83" s="40">
         <f t="shared" si="140"/>
         <v>-57.695906234315359</v>
       </c>
-      <c r="Y80" s="40">
-        <f>Y73/SUM(V22:Y22)</f>
+      <c r="Y83" s="40">
+        <f>Y76/SUM(V22:Y22)</f>
         <v>-33.274743486600045</v>
       </c>
-      <c r="AG80" s="40">
-        <f t="shared" ref="AG80" si="141">AG73/AG22</f>
+      <c r="AG83" s="40">
+        <f t="shared" ref="AG83" si="141">AG76/AG22</f>
         <v>-81.669936332863827</v>
       </c>
-      <c r="AH80" s="40">
-        <f>AH73/AH22</f>
+      <c r="AH83" s="40">
+        <f>AH76/AH22</f>
         <v>-85.233065551478504</v>
       </c>
     </row>
-    <row r="81" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B81" s="1" t="s">
+    <row r="84" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B84" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="V81" s="40"/>
-      <c r="W81" s="40"/>
-      <c r="X81" s="40"/>
-      <c r="Y81" s="40"/>
-    </row>
-    <row r="82" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B82" s="1" t="s">
+      <c r="V84" s="40"/>
+      <c r="W84" s="40"/>
+      <c r="X84" s="40"/>
+      <c r="Y84" s="40"/>
+    </row>
+    <row r="85" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B85" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="84" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B84" s="37" t="s">
+    <row r="87" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B87" s="37" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="86" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B86" s="1" t="s">
+    <row r="89" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B89" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B88" s="1" t="s">
+    <row r="91" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B91" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="90" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="2" t="s">
+    <row r="93" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B93" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Z90" s="53"/>
-      <c r="AI90" s="52"/>
+      <c r="Z93" s="53"/>
+      <c r="AI93" s="52"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6385,7 +6426,7 @@
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
   <ignoredErrors>
     <ignoredError sqref="AF4 AF5" formulaRange="1"/>
-    <ignoredError sqref="AH42 AH55 V6:V23 R6 R19 AI10 AI19:AI21" formula="1"/>
+    <ignoredError sqref="AH45 AH58 V6:V23 R6 R19 AI10 AI19:AI21" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId6"/>
 </worksheet>

</xml_diff>